<commit_message>
Updated CHE_grids model - 2025-08-15 15:13
</commit_message>
<xml_diff>
--- a/VerveStacks_CHE_grids/ReportDefs_vervestacks.xlsx
+++ b/VerveStacks_CHE_grids/ReportDefs_vervestacks.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Veda\VerveStacks\assumptions\VerveStacks_ISO_template\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Veda\Veda\Veda_models\vervestacks_models\VerveStacks_ITA_grids\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADE8D2E2-3532-4203-B088-884C639FA604}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA5084DB-70AB-4280-8176-3DF29E338507}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="17475" firstSheet="1" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="17475" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ScenMap" sheetId="56" r:id="rId1"/>
@@ -80,7 +80,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="286" uniqueCount="168">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="287" uniqueCount="169">
   <si>
     <t>Unit</t>
   </si>
@@ -584,6 +584,9 @@
   </si>
   <si>
     <t>$/tCO2</t>
+  </si>
+  <si>
+    <t>ELE,STG,IRE,-Grid</t>
   </si>
 </sst>
 </file>
@@ -1829,7 +1832,7 @@
   <sheetPr codeName="Sheet31"/>
   <dimension ref="A1:D7"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
@@ -1947,9 +1950,9 @@
   <sheetPr codeName="Sheet19"/>
   <dimension ref="A1:U13"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K11" sqref="K11"/>
+      <selection pane="bottomLeft" activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25"/>
@@ -1965,11 +1968,11 @@
     <col min="10" max="10" width="8.59765625" bestFit="1" customWidth="1"/>
     <col min="11" max="12" width="8.73046875" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="9.265625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="27" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="23.73046875" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="38.265625" customWidth="1"/>
-    <col min="17" max="17" width="9.265625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="7.265625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="15.1328125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="4.53125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="22.59765625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="8.6640625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="6.53125" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="11.59765625" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="2.1328125" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="13.86328125" bestFit="1" customWidth="1"/>
@@ -2108,7 +2111,11 @@
         <v>64</v>
       </c>
       <c r="C6" t="s">
-        <v>121</v>
+        <v>168</v>
+      </c>
+      <c r="D6" s="2"/>
+      <c r="H6" t="s">
+        <v>28</v>
       </c>
       <c r="I6" s="2" t="s">
         <v>105</v>

</xml_diff>

<commit_message>
Updated CHE_grids model - 2025-08-16 12:12
</commit_message>
<xml_diff>
--- a/VerveStacks_CHE_grids/ReportDefs_vervestacks.xlsx
+++ b/VerveStacks_CHE_grids/ReportDefs_vervestacks.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Veda\Veda\Veda_models\vervestacks_models\VerveStacks_ITA_grids\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Veda\VerveStacks\assumptions\VerveStacks_ISO_template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA5084DB-70AB-4280-8176-3DF29E338507}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90B09016-70C2-4AF1-A252-6411BA1F4B3B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="17475" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="17475" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ScenMap" sheetId="56" r:id="rId1"/>
@@ -19,7 +19,7 @@
     <sheet name="PSet_MAP coarse" sheetId="57" r:id="rId4"/>
     <sheet name="CSET_MAP" sheetId="66" r:id="rId5"/>
     <sheet name="CName_MAP" sheetId="58" r:id="rId6"/>
-    <sheet name="varbl map" sheetId="64" r:id="rId7"/>
+    <sheet name="timeslice map" sheetId="64" r:id="rId7"/>
     <sheet name="process map" sheetId="65" r:id="rId8"/>
     <sheet name="commodity map" sheetId="67" r:id="rId9"/>
     <sheet name="ATS" sheetId="63" r:id="rId10"/>
@@ -80,7 +80,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="287" uniqueCount="169">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="305" uniqueCount="181">
   <si>
     <t>Unit</t>
   </si>
@@ -250,9 +250,6 @@
     <t>process</t>
   </si>
   <si>
-    <t>~Varbl_map</t>
-  </si>
-  <si>
     <t>dimension</t>
   </si>
   <si>
@@ -587,6 +584,45 @@
   </si>
   <si>
     <t>ELE,STG,IRE,-Grid</t>
+  </si>
+  <si>
+    <t>s?a*</t>
+  </si>
+  <si>
+    <t>*,-s?a*</t>
+  </si>
+  <si>
+    <t>hourly</t>
+  </si>
+  <si>
+    <t>aggregated</t>
+  </si>
+  <si>
+    <t>ts_type</t>
+  </si>
+  <si>
+    <t>ts_season</t>
+  </si>
+  <si>
+    <t>S1*</t>
+  </si>
+  <si>
+    <t>S2*</t>
+  </si>
+  <si>
+    <t>S3*</t>
+  </si>
+  <si>
+    <t>S4*</t>
+  </si>
+  <si>
+    <t>S5*</t>
+  </si>
+  <si>
+    <t>S6*</t>
+  </si>
+  <si>
+    <t>~Timeslice_Map</t>
   </si>
 </sst>
 </file>
@@ -1146,13 +1182,13 @@
   <sheetData>
     <row r="1" spans="1:16">
       <c r="A1" t="s">
+        <v>130</v>
+      </c>
+      <c r="B1" t="s">
         <v>131</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>132</v>
-      </c>
-      <c r="C1" t="s">
-        <v>133</v>
       </c>
       <c r="H1" t="s">
         <v>39</v>
@@ -1160,18 +1196,18 @@
     </row>
     <row r="2" spans="1:16">
       <c r="H2" t="s">
+        <v>133</v>
+      </c>
+      <c r="I2" t="s">
         <v>134</v>
-      </c>
-      <c r="I2" t="s">
-        <v>135</v>
       </c>
     </row>
     <row r="4" spans="1:16">
       <c r="A4" t="s">
+        <v>65</v>
+      </c>
+      <c r="G4" t="s">
         <v>66</v>
-      </c>
-      <c r="G4" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="5" spans="1:16">
@@ -1213,16 +1249,16 @@
         <v>Delayed transition_3d</v>
       </c>
       <c r="H6" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="I6" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="N6">
         <v>1</v>
       </c>
       <c r="P6" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="7" spans="1:16">
@@ -1239,16 +1275,16 @@
         <v>Net Zero 2050_3d</v>
       </c>
       <c r="H7" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="I7" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="N7">
         <v>2</v>
       </c>
       <c r="P7" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="8" spans="1:16">
@@ -1265,16 +1301,16 @@
         <v>NDCs_3d</v>
       </c>
       <c r="H8" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="I8" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="N8">
         <v>3</v>
       </c>
       <c r="P8" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="9" spans="1:16">
@@ -1291,16 +1327,16 @@
         <v>Below 2deg_3d</v>
       </c>
       <c r="H9" t="s">
+        <v>141</v>
+      </c>
+      <c r="I9" t="s">
         <v>142</v>
-      </c>
-      <c r="I9" t="s">
-        <v>143</v>
       </c>
       <c r="N9">
         <v>4</v>
       </c>
       <c r="P9" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="10" spans="1:16">
@@ -1317,16 +1353,16 @@
         <v>Current Policies_3d</v>
       </c>
       <c r="H10" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="I10" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="N10">
         <v>5</v>
       </c>
       <c r="P10" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="11" spans="1:16">
@@ -1343,16 +1379,16 @@
         <v>Low demand_3d</v>
       </c>
       <c r="H11" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="I11" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="N11">
         <v>6</v>
       </c>
       <c r="P11" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="12" spans="1:16">
@@ -1369,16 +1405,16 @@
         <v>Fragmented World_3d</v>
       </c>
       <c r="H12" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="I12" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="N12">
         <v>7</v>
       </c>
       <c r="P12" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="13" spans="1:16">
@@ -1399,14 +1435,14 @@
         <v>Delayed transition</v>
       </c>
       <c r="I13" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="N13">
         <f>N6</f>
         <v>1</v>
       </c>
       <c r="P13" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="14" spans="1:16">
@@ -1427,14 +1463,14 @@
         <v>Net Zero 2050</v>
       </c>
       <c r="I14" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="N14">
         <f t="shared" ref="N14:N26" si="5">N7</f>
         <v>2</v>
       </c>
       <c r="P14" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="15" spans="1:16">
@@ -1455,14 +1491,14 @@
         <v>NDCs</v>
       </c>
       <c r="I15" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="N15">
         <f t="shared" si="5"/>
         <v>3</v>
       </c>
       <c r="P15" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="16" spans="1:16">
@@ -1483,14 +1519,14 @@
         <v>Below 2deg</v>
       </c>
       <c r="I16" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="N16">
         <f t="shared" si="5"/>
         <v>4</v>
       </c>
       <c r="P16" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="17" spans="1:16">
@@ -1511,14 +1547,14 @@
         <v>Current Policies</v>
       </c>
       <c r="I17" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="N17">
         <f t="shared" si="5"/>
         <v>5</v>
       </c>
       <c r="P17" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="18" spans="1:16">
@@ -1539,14 +1575,14 @@
         <v>Low demand</v>
       </c>
       <c r="I18" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="N18">
         <f t="shared" si="5"/>
         <v>6</v>
       </c>
       <c r="P18" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="19" spans="1:16">
@@ -1567,14 +1603,14 @@
         <v>Fragmented World</v>
       </c>
       <c r="I19" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="N19">
         <f t="shared" si="5"/>
         <v>7</v>
       </c>
       <c r="P19" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="20" spans="1:16">
@@ -1595,14 +1631,14 @@
         <v>Delayed transition</v>
       </c>
       <c r="I20" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="N20">
         <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="P20" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="21" spans="1:16">
@@ -1623,14 +1659,14 @@
         <v>Net Zero 2050</v>
       </c>
       <c r="I21" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="N21">
         <f t="shared" si="5"/>
         <v>2</v>
       </c>
       <c r="P21" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="22" spans="1:16">
@@ -1651,14 +1687,14 @@
         <v>NDCs</v>
       </c>
       <c r="I22" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="N22">
         <f t="shared" si="5"/>
         <v>3</v>
       </c>
       <c r="P22" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="23" spans="1:16">
@@ -1679,14 +1715,14 @@
         <v>Below 2deg</v>
       </c>
       <c r="I23" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="N23">
         <f t="shared" si="5"/>
         <v>4</v>
       </c>
       <c r="P23" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="24" spans="1:16">
@@ -1707,14 +1743,14 @@
         <v>Current Policies</v>
       </c>
       <c r="I24" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="N24">
         <f t="shared" si="5"/>
         <v>5</v>
       </c>
       <c r="P24" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="25" spans="1:16">
@@ -1735,14 +1771,14 @@
         <v>Low demand</v>
       </c>
       <c r="I25" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="N25">
         <f t="shared" si="5"/>
         <v>6</v>
       </c>
       <c r="P25" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="26" spans="1:16">
@@ -1763,14 +1799,14 @@
         <v>Fragmented World</v>
       </c>
       <c r="I26" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="N26">
         <f t="shared" si="5"/>
         <v>7</v>
       </c>
       <c r="P26" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
   </sheetData>
@@ -1870,10 +1906,10 @@
     </row>
     <row r="3" spans="1:4">
       <c r="A3" t="s">
+        <v>88</v>
+      </c>
+      <c r="B3" t="s">
         <v>89</v>
-      </c>
-      <c r="B3" t="s">
-        <v>90</v>
       </c>
       <c r="C3" t="s">
         <v>10</v>
@@ -1885,13 +1921,13 @@
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B4" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C4" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D4">
         <f>1/8.76*100</f>
@@ -1900,13 +1936,13 @@
     </row>
     <row r="5" spans="1:4">
       <c r="A5" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B5" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C5" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="D5">
         <v>1E-3</v>
@@ -1914,13 +1950,13 @@
     </row>
     <row r="6" spans="1:4">
       <c r="A6" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B6" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C6" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="D6">
         <v>-1E-3</v>
@@ -1928,13 +1964,13 @@
     </row>
     <row r="7" spans="1:4">
       <c r="A7" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B7" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C7" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D7">
         <v>-1000</v>
@@ -1950,7 +1986,7 @@
   <sheetPr codeName="Sheet19"/>
   <dimension ref="A1:U13"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="H6" sqref="H6"/>
     </sheetView>
@@ -2036,10 +2072,10 @@
         <v>12</v>
       </c>
       <c r="Q2" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="R2" s="6" t="s">
         <v>62</v>
-      </c>
-      <c r="R2" s="6" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="3" spans="1:21">
@@ -2047,16 +2083,16 @@
         <v>9</v>
       </c>
       <c r="C3" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="K3" t="s">
         <v>10</v>
       </c>
       <c r="N3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="4" spans="1:21">
@@ -2064,16 +2100,16 @@
         <v>38</v>
       </c>
       <c r="C4" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="K4" t="s">
         <v>10</v>
       </c>
       <c r="N4" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="T4" s="8" t="s">
         <v>46</v>
@@ -2085,19 +2121,19 @@
         <v>7</v>
       </c>
       <c r="C5" t="s">
+        <v>121</v>
+      </c>
+      <c r="D5" s="2" t="s">
         <v>122</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="I5" t="s">
         <v>123</v>
       </c>
-      <c r="I5" t="s">
-        <v>124</v>
-      </c>
       <c r="K5" t="s">
+        <v>83</v>
+      </c>
+      <c r="N5" t="s">
         <v>84</v>
-      </c>
-      <c r="N5" t="s">
-        <v>85</v>
       </c>
       <c r="T5" s="3" t="s">
         <v>47</v>
@@ -2108,26 +2144,26 @@
     </row>
     <row r="6" spans="1:21">
       <c r="A6" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C6" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="D6" s="2"/>
       <c r="H6" t="s">
         <v>28</v>
       </c>
       <c r="I6" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="K6" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="N6" t="s">
         <v>44</v>
       </c>
       <c r="Q6" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="T6" s="3"/>
       <c r="U6" s="3"/>
@@ -2137,13 +2173,13 @@
         <v>7</v>
       </c>
       <c r="I7" s="2" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="K7" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="N7" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="T7" s="3"/>
       <c r="U7" s="3"/>
@@ -2153,13 +2189,13 @@
         <v>7</v>
       </c>
       <c r="I8" s="2" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="K8" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="N8" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="T8" s="3"/>
       <c r="U8" s="3"/>
@@ -2169,16 +2205,16 @@
         <v>32</v>
       </c>
       <c r="C9" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="K9" t="s">
         <v>45</v>
       </c>
       <c r="N9" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="10" spans="1:21">
@@ -2186,13 +2222,13 @@
         <v>31</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="H10" t="s">
         <v>28</v>
       </c>
       <c r="K10" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="N10" t="s">
         <v>48</v>
@@ -2209,16 +2245,16 @@
         <v>31</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="I11" t="s">
+        <v>163</v>
+      </c>
+      <c r="K11" t="s">
         <v>164</v>
       </c>
-      <c r="K11" t="s">
+      <c r="N11" t="s">
         <v>165</v>
-      </c>
-      <c r="N11" t="s">
-        <v>166</v>
       </c>
     </row>
     <row r="12" spans="1:21">
@@ -2226,7 +2262,7 @@
         <v>51</v>
       </c>
       <c r="K12" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="N12" t="s">
         <v>52</v>
@@ -2240,16 +2276,16 @@
     </row>
     <row r="13" spans="1:21">
       <c r="A13" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B13" s="4" t="s">
         <v>38</v>
       </c>
       <c r="K13" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="N13" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="Q13" t="s">
         <v>47</v>
@@ -2287,15 +2323,15 @@
   <sheetData>
     <row r="1" spans="3:11">
       <c r="C1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="2" spans="3:11">
       <c r="C2" t="s">
+        <v>109</v>
+      </c>
+      <c r="D2" t="s">
         <v>110</v>
-      </c>
-      <c r="D2" t="s">
-        <v>111</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>2</v>
@@ -2304,16 +2340,16 @@
         <v>0</v>
       </c>
       <c r="G2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="H2" t="s">
+        <v>111</v>
+      </c>
+      <c r="I2" t="s">
         <v>112</v>
       </c>
-      <c r="I2" t="s">
+      <c r="J2" t="s">
         <v>113</v>
-      </c>
-      <c r="J2" t="s">
-        <v>114</v>
       </c>
       <c r="K2" t="s">
         <v>12</v>
@@ -2321,22 +2357,22 @@
     </row>
     <row r="3" spans="3:11">
       <c r="C3" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E3" s="7" t="s">
+        <v>114</v>
+      </c>
+      <c r="F3" t="s">
         <v>115</v>
-      </c>
-      <c r="F3" t="s">
-        <v>116</v>
       </c>
       <c r="G3" t="s">
         <v>47</v>
       </c>
       <c r="I3" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="J3" t="s">
         <v>47</v>
@@ -2402,12 +2438,12 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B2" t="s">
         <v>1</v>
@@ -2464,31 +2500,127 @@
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{32957E82-8232-40A9-A839-CC5F79005B92}">
   <sheetPr codeName="Sheet3"/>
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C10"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="11.59765625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="28.86328125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.59765625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.1328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.19921875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.59765625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" t="s">
-        <v>56</v>
+        <v>180</v>
       </c>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" t="s">
+        <v>56</v>
+      </c>
+      <c r="B2" t="s">
         <v>57</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>58</v>
       </c>
-      <c r="C2" t="s">
-        <v>59</v>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" t="s">
+        <v>172</v>
+      </c>
+      <c r="B3" t="s">
+        <v>169</v>
+      </c>
+      <c r="C3" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" t="s">
+        <v>172</v>
+      </c>
+      <c r="B4" t="s">
+        <v>168</v>
+      </c>
+      <c r="C4" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" t="s">
+        <v>173</v>
+      </c>
+      <c r="B5" t="s">
+        <v>174</v>
+      </c>
+      <c r="C5" t="str">
+        <f>LEFT(B5,2)</f>
+        <v>S1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" t="s">
+        <v>173</v>
+      </c>
+      <c r="B6" t="s">
+        <v>175</v>
+      </c>
+      <c r="C6" t="str">
+        <f t="shared" ref="C6:C10" si="0">LEFT(B6,2)</f>
+        <v>S2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" t="s">
+        <v>173</v>
+      </c>
+      <c r="B7" t="s">
+        <v>176</v>
+      </c>
+      <c r="C7" t="str">
+        <f t="shared" si="0"/>
+        <v>S3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8" t="s">
+        <v>173</v>
+      </c>
+      <c r="B8" t="s">
+        <v>177</v>
+      </c>
+      <c r="C8" t="str">
+        <f t="shared" si="0"/>
+        <v>S4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9" t="s">
+        <v>173</v>
+      </c>
+      <c r="B9" t="s">
+        <v>178</v>
+      </c>
+      <c r="C9" t="str">
+        <f t="shared" si="0"/>
+        <v>S5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10" t="s">
+        <v>173</v>
+      </c>
+      <c r="B10" t="s">
+        <v>179</v>
+      </c>
+      <c r="C10" t="str">
+        <f t="shared" si="0"/>
+        <v>S6</v>
       </c>
     </row>
   </sheetData>
@@ -2516,71 +2648,71 @@
   <sheetData>
     <row r="1" spans="1:7" ht="17.25" thickBot="1">
       <c r="A1" s="5" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="15" thickTop="1" thickBot="1">
       <c r="A2" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="B2" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="C2" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="C2" s="6" t="s">
-        <v>59</v>
-      </c>
       <c r="D2" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="E2" s="6" t="s">
         <v>69</v>
       </c>
-      <c r="E2" s="6" t="s">
+      <c r="F2" s="6" t="s">
         <v>70</v>
       </c>
-      <c r="F2" s="6" t="s">
+      <c r="G2" s="6" t="s">
         <v>71</v>
-      </c>
-      <c r="G2" s="6" t="s">
-        <v>72</v>
       </c>
     </row>
     <row r="3" spans="1:7">
       <c r="A3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C3" t="str">
         <f>D3</f>
         <v>CCGT</v>
       </c>
       <c r="D3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="4" spans="1:7">
       <c r="A4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C4" t="str">
         <f t="shared" ref="C4:C20" si="0">D4</f>
         <v>Int Comb</v>
       </c>
       <c r="D4" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="5" spans="1:7">
       <c r="A5" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C5" t="str">
         <f t="shared" si="0"/>
         <v>Gas_Oil Steam</v>
       </c>
       <c r="D5" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="6" spans="1:7">
       <c r="A6" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C6" t="str">
         <f t="shared" si="0"/>
@@ -2592,67 +2724,67 @@
     </row>
     <row r="7" spans="1:7">
       <c r="A7" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C7" t="str">
         <f t="shared" si="0"/>
         <v>OCGT (Peaker)</v>
       </c>
       <c r="D7" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="8" spans="1:7">
       <c r="A8" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C8" t="str">
         <f t="shared" si="0"/>
         <v>Subcritical Coal</v>
       </c>
       <c r="D8" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="9" spans="1:7">
       <c r="A9" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C9" t="str">
         <f t="shared" si="0"/>
         <v>Supercritical Coal</v>
       </c>
       <c r="D9" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="10" spans="1:7">
       <c r="A10" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C10" t="str">
         <f t="shared" si="0"/>
         <v>IGCC</v>
       </c>
       <c r="D10" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="11" spans="1:7">
       <c r="A11" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C11" t="str">
         <f t="shared" si="0"/>
         <v>Bioenergy</v>
       </c>
       <c r="D11" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="12" spans="1:7">
       <c r="A12" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C12" t="str">
         <f t="shared" si="0"/>
@@ -2664,43 +2796,43 @@
     </row>
     <row r="13" spans="1:7">
       <c r="A13" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C13" t="str">
         <f t="shared" si="0"/>
         <v>Wind onshore</v>
       </c>
       <c r="D13" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="14" spans="1:7">
       <c r="A14" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C14" t="str">
         <f t="shared" si="0"/>
         <v>Wind offshore</v>
       </c>
       <c r="D14" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="15" spans="1:7">
       <c r="A15" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C15" t="str">
         <f t="shared" si="0"/>
         <v>Geothermal</v>
       </c>
       <c r="D15" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="16" spans="1:7">
       <c r="A16" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C16" t="str">
         <f t="shared" si="0"/>
@@ -2712,7 +2844,7 @@
     </row>
     <row r="17" spans="1:6">
       <c r="A17" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C17" t="str">
         <f t="shared" si="0"/>
@@ -2724,102 +2856,102 @@
     </row>
     <row r="18" spans="1:6">
       <c r="A18" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C18" t="str">
         <f t="shared" si="0"/>
         <v>Hydro pumped stg</v>
       </c>
       <c r="D18" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="19" spans="1:6">
       <c r="A19" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C19" t="str">
         <f t="shared" si="0"/>
         <v>Util Batt Stg</v>
       </c>
       <c r="D19" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="20" spans="1:6">
       <c r="A20" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C20" t="str">
         <f t="shared" si="0"/>
         <v>EV Batt</v>
       </c>
       <c r="D20" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="21" spans="1:6">
       <c r="A21" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C21" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="E21" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="F21" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="22" spans="1:6">
       <c r="A22" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C22" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="E22" t="s">
+        <v>160</v>
+      </c>
+      <c r="F22" t="s">
         <v>161</v>
-      </c>
-      <c r="F22" t="s">
-        <v>162</v>
       </c>
     </row>
     <row r="23" spans="1:6">
       <c r="A23" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B23" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C23" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="E23" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="24" spans="1:6">
       <c r="A24" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B24" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C24" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="E24" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="25" spans="1:6">
       <c r="A25" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B25" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C25" t="s">
         <v>5</v>
@@ -2827,46 +2959,46 @@
     </row>
     <row r="26" spans="1:6">
       <c r="A26" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B26" t="s">
+        <v>106</v>
+      </c>
+      <c r="C26" t="s">
         <v>107</v>
-      </c>
-      <c r="C26" t="s">
-        <v>108</v>
       </c>
     </row>
     <row r="27" spans="1:6">
       <c r="A27" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B27" t="s">
+        <v>118</v>
+      </c>
+      <c r="C27" t="s">
         <v>119</v>
-      </c>
-      <c r="C27" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="28" spans="1:6">
       <c r="A28" t="s">
+        <v>125</v>
+      </c>
+      <c r="B28" t="s">
         <v>126</v>
       </c>
-      <c r="B28" t="s">
+      <c r="C28" t="s">
         <v>127</v>
-      </c>
-      <c r="C28" t="s">
-        <v>128</v>
       </c>
     </row>
     <row r="29" spans="1:6">
       <c r="A29" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B29" t="s">
+        <v>128</v>
+      </c>
+      <c r="C29" t="s">
         <v>129</v>
-      </c>
-      <c r="C29" t="s">
-        <v>130</v>
       </c>
     </row>
   </sheetData>
@@ -2894,33 +3026,33 @@
   <sheetData>
     <row r="1" spans="1:8">
       <c r="A1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="2" spans="1:8">
       <c r="A2" t="s">
+        <v>56</v>
+      </c>
+      <c r="B2" t="s">
         <v>57</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>58</v>
       </c>
-      <c r="C2" t="s">
-        <v>59</v>
-      </c>
       <c r="D2" t="s">
+        <v>77</v>
+      </c>
+      <c r="E2" t="s">
         <v>78</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
+        <v>80</v>
+      </c>
+      <c r="G2" t="s">
         <v>79</v>
       </c>
-      <c r="F2" t="s">
+      <c r="H2" t="s">
         <v>81</v>
-      </c>
-      <c r="G2" t="s">
-        <v>80</v>
-      </c>
-      <c r="H2" t="s">
-        <v>82</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated CHE_grids model - 2025-08-18 23:29
</commit_message>
<xml_diff>
--- a/VerveStacks_CHE_grids/ReportDefs_vervestacks.xlsx
+++ b/VerveStacks_CHE_grids/ReportDefs_vervestacks.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Veda\Veda\Veda_models\vervestacks_models\VerveStacks_CHE_grids\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Veda\VerveStacks\assumptions\VerveStacks_ISO_template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0A1C99C-5F8D-45F1-924D-AB56EE0C873A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F722313C-51C9-4AE2-9912-CBFFFD05F5D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="17475" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="17475" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ScenMap" sheetId="56" r:id="rId1"/>
@@ -80,7 +80,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="307" uniqueCount="184">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="335" uniqueCount="187">
   <si>
     <t>Unit</t>
   </si>
@@ -451,6 +451,9 @@
     <t>-ElcAgg*,-*EV*</t>
   </si>
   <si>
+    <t>ELC,ELC_???-???</t>
+  </si>
+  <si>
     <t>t</t>
   </si>
   <si>
@@ -622,16 +625,22 @@
     <t>~Timeslice_Map</t>
   </si>
   <si>
-    <t>p,c</t>
-  </si>
-  <si>
-    <t>-ElcAgg*,-*EV*,-g[_]*</t>
-  </si>
-  <si>
-    <t>-ElcAgg*,-*EV*,-g[_]*,-distr*</t>
-  </si>
-  <si>
-    <t>ELC,ELC_???-???,e[_]*</t>
+    <t>vstacks_ts16~</t>
+  </si>
+  <si>
+    <t>vstacks_t_annual~</t>
+  </si>
+  <si>
+    <t>ts-16</t>
+  </si>
+  <si>
+    <t>ts-annual</t>
+  </si>
+  <si>
+    <t>_16</t>
+  </si>
+  <si>
+    <t>_ann</t>
   </si>
 </sst>
 </file>
@@ -643,7 +652,7 @@
     <numFmt numFmtId="165" formatCode="#.00"/>
     <numFmt numFmtId="166" formatCode="#."/>
   </numFmts>
-  <fonts count="18">
+  <fonts count="19">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -756,6 +765,12 @@
       <color indexed="81"/>
       <name val="Tahoma"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="4">
@@ -1170,15 +1185,15 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet11"/>
-  <dimension ref="A1:P26"/>
+  <dimension ref="A1:P40"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A33" sqref="A33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.73046875" defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.6640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="19.59765625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.59765625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="5" bestFit="1" customWidth="1"/>
@@ -1191,13 +1206,19 @@
   <sheetData>
     <row r="1" spans="1:16">
       <c r="A1" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="B1" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="C1" t="s">
-        <v>131</v>
+        <v>132</v>
+      </c>
+      <c r="D1" t="s">
+        <v>181</v>
+      </c>
+      <c r="E1" t="s">
+        <v>182</v>
       </c>
       <c r="H1" t="s">
         <v>39</v>
@@ -1205,10 +1226,10 @@
     </row>
     <row r="2" spans="1:16">
       <c r="H2" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="I2" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
     </row>
     <row r="4" spans="1:16">
@@ -1258,16 +1279,16 @@
         <v>Delayed transition_3d</v>
       </c>
       <c r="H6" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="I6" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="N6">
         <v>1</v>
       </c>
       <c r="P6" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
     </row>
     <row r="7" spans="1:16">
@@ -1284,16 +1305,16 @@
         <v>Net Zero 2050_3d</v>
       </c>
       <c r="H7" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="I7" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="N7">
         <v>2</v>
       </c>
       <c r="P7" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
     </row>
     <row r="8" spans="1:16">
@@ -1310,16 +1331,16 @@
         <v>NDCs_3d</v>
       </c>
       <c r="H8" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="I8" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="N8">
         <v>3</v>
       </c>
       <c r="P8" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
     </row>
     <row r="9" spans="1:16">
@@ -1336,16 +1357,16 @@
         <v>Below 2deg_3d</v>
       </c>
       <c r="H9" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="I9" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="N9">
         <v>4</v>
       </c>
       <c r="P9" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
     </row>
     <row r="10" spans="1:16">
@@ -1362,16 +1383,16 @@
         <v>Current Policies_3d</v>
       </c>
       <c r="H10" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="I10" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="N10">
         <v>5</v>
       </c>
       <c r="P10" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
     </row>
     <row r="11" spans="1:16">
@@ -1388,16 +1409,16 @@
         <v>Low demand_3d</v>
       </c>
       <c r="H11" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="I11" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="N11">
         <v>6</v>
       </c>
       <c r="P11" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
     </row>
     <row r="12" spans="1:16">
@@ -1414,16 +1435,16 @@
         <v>Fragmented World_3d</v>
       </c>
       <c r="H12" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="I12" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="N12">
         <v>7</v>
       </c>
       <c r="P12" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
     </row>
     <row r="13" spans="1:16">
@@ -1444,14 +1465,14 @@
         <v>Delayed transition</v>
       </c>
       <c r="I13" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="N13">
         <f>N6</f>
         <v>1</v>
       </c>
       <c r="P13" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
     </row>
     <row r="14" spans="1:16">
@@ -1468,18 +1489,18 @@
         <v>Net Zero 2050_15d</v>
       </c>
       <c r="H14" t="str">
-        <f t="shared" ref="H14:H26" si="4">H7</f>
+        <f t="shared" ref="H14:H41" si="4">H7</f>
         <v>Net Zero 2050</v>
       </c>
       <c r="I14" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="N14">
-        <f t="shared" ref="N14:N26" si="5">N7</f>
+        <f t="shared" ref="N14:N40" si="5">N7</f>
         <v>2</v>
       </c>
       <c r="P14" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
     </row>
     <row r="15" spans="1:16">
@@ -1500,14 +1521,14 @@
         <v>NDCs</v>
       </c>
       <c r="I15" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="N15">
         <f t="shared" si="5"/>
         <v>3</v>
       </c>
       <c r="P15" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
     </row>
     <row r="16" spans="1:16">
@@ -1528,14 +1549,14 @@
         <v>Below 2deg</v>
       </c>
       <c r="I16" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="N16">
         <f t="shared" si="5"/>
         <v>4</v>
       </c>
       <c r="P16" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
     </row>
     <row r="17" spans="1:16">
@@ -1556,14 +1577,14 @@
         <v>Current Policies</v>
       </c>
       <c r="I17" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="N17">
         <f t="shared" si="5"/>
         <v>5</v>
       </c>
       <c r="P17" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
     </row>
     <row r="18" spans="1:16">
@@ -1584,14 +1605,14 @@
         <v>Low demand</v>
       </c>
       <c r="I18" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="N18">
         <f t="shared" si="5"/>
         <v>6</v>
       </c>
       <c r="P18" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
     </row>
     <row r="19" spans="1:16">
@@ -1612,14 +1633,14 @@
         <v>Fragmented World</v>
       </c>
       <c r="I19" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="N19">
         <f t="shared" si="5"/>
         <v>7</v>
       </c>
       <c r="P19" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
     </row>
     <row r="20" spans="1:16">
@@ -1640,14 +1661,14 @@
         <v>Delayed transition</v>
       </c>
       <c r="I20" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="N20">
         <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="P20" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
     </row>
     <row r="21" spans="1:16">
@@ -1668,14 +1689,14 @@
         <v>Net Zero 2050</v>
       </c>
       <c r="I21" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="N21">
         <f t="shared" si="5"/>
         <v>2</v>
       </c>
       <c r="P21" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
     </row>
     <row r="22" spans="1:16">
@@ -1696,14 +1717,14 @@
         <v>NDCs</v>
       </c>
       <c r="I22" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="N22">
         <f t="shared" si="5"/>
         <v>3</v>
       </c>
       <c r="P22" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
     </row>
     <row r="23" spans="1:16">
@@ -1724,14 +1745,14 @@
         <v>Below 2deg</v>
       </c>
       <c r="I23" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="N23">
         <f t="shared" si="5"/>
         <v>4</v>
       </c>
       <c r="P23" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
     </row>
     <row r="24" spans="1:16">
@@ -1752,14 +1773,14 @@
         <v>Current Policies</v>
       </c>
       <c r="I24" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="N24">
         <f t="shared" si="5"/>
         <v>5</v>
       </c>
       <c r="P24" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
     </row>
     <row r="25" spans="1:16">
@@ -1780,14 +1801,14 @@
         <v>Low demand</v>
       </c>
       <c r="I25" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="N25">
         <f t="shared" si="5"/>
         <v>6</v>
       </c>
       <c r="P25" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
     </row>
     <row r="26" spans="1:16">
@@ -1808,17 +1829,410 @@
         <v>Fragmented World</v>
       </c>
       <c r="I26" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="N26">
         <f t="shared" si="5"/>
         <v>7</v>
       </c>
       <c r="P26" t="s">
-        <v>146</v>
+        <v>147</v>
+      </c>
+    </row>
+    <row r="27" spans="1:16">
+      <c r="A27" t="str">
+        <f>$D$1&amp;TEXT(N27,"0000")</f>
+        <v>vstacks_ts16~0001</v>
+      </c>
+      <c r="B27" t="str">
+        <f t="shared" ref="B27:B41" si="7">G27</f>
+        <v>Delayed transition_16</v>
+      </c>
+      <c r="G27" t="str">
+        <f t="shared" ref="G27:G41" si="8">H27&amp;P27</f>
+        <v>Delayed transition_16</v>
+      </c>
+      <c r="H27" t="str">
+        <f t="shared" si="4"/>
+        <v>Delayed transition</v>
+      </c>
+      <c r="I27" t="s">
+        <v>183</v>
+      </c>
+      <c r="N27">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="P27" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="28" spans="1:16">
+      <c r="A28" t="str">
+        <f t="shared" ref="A28:A40" si="9">$D$1&amp;TEXT(N28,"0000")</f>
+        <v>vstacks_ts16~0002</v>
+      </c>
+      <c r="B28" t="str">
+        <f t="shared" si="7"/>
+        <v>Net Zero 2050_16</v>
+      </c>
+      <c r="G28" t="str">
+        <f t="shared" si="8"/>
+        <v>Net Zero 2050_16</v>
+      </c>
+      <c r="H28" t="str">
+        <f t="shared" si="4"/>
+        <v>Net Zero 2050</v>
+      </c>
+      <c r="I28" t="s">
+        <v>183</v>
+      </c>
+      <c r="N28">
+        <f t="shared" si="5"/>
+        <v>2</v>
+      </c>
+      <c r="P28" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="29" spans="1:16">
+      <c r="A29" t="str">
+        <f t="shared" si="9"/>
+        <v>vstacks_ts16~0003</v>
+      </c>
+      <c r="B29" t="str">
+        <f t="shared" si="7"/>
+        <v>NDCs_16</v>
+      </c>
+      <c r="G29" t="str">
+        <f t="shared" si="8"/>
+        <v>NDCs_16</v>
+      </c>
+      <c r="H29" t="str">
+        <f t="shared" si="4"/>
+        <v>NDCs</v>
+      </c>
+      <c r="I29" t="s">
+        <v>183</v>
+      </c>
+      <c r="N29">
+        <f t="shared" si="5"/>
+        <v>3</v>
+      </c>
+      <c r="P29" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="30" spans="1:16">
+      <c r="A30" t="str">
+        <f t="shared" si="9"/>
+        <v>vstacks_ts16~0004</v>
+      </c>
+      <c r="B30" t="str">
+        <f t="shared" si="7"/>
+        <v>Below 2deg_16</v>
+      </c>
+      <c r="G30" t="str">
+        <f t="shared" si="8"/>
+        <v>Below 2deg_16</v>
+      </c>
+      <c r="H30" t="str">
+        <f t="shared" si="4"/>
+        <v>Below 2deg</v>
+      </c>
+      <c r="I30" t="s">
+        <v>183</v>
+      </c>
+      <c r="N30">
+        <f t="shared" si="5"/>
+        <v>4</v>
+      </c>
+      <c r="P30" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="31" spans="1:16">
+      <c r="A31" t="str">
+        <f t="shared" si="9"/>
+        <v>vstacks_ts16~0005</v>
+      </c>
+      <c r="B31" t="str">
+        <f t="shared" si="7"/>
+        <v>Current Policies_16</v>
+      </c>
+      <c r="G31" t="str">
+        <f t="shared" si="8"/>
+        <v>Current Policies_16</v>
+      </c>
+      <c r="H31" t="str">
+        <f t="shared" si="4"/>
+        <v>Current Policies</v>
+      </c>
+      <c r="I31" t="s">
+        <v>183</v>
+      </c>
+      <c r="N31">
+        <f t="shared" si="5"/>
+        <v>5</v>
+      </c>
+      <c r="P31" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="32" spans="1:16">
+      <c r="A32" t="str">
+        <f t="shared" si="9"/>
+        <v>vstacks_ts16~0006</v>
+      </c>
+      <c r="B32" t="str">
+        <f t="shared" si="7"/>
+        <v>Low demand_16</v>
+      </c>
+      <c r="G32" t="str">
+        <f t="shared" si="8"/>
+        <v>Low demand_16</v>
+      </c>
+      <c r="H32" t="str">
+        <f t="shared" si="4"/>
+        <v>Low demand</v>
+      </c>
+      <c r="I32" t="s">
+        <v>183</v>
+      </c>
+      <c r="N32">
+        <f t="shared" si="5"/>
+        <v>6</v>
+      </c>
+      <c r="P32" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="33" spans="1:16">
+      <c r="A33" t="str">
+        <f t="shared" si="9"/>
+        <v>vstacks_ts16~0007</v>
+      </c>
+      <c r="B33" t="str">
+        <f t="shared" si="7"/>
+        <v>Fragmented World_16</v>
+      </c>
+      <c r="G33" t="str">
+        <f t="shared" si="8"/>
+        <v>Fragmented World_16</v>
+      </c>
+      <c r="H33" t="str">
+        <f t="shared" si="4"/>
+        <v>Fragmented World</v>
+      </c>
+      <c r="I33" t="s">
+        <v>183</v>
+      </c>
+      <c r="N33">
+        <f t="shared" si="5"/>
+        <v>7</v>
+      </c>
+      <c r="P33" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="34" spans="1:16">
+      <c r="A34" t="str">
+        <f>$E$1&amp;TEXT(N34,"0000")</f>
+        <v>vstacks_t_annual~0001</v>
+      </c>
+      <c r="B34" t="str">
+        <f t="shared" si="7"/>
+        <v>Delayed transition_ann</v>
+      </c>
+      <c r="G34" t="str">
+        <f t="shared" si="8"/>
+        <v>Delayed transition_ann</v>
+      </c>
+      <c r="H34" t="str">
+        <f t="shared" si="4"/>
+        <v>Delayed transition</v>
+      </c>
+      <c r="I34" t="s">
+        <v>184</v>
+      </c>
+      <c r="N34">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="P34" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="35" spans="1:16">
+      <c r="A35" t="str">
+        <f t="shared" ref="A35:A40" si="10">$E$1&amp;TEXT(N35,"0000")</f>
+        <v>vstacks_t_annual~0002</v>
+      </c>
+      <c r="B35" t="str">
+        <f t="shared" si="7"/>
+        <v>Net Zero 2050_ann</v>
+      </c>
+      <c r="G35" t="str">
+        <f t="shared" si="8"/>
+        <v>Net Zero 2050_ann</v>
+      </c>
+      <c r="H35" t="str">
+        <f t="shared" si="4"/>
+        <v>Net Zero 2050</v>
+      </c>
+      <c r="I35" t="s">
+        <v>184</v>
+      </c>
+      <c r="N35">
+        <f t="shared" si="5"/>
+        <v>2</v>
+      </c>
+      <c r="P35" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="36" spans="1:16">
+      <c r="A36" t="str">
+        <f t="shared" si="10"/>
+        <v>vstacks_t_annual~0003</v>
+      </c>
+      <c r="B36" t="str">
+        <f t="shared" si="7"/>
+        <v>NDCs_ann</v>
+      </c>
+      <c r="G36" t="str">
+        <f t="shared" si="8"/>
+        <v>NDCs_ann</v>
+      </c>
+      <c r="H36" t="str">
+        <f t="shared" si="4"/>
+        <v>NDCs</v>
+      </c>
+      <c r="I36" t="s">
+        <v>184</v>
+      </c>
+      <c r="N36">
+        <f t="shared" si="5"/>
+        <v>3</v>
+      </c>
+      <c r="P36" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="37" spans="1:16">
+      <c r="A37" t="str">
+        <f t="shared" si="10"/>
+        <v>vstacks_t_annual~0004</v>
+      </c>
+      <c r="B37" t="str">
+        <f t="shared" si="7"/>
+        <v>Below 2deg_ann</v>
+      </c>
+      <c r="G37" t="str">
+        <f t="shared" si="8"/>
+        <v>Below 2deg_ann</v>
+      </c>
+      <c r="H37" t="str">
+        <f t="shared" si="4"/>
+        <v>Below 2deg</v>
+      </c>
+      <c r="I37" t="s">
+        <v>184</v>
+      </c>
+      <c r="N37">
+        <f t="shared" si="5"/>
+        <v>4</v>
+      </c>
+      <c r="P37" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="38" spans="1:16">
+      <c r="A38" t="str">
+        <f t="shared" si="10"/>
+        <v>vstacks_t_annual~0005</v>
+      </c>
+      <c r="B38" t="str">
+        <f t="shared" si="7"/>
+        <v>Current Policies_ann</v>
+      </c>
+      <c r="G38" t="str">
+        <f t="shared" si="8"/>
+        <v>Current Policies_ann</v>
+      </c>
+      <c r="H38" t="str">
+        <f t="shared" si="4"/>
+        <v>Current Policies</v>
+      </c>
+      <c r="I38" t="s">
+        <v>184</v>
+      </c>
+      <c r="N38">
+        <f t="shared" si="5"/>
+        <v>5</v>
+      </c>
+      <c r="P38" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="39" spans="1:16">
+      <c r="A39" t="str">
+        <f t="shared" si="10"/>
+        <v>vstacks_t_annual~0006</v>
+      </c>
+      <c r="B39" t="str">
+        <f t="shared" si="7"/>
+        <v>Low demand_ann</v>
+      </c>
+      <c r="G39" t="str">
+        <f t="shared" si="8"/>
+        <v>Low demand_ann</v>
+      </c>
+      <c r="H39" t="str">
+        <f t="shared" si="4"/>
+        <v>Low demand</v>
+      </c>
+      <c r="I39" t="s">
+        <v>184</v>
+      </c>
+      <c r="N39">
+        <f t="shared" si="5"/>
+        <v>6</v>
+      </c>
+      <c r="P39" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="40" spans="1:16">
+      <c r="A40" t="str">
+        <f t="shared" si="10"/>
+        <v>vstacks_t_annual~0007</v>
+      </c>
+      <c r="B40" t="str">
+        <f t="shared" si="7"/>
+        <v>Fragmented World_ann</v>
+      </c>
+      <c r="G40" t="str">
+        <f t="shared" si="8"/>
+        <v>Fragmented World_ann</v>
+      </c>
+      <c r="H40" t="str">
+        <f t="shared" si="4"/>
+        <v>Fragmented World</v>
+      </c>
+      <c r="I40" t="s">
+        <v>184</v>
+      </c>
+      <c r="N40">
+        <f t="shared" si="5"/>
+        <v>7</v>
+      </c>
+      <c r="P40" t="s">
+        <v>186</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="18" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -1948,10 +2362,10 @@
         <v>88</v>
       </c>
       <c r="B5" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="C5" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="D5">
         <v>1E-3</v>
@@ -1962,10 +2376,10 @@
         <v>88</v>
       </c>
       <c r="B6" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="C6" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="D6">
         <v>-1E-3</v>
@@ -1976,10 +2390,10 @@
         <v>88</v>
       </c>
       <c r="B7" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="C7" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="D7">
         <v>-1000</v>
@@ -1995,9 +2409,9 @@
   <sheetPr codeName="Sheet19"/>
   <dimension ref="A1:U13"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="Q5" sqref="Q5"/>
+      <selection pane="bottomLeft" activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25"/>
@@ -2095,16 +2509,13 @@
         <v>120</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>181</v>
+        <v>122</v>
       </c>
       <c r="K3" t="s">
         <v>10</v>
       </c>
       <c r="N3" t="s">
         <v>73</v>
-      </c>
-      <c r="Q3" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="4" spans="1:21">
@@ -2115,7 +2526,7 @@
         <v>120</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>181</v>
+        <v>122</v>
       </c>
       <c r="K4" t="s">
         <v>10</v>
@@ -2136,19 +2547,16 @@
         <v>121</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>182</v>
+        <v>122</v>
       </c>
       <c r="I5" t="s">
-        <v>183</v>
+        <v>123</v>
       </c>
       <c r="K5" t="s">
         <v>83</v>
       </c>
       <c r="N5" t="s">
         <v>84</v>
-      </c>
-      <c r="Q5" t="s">
-        <v>180</v>
       </c>
       <c r="T5" s="3" t="s">
         <v>47</v>
@@ -2162,7 +2570,7 @@
         <v>63</v>
       </c>
       <c r="C6" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="D6" s="2"/>
       <c r="H6" t="s">
@@ -2178,7 +2586,7 @@
         <v>44</v>
       </c>
       <c r="Q6" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="T6" s="3"/>
       <c r="U6" s="3"/>
@@ -2188,13 +2596,13 @@
         <v>7</v>
       </c>
       <c r="I7" s="2" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="K7" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="N7" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="T7" s="3"/>
       <c r="U7" s="3"/>
@@ -2204,13 +2612,13 @@
         <v>7</v>
       </c>
       <c r="I8" s="2" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="K8" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="N8" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="T8" s="3"/>
       <c r="U8" s="3"/>
@@ -2263,13 +2671,13 @@
         <v>59</v>
       </c>
       <c r="I11" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="K11" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="N11" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
     </row>
     <row r="12" spans="1:21">
@@ -2530,7 +2938,7 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
     </row>
     <row r="2" spans="1:3">
@@ -2546,32 +2954,32 @@
     </row>
     <row r="3" spans="1:3">
       <c r="A3" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="B3" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="C3" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" t="s">
+        <v>172</v>
+      </c>
+      <c r="B4" t="s">
+        <v>168</v>
+      </c>
+      <c r="C4" t="s">
         <v>171</v>
-      </c>
-      <c r="B4" t="s">
-        <v>167</v>
-      </c>
-      <c r="C4" t="s">
-        <v>170</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="B5" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="C5" t="str">
         <f>LEFT(B5,2)</f>
@@ -2580,10 +2988,10 @@
     </row>
     <row r="6" spans="1:3">
       <c r="A6" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="B6" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="C6" t="str">
         <f t="shared" ref="C6:C10" si="0">LEFT(B6,2)</f>
@@ -2592,10 +3000,10 @@
     </row>
     <row r="7" spans="1:3">
       <c r="A7" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="B7" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="C7" t="str">
         <f t="shared" si="0"/>
@@ -2604,10 +3012,10 @@
     </row>
     <row r="8" spans="1:3">
       <c r="A8" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="B8" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="C8" t="str">
         <f t="shared" si="0"/>
@@ -2616,10 +3024,10 @@
     </row>
     <row r="9" spans="1:3">
       <c r="A9" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="B9" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="C9" t="str">
         <f t="shared" si="0"/>
@@ -2628,10 +3036,10 @@
     </row>
     <row r="10" spans="1:3">
       <c r="A10" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="B10" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="C10" t="str">
         <f t="shared" si="0"/>
@@ -2910,13 +3318,13 @@
         <v>72</v>
       </c>
       <c r="C21" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="E21" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="F21" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
     </row>
     <row r="22" spans="1:6">
@@ -2924,13 +3332,13 @@
         <v>72</v>
       </c>
       <c r="C22" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="E22" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="F22" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
     </row>
     <row r="23" spans="1:6">
@@ -2938,13 +3346,13 @@
         <v>72</v>
       </c>
       <c r="B23" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="C23" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="E23" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
     </row>
     <row r="24" spans="1:6">
@@ -2952,13 +3360,13 @@
         <v>72</v>
       </c>
       <c r="B24" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="C24" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="E24" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
     </row>
     <row r="25" spans="1:6">
@@ -2996,24 +3404,24 @@
     </row>
     <row r="28" spans="1:6">
       <c r="A28" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="B28" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="C28" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
     </row>
     <row r="29" spans="1:6">
       <c r="A29" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="B29" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="C29" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated CHE_grids model - 2025-08-19 17:16
</commit_message>
<xml_diff>
--- a/VerveStacks_CHE_grids/ReportDefs_vervestacks.xlsx
+++ b/VerveStacks_CHE_grids/ReportDefs_vervestacks.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Veda\VerveStacks\assumptions\VerveStacks_ISO_template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50590F17-0DF5-46F5-9D74-7B91F86C55D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71AFBD00-C23B-4D68-8C24-F1A9F57C2964}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="17475" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="17475" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ScenMap" sheetId="56" r:id="rId1"/>
@@ -81,7 +81,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="442" uniqueCount="262">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="493" uniqueCount="257">
   <si>
     <t>Unit</t>
   </si>
@@ -92,12 +92,6 @@
     <t>Name</t>
   </si>
   <si>
-    <t>Hydro</t>
-  </si>
-  <si>
-    <t>Nuclear</t>
-  </si>
-  <si>
     <t>Solar</t>
   </si>
   <si>
@@ -380,15 +374,9 @@
     <t>Wind offshore</t>
   </si>
   <si>
-    <t>Geothermal</t>
-  </si>
-  <si>
     <t>Hydro pumped stg</t>
   </si>
   <si>
-    <t>Bioenergy</t>
-  </si>
-  <si>
     <t>Util Batt Stg</t>
   </si>
   <si>
@@ -485,27 +473,12 @@
     <t>timeslice</t>
   </si>
   <si>
-    <t>Delayed transition</t>
-  </si>
-  <si>
-    <t>Net Zero 2050</t>
-  </si>
-  <si>
-    <t>Current Policies</t>
-  </si>
-  <si>
     <t>Low demand</t>
   </si>
   <si>
     <t>Fragmented World</t>
   </si>
   <si>
-    <t>NDCs</t>
-  </si>
-  <si>
-    <t>Below 2deg</t>
-  </si>
-  <si>
     <t>3 days</t>
   </si>
   <si>
@@ -647,9 +620,6 @@
     <t>ELC,ELC_???-???,e[_]*</t>
   </si>
   <si>
-    <t>Grid</t>
-  </si>
-  <si>
     <t>T_neg_andor</t>
   </si>
   <si>
@@ -867,6 +837,21 @@
   </si>
   <si>
     <t>Transformers Up</t>
+  </si>
+  <si>
+    <t>Actual Policies</t>
+  </si>
+  <si>
+    <t>Declared NDCs</t>
+  </si>
+  <si>
+    <t>Limited to 2 deg</t>
+  </si>
+  <si>
+    <t>Postponed Transition</t>
+  </si>
+  <si>
+    <t>Target Net Zero 2050</t>
   </si>
 </sst>
 </file>
@@ -1413,8 +1398,8 @@
   <sheetPr codeName="Sheet11"/>
   <dimension ref="A1:P40"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A33" sqref="A33"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="L6" sqref="L6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.73046875" defaultRowHeight="14.25"/>
@@ -1432,43 +1417,43 @@
   <sheetData>
     <row r="1" spans="1:16">
       <c r="A1" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="B1" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="C1" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="D1" t="s">
-        <v>180</v>
+        <v>171</v>
       </c>
       <c r="E1" t="s">
-        <v>181</v>
+        <v>172</v>
       </c>
       <c r="H1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="2" spans="1:16">
       <c r="H2" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="I2" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
     </row>
     <row r="4" spans="1:16">
       <c r="A4" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="G4" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="5" spans="1:16">
       <c r="A5" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B5" t="s">
         <v>2</v>
@@ -1477,10 +1462,10 @@
         <v>1</v>
       </c>
       <c r="D5" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="G5" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="H5" t="str">
         <f>"sg_"&amp;H2</f>
@@ -1498,23 +1483,23 @@
       </c>
       <c r="B6" t="str">
         <f>G6</f>
-        <v>Delayed transition_3d</v>
+        <v>Postponed Transition_3d</v>
       </c>
       <c r="G6" t="str">
         <f>H6&amp;P6</f>
-        <v>Delayed transition_3d</v>
+        <v>Postponed Transition_3d</v>
       </c>
       <c r="H6" t="s">
-        <v>134</v>
+        <v>255</v>
       </c>
       <c r="I6" t="s">
-        <v>141</v>
+        <v>132</v>
       </c>
       <c r="N6">
         <v>1</v>
       </c>
       <c r="P6" t="s">
-        <v>144</v>
+        <v>135</v>
       </c>
     </row>
     <row r="7" spans="1:16">
@@ -1524,23 +1509,23 @@
       </c>
       <c r="B7" t="str">
         <f t="shared" ref="B7:B26" si="1">G7</f>
-        <v>Net Zero 2050_3d</v>
+        <v>Target Net Zero 2050_3d</v>
       </c>
       <c r="G7" t="str">
         <f t="shared" ref="G7:G26" si="2">H7&amp;P7</f>
-        <v>Net Zero 2050_3d</v>
+        <v>Target Net Zero 2050_3d</v>
       </c>
       <c r="H7" t="s">
-        <v>135</v>
+        <v>256</v>
       </c>
       <c r="I7" t="s">
-        <v>141</v>
+        <v>132</v>
       </c>
       <c r="N7">
         <v>2</v>
       </c>
       <c r="P7" t="s">
-        <v>144</v>
+        <v>135</v>
       </c>
     </row>
     <row r="8" spans="1:16">
@@ -1550,23 +1535,23 @@
       </c>
       <c r="B8" t="str">
         <f t="shared" si="1"/>
-        <v>NDCs_3d</v>
+        <v>Declared NDCs_3d</v>
       </c>
       <c r="G8" t="str">
         <f t="shared" si="2"/>
-        <v>NDCs_3d</v>
+        <v>Declared NDCs_3d</v>
       </c>
       <c r="H8" t="s">
-        <v>139</v>
+        <v>253</v>
       </c>
       <c r="I8" t="s">
-        <v>141</v>
+        <v>132</v>
       </c>
       <c r="N8">
         <v>3</v>
       </c>
       <c r="P8" t="s">
-        <v>144</v>
+        <v>135</v>
       </c>
     </row>
     <row r="9" spans="1:16">
@@ -1576,23 +1561,23 @@
       </c>
       <c r="B9" t="str">
         <f t="shared" si="1"/>
-        <v>Below 2deg_3d</v>
+        <v>Limited to 2 deg_3d</v>
       </c>
       <c r="G9" t="str">
         <f t="shared" si="2"/>
-        <v>Below 2deg_3d</v>
+        <v>Limited to 2 deg_3d</v>
       </c>
       <c r="H9" t="s">
-        <v>140</v>
+        <v>254</v>
       </c>
       <c r="I9" t="s">
-        <v>141</v>
+        <v>132</v>
       </c>
       <c r="N9">
         <v>4</v>
       </c>
       <c r="P9" t="s">
-        <v>144</v>
+        <v>135</v>
       </c>
     </row>
     <row r="10" spans="1:16">
@@ -1602,23 +1587,23 @@
       </c>
       <c r="B10" t="str">
         <f t="shared" si="1"/>
-        <v>Current Policies_3d</v>
+        <v>Actual Policies_3d</v>
       </c>
       <c r="G10" t="str">
         <f t="shared" si="2"/>
-        <v>Current Policies_3d</v>
+        <v>Actual Policies_3d</v>
       </c>
       <c r="H10" t="s">
-        <v>136</v>
+        <v>252</v>
       </c>
       <c r="I10" t="s">
-        <v>141</v>
+        <v>132</v>
       </c>
       <c r="N10">
         <v>5</v>
       </c>
       <c r="P10" t="s">
-        <v>144</v>
+        <v>135</v>
       </c>
     </row>
     <row r="11" spans="1:16">
@@ -1635,16 +1620,16 @@
         <v>Low demand_3d</v>
       </c>
       <c r="H11" t="s">
-        <v>137</v>
+        <v>130</v>
       </c>
       <c r="I11" t="s">
-        <v>141</v>
+        <v>132</v>
       </c>
       <c r="N11">
         <v>6</v>
       </c>
       <c r="P11" t="s">
-        <v>144</v>
+        <v>135</v>
       </c>
     </row>
     <row r="12" spans="1:16">
@@ -1661,16 +1646,16 @@
         <v>Fragmented World_3d</v>
       </c>
       <c r="H12" t="s">
-        <v>138</v>
+        <v>131</v>
       </c>
       <c r="I12" t="s">
-        <v>141</v>
+        <v>132</v>
       </c>
       <c r="N12">
         <v>7</v>
       </c>
       <c r="P12" t="s">
-        <v>144</v>
+        <v>135</v>
       </c>
     </row>
     <row r="13" spans="1:16">
@@ -1680,25 +1665,25 @@
       </c>
       <c r="B13" t="str">
         <f t="shared" si="1"/>
-        <v>Delayed transition_15d</v>
+        <v>Postponed Transition_15d</v>
       </c>
       <c r="G13" t="str">
         <f t="shared" si="2"/>
-        <v>Delayed transition_15d</v>
+        <v>Postponed Transition_15d</v>
       </c>
       <c r="H13" t="str">
         <f>H6</f>
-        <v>Delayed transition</v>
+        <v>Postponed Transition</v>
       </c>
       <c r="I13" t="s">
-        <v>142</v>
+        <v>133</v>
       </c>
       <c r="N13">
         <f>N6</f>
         <v>1</v>
       </c>
       <c r="P13" t="s">
-        <v>145</v>
+        <v>136</v>
       </c>
     </row>
     <row r="14" spans="1:16">
@@ -1708,25 +1693,25 @@
       </c>
       <c r="B14" t="str">
         <f t="shared" si="1"/>
-        <v>Net Zero 2050_15d</v>
+        <v>Target Net Zero 2050_15d</v>
       </c>
       <c r="G14" t="str">
         <f t="shared" si="2"/>
-        <v>Net Zero 2050_15d</v>
+        <v>Target Net Zero 2050_15d</v>
       </c>
       <c r="H14" t="str">
         <f t="shared" ref="H14:H40" si="4">H7</f>
-        <v>Net Zero 2050</v>
+        <v>Target Net Zero 2050</v>
       </c>
       <c r="I14" t="s">
-        <v>142</v>
+        <v>133</v>
       </c>
       <c r="N14">
         <f t="shared" ref="N14:N40" si="5">N7</f>
         <v>2</v>
       </c>
       <c r="P14" t="s">
-        <v>145</v>
+        <v>136</v>
       </c>
     </row>
     <row r="15" spans="1:16">
@@ -1736,25 +1721,25 @@
       </c>
       <c r="B15" t="str">
         <f t="shared" si="1"/>
-        <v>NDCs_15d</v>
+        <v>Declared NDCs_15d</v>
       </c>
       <c r="G15" t="str">
         <f t="shared" si="2"/>
-        <v>NDCs_15d</v>
+        <v>Declared NDCs_15d</v>
       </c>
       <c r="H15" t="str">
         <f t="shared" si="4"/>
-        <v>NDCs</v>
+        <v>Declared NDCs</v>
       </c>
       <c r="I15" t="s">
-        <v>142</v>
+        <v>133</v>
       </c>
       <c r="N15">
         <f t="shared" si="5"/>
         <v>3</v>
       </c>
       <c r="P15" t="s">
-        <v>145</v>
+        <v>136</v>
       </c>
     </row>
     <row r="16" spans="1:16">
@@ -1764,25 +1749,25 @@
       </c>
       <c r="B16" t="str">
         <f t="shared" si="1"/>
-        <v>Below 2deg_15d</v>
+        <v>Limited to 2 deg_15d</v>
       </c>
       <c r="G16" t="str">
         <f t="shared" si="2"/>
-        <v>Below 2deg_15d</v>
+        <v>Limited to 2 deg_15d</v>
       </c>
       <c r="H16" t="str">
         <f t="shared" si="4"/>
-        <v>Below 2deg</v>
+        <v>Limited to 2 deg</v>
       </c>
       <c r="I16" t="s">
-        <v>142</v>
+        <v>133</v>
       </c>
       <c r="N16">
         <f t="shared" si="5"/>
         <v>4</v>
       </c>
       <c r="P16" t="s">
-        <v>145</v>
+        <v>136</v>
       </c>
     </row>
     <row r="17" spans="1:16">
@@ -1792,25 +1777,25 @@
       </c>
       <c r="B17" t="str">
         <f t="shared" si="1"/>
-        <v>Current Policies_15d</v>
+        <v>Actual Policies_15d</v>
       </c>
       <c r="G17" t="str">
         <f t="shared" si="2"/>
-        <v>Current Policies_15d</v>
+        <v>Actual Policies_15d</v>
       </c>
       <c r="H17" t="str">
         <f t="shared" si="4"/>
-        <v>Current Policies</v>
+        <v>Actual Policies</v>
       </c>
       <c r="I17" t="s">
-        <v>142</v>
+        <v>133</v>
       </c>
       <c r="N17">
         <f t="shared" si="5"/>
         <v>5</v>
       </c>
       <c r="P17" t="s">
-        <v>145</v>
+        <v>136</v>
       </c>
     </row>
     <row r="18" spans="1:16">
@@ -1831,14 +1816,14 @@
         <v>Low demand</v>
       </c>
       <c r="I18" t="s">
-        <v>142</v>
+        <v>133</v>
       </c>
       <c r="N18">
         <f t="shared" si="5"/>
         <v>6</v>
       </c>
       <c r="P18" t="s">
-        <v>145</v>
+        <v>136</v>
       </c>
     </row>
     <row r="19" spans="1:16">
@@ -1859,14 +1844,14 @@
         <v>Fragmented World</v>
       </c>
       <c r="I19" t="s">
-        <v>142</v>
+        <v>133</v>
       </c>
       <c r="N19">
         <f t="shared" si="5"/>
         <v>7</v>
       </c>
       <c r="P19" t="s">
-        <v>145</v>
+        <v>136</v>
       </c>
     </row>
     <row r="20" spans="1:16">
@@ -1876,25 +1861,25 @@
       </c>
       <c r="B20" t="str">
         <f t="shared" si="1"/>
-        <v>Delayed transition_2w</v>
+        <v>Postponed Transition_2w</v>
       </c>
       <c r="G20" t="str">
         <f t="shared" si="2"/>
-        <v>Delayed transition_2w</v>
+        <v>Postponed Transition_2w</v>
       </c>
       <c r="H20" t="str">
         <f t="shared" si="4"/>
-        <v>Delayed transition</v>
+        <v>Postponed Transition</v>
       </c>
       <c r="I20" t="s">
-        <v>143</v>
+        <v>134</v>
       </c>
       <c r="N20">
         <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="P20" t="s">
-        <v>146</v>
+        <v>137</v>
       </c>
     </row>
     <row r="21" spans="1:16">
@@ -1904,25 +1889,25 @@
       </c>
       <c r="B21" t="str">
         <f t="shared" si="1"/>
-        <v>Net Zero 2050_2w</v>
+        <v>Target Net Zero 2050_2w</v>
       </c>
       <c r="G21" t="str">
         <f t="shared" si="2"/>
-        <v>Net Zero 2050_2w</v>
+        <v>Target Net Zero 2050_2w</v>
       </c>
       <c r="H21" t="str">
         <f t="shared" si="4"/>
-        <v>Net Zero 2050</v>
+        <v>Target Net Zero 2050</v>
       </c>
       <c r="I21" t="s">
-        <v>143</v>
+        <v>134</v>
       </c>
       <c r="N21">
         <f t="shared" si="5"/>
         <v>2</v>
       </c>
       <c r="P21" t="s">
-        <v>146</v>
+        <v>137</v>
       </c>
     </row>
     <row r="22" spans="1:16">
@@ -1932,25 +1917,25 @@
       </c>
       <c r="B22" t="str">
         <f t="shared" si="1"/>
-        <v>NDCs_2w</v>
+        <v>Declared NDCs_2w</v>
       </c>
       <c r="G22" t="str">
         <f t="shared" si="2"/>
-        <v>NDCs_2w</v>
+        <v>Declared NDCs_2w</v>
       </c>
       <c r="H22" t="str">
         <f t="shared" si="4"/>
-        <v>NDCs</v>
+        <v>Declared NDCs</v>
       </c>
       <c r="I22" t="s">
-        <v>143</v>
+        <v>134</v>
       </c>
       <c r="N22">
         <f t="shared" si="5"/>
         <v>3</v>
       </c>
       <c r="P22" t="s">
-        <v>146</v>
+        <v>137</v>
       </c>
     </row>
     <row r="23" spans="1:16">
@@ -1960,25 +1945,25 @@
       </c>
       <c r="B23" t="str">
         <f t="shared" si="1"/>
-        <v>Below 2deg_2w</v>
+        <v>Limited to 2 deg_2w</v>
       </c>
       <c r="G23" t="str">
         <f t="shared" si="2"/>
-        <v>Below 2deg_2w</v>
+        <v>Limited to 2 deg_2w</v>
       </c>
       <c r="H23" t="str">
         <f t="shared" si="4"/>
-        <v>Below 2deg</v>
+        <v>Limited to 2 deg</v>
       </c>
       <c r="I23" t="s">
-        <v>143</v>
+        <v>134</v>
       </c>
       <c r="N23">
         <f t="shared" si="5"/>
         <v>4</v>
       </c>
       <c r="P23" t="s">
-        <v>146</v>
+        <v>137</v>
       </c>
     </row>
     <row r="24" spans="1:16">
@@ -1988,25 +1973,25 @@
       </c>
       <c r="B24" t="str">
         <f t="shared" si="1"/>
-        <v>Current Policies_2w</v>
+        <v>Actual Policies_2w</v>
       </c>
       <c r="G24" t="str">
         <f t="shared" si="2"/>
-        <v>Current Policies_2w</v>
+        <v>Actual Policies_2w</v>
       </c>
       <c r="H24" t="str">
         <f t="shared" si="4"/>
-        <v>Current Policies</v>
+        <v>Actual Policies</v>
       </c>
       <c r="I24" t="s">
-        <v>143</v>
+        <v>134</v>
       </c>
       <c r="N24">
         <f t="shared" si="5"/>
         <v>5</v>
       </c>
       <c r="P24" t="s">
-        <v>146</v>
+        <v>137</v>
       </c>
     </row>
     <row r="25" spans="1:16">
@@ -2027,14 +2012,14 @@
         <v>Low demand</v>
       </c>
       <c r="I25" t="s">
-        <v>143</v>
+        <v>134</v>
       </c>
       <c r="N25">
         <f t="shared" si="5"/>
         <v>6</v>
       </c>
       <c r="P25" t="s">
-        <v>146</v>
+        <v>137</v>
       </c>
     </row>
     <row r="26" spans="1:16">
@@ -2055,14 +2040,14 @@
         <v>Fragmented World</v>
       </c>
       <c r="I26" t="s">
-        <v>143</v>
+        <v>134</v>
       </c>
       <c r="N26">
         <f t="shared" si="5"/>
         <v>7</v>
       </c>
       <c r="P26" t="s">
-        <v>146</v>
+        <v>137</v>
       </c>
     </row>
     <row r="27" spans="1:16">
@@ -2072,25 +2057,25 @@
       </c>
       <c r="B27" t="str">
         <f t="shared" ref="B27:B40" si="7">G27</f>
-        <v>Delayed transition_16</v>
+        <v>Postponed Transition_16</v>
       </c>
       <c r="G27" t="str">
         <f t="shared" ref="G27:G40" si="8">H27&amp;P27</f>
-        <v>Delayed transition_16</v>
+        <v>Postponed Transition_16</v>
       </c>
       <c r="H27" t="str">
         <f t="shared" si="4"/>
-        <v>Delayed transition</v>
+        <v>Postponed Transition</v>
       </c>
       <c r="I27" t="s">
-        <v>182</v>
+        <v>173</v>
       </c>
       <c r="N27">
         <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="P27" t="s">
-        <v>184</v>
+        <v>175</v>
       </c>
     </row>
     <row r="28" spans="1:16">
@@ -2100,25 +2085,25 @@
       </c>
       <c r="B28" t="str">
         <f t="shared" si="7"/>
-        <v>Net Zero 2050_16</v>
+        <v>Target Net Zero 2050_16</v>
       </c>
       <c r="G28" t="str">
         <f t="shared" si="8"/>
-        <v>Net Zero 2050_16</v>
+        <v>Target Net Zero 2050_16</v>
       </c>
       <c r="H28" t="str">
         <f t="shared" si="4"/>
-        <v>Net Zero 2050</v>
+        <v>Target Net Zero 2050</v>
       </c>
       <c r="I28" t="s">
-        <v>182</v>
+        <v>173</v>
       </c>
       <c r="N28">
         <f t="shared" si="5"/>
         <v>2</v>
       </c>
       <c r="P28" t="s">
-        <v>184</v>
+        <v>175</v>
       </c>
     </row>
     <row r="29" spans="1:16">
@@ -2128,25 +2113,25 @@
       </c>
       <c r="B29" t="str">
         <f t="shared" si="7"/>
-        <v>NDCs_16</v>
+        <v>Declared NDCs_16</v>
       </c>
       <c r="G29" t="str">
         <f t="shared" si="8"/>
-        <v>NDCs_16</v>
+        <v>Declared NDCs_16</v>
       </c>
       <c r="H29" t="str">
         <f t="shared" si="4"/>
-        <v>NDCs</v>
+        <v>Declared NDCs</v>
       </c>
       <c r="I29" t="s">
-        <v>182</v>
+        <v>173</v>
       </c>
       <c r="N29">
         <f t="shared" si="5"/>
         <v>3</v>
       </c>
       <c r="P29" t="s">
-        <v>184</v>
+        <v>175</v>
       </c>
     </row>
     <row r="30" spans="1:16">
@@ -2156,25 +2141,25 @@
       </c>
       <c r="B30" t="str">
         <f t="shared" si="7"/>
-        <v>Below 2deg_16</v>
+        <v>Limited to 2 deg_16</v>
       </c>
       <c r="G30" t="str">
         <f t="shared" si="8"/>
-        <v>Below 2deg_16</v>
+        <v>Limited to 2 deg_16</v>
       </c>
       <c r="H30" t="str">
         <f t="shared" si="4"/>
-        <v>Below 2deg</v>
+        <v>Limited to 2 deg</v>
       </c>
       <c r="I30" t="s">
-        <v>182</v>
+        <v>173</v>
       </c>
       <c r="N30">
         <f t="shared" si="5"/>
         <v>4</v>
       </c>
       <c r="P30" t="s">
-        <v>184</v>
+        <v>175</v>
       </c>
     </row>
     <row r="31" spans="1:16">
@@ -2184,25 +2169,25 @@
       </c>
       <c r="B31" t="str">
         <f t="shared" si="7"/>
-        <v>Current Policies_16</v>
+        <v>Actual Policies_16</v>
       </c>
       <c r="G31" t="str">
         <f t="shared" si="8"/>
-        <v>Current Policies_16</v>
+        <v>Actual Policies_16</v>
       </c>
       <c r="H31" t="str">
         <f t="shared" si="4"/>
-        <v>Current Policies</v>
+        <v>Actual Policies</v>
       </c>
       <c r="I31" t="s">
-        <v>182</v>
+        <v>173</v>
       </c>
       <c r="N31">
         <f t="shared" si="5"/>
         <v>5</v>
       </c>
       <c r="P31" t="s">
-        <v>184</v>
+        <v>175</v>
       </c>
     </row>
     <row r="32" spans="1:16">
@@ -2223,14 +2208,14 @@
         <v>Low demand</v>
       </c>
       <c r="I32" t="s">
-        <v>182</v>
+        <v>173</v>
       </c>
       <c r="N32">
         <f t="shared" si="5"/>
         <v>6</v>
       </c>
       <c r="P32" t="s">
-        <v>184</v>
+        <v>175</v>
       </c>
     </row>
     <row r="33" spans="1:16">
@@ -2251,14 +2236,14 @@
         <v>Fragmented World</v>
       </c>
       <c r="I33" t="s">
-        <v>182</v>
+        <v>173</v>
       </c>
       <c r="N33">
         <f t="shared" si="5"/>
         <v>7</v>
       </c>
       <c r="P33" t="s">
-        <v>184</v>
+        <v>175</v>
       </c>
     </row>
     <row r="34" spans="1:16">
@@ -2268,25 +2253,25 @@
       </c>
       <c r="B34" t="str">
         <f t="shared" si="7"/>
-        <v>Delayed transition_ann</v>
+        <v>Postponed Transition_ann</v>
       </c>
       <c r="G34" t="str">
         <f t="shared" si="8"/>
-        <v>Delayed transition_ann</v>
+        <v>Postponed Transition_ann</v>
       </c>
       <c r="H34" t="str">
         <f t="shared" si="4"/>
-        <v>Delayed transition</v>
+        <v>Postponed Transition</v>
       </c>
       <c r="I34" t="s">
-        <v>183</v>
+        <v>174</v>
       </c>
       <c r="N34">
         <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="P34" t="s">
-        <v>185</v>
+        <v>176</v>
       </c>
     </row>
     <row r="35" spans="1:16">
@@ -2296,25 +2281,25 @@
       </c>
       <c r="B35" t="str">
         <f t="shared" si="7"/>
-        <v>Net Zero 2050_ann</v>
+        <v>Target Net Zero 2050_ann</v>
       </c>
       <c r="G35" t="str">
         <f t="shared" si="8"/>
-        <v>Net Zero 2050_ann</v>
+        <v>Target Net Zero 2050_ann</v>
       </c>
       <c r="H35" t="str">
         <f t="shared" si="4"/>
-        <v>Net Zero 2050</v>
+        <v>Target Net Zero 2050</v>
       </c>
       <c r="I35" t="s">
-        <v>183</v>
+        <v>174</v>
       </c>
       <c r="N35">
         <f t="shared" si="5"/>
         <v>2</v>
       </c>
       <c r="P35" t="s">
-        <v>185</v>
+        <v>176</v>
       </c>
     </row>
     <row r="36" spans="1:16">
@@ -2324,25 +2309,25 @@
       </c>
       <c r="B36" t="str">
         <f t="shared" si="7"/>
-        <v>NDCs_ann</v>
+        <v>Declared NDCs_ann</v>
       </c>
       <c r="G36" t="str">
         <f t="shared" si="8"/>
-        <v>NDCs_ann</v>
+        <v>Declared NDCs_ann</v>
       </c>
       <c r="H36" t="str">
         <f t="shared" si="4"/>
-        <v>NDCs</v>
+        <v>Declared NDCs</v>
       </c>
       <c r="I36" t="s">
-        <v>183</v>
+        <v>174</v>
       </c>
       <c r="N36">
         <f t="shared" si="5"/>
         <v>3</v>
       </c>
       <c r="P36" t="s">
-        <v>185</v>
+        <v>176</v>
       </c>
     </row>
     <row r="37" spans="1:16">
@@ -2352,25 +2337,25 @@
       </c>
       <c r="B37" t="str">
         <f t="shared" si="7"/>
-        <v>Below 2deg_ann</v>
+        <v>Limited to 2 deg_ann</v>
       </c>
       <c r="G37" t="str">
         <f t="shared" si="8"/>
-        <v>Below 2deg_ann</v>
+        <v>Limited to 2 deg_ann</v>
       </c>
       <c r="H37" t="str">
         <f t="shared" si="4"/>
-        <v>Below 2deg</v>
+        <v>Limited to 2 deg</v>
       </c>
       <c r="I37" t="s">
-        <v>183</v>
+        <v>174</v>
       </c>
       <c r="N37">
         <f t="shared" si="5"/>
         <v>4</v>
       </c>
       <c r="P37" t="s">
-        <v>185</v>
+        <v>176</v>
       </c>
     </row>
     <row r="38" spans="1:16">
@@ -2380,25 +2365,25 @@
       </c>
       <c r="B38" t="str">
         <f t="shared" si="7"/>
-        <v>Current Policies_ann</v>
+        <v>Actual Policies_ann</v>
       </c>
       <c r="G38" t="str">
         <f t="shared" si="8"/>
-        <v>Current Policies_ann</v>
+        <v>Actual Policies_ann</v>
       </c>
       <c r="H38" t="str">
         <f t="shared" si="4"/>
-        <v>Current Policies</v>
+        <v>Actual Policies</v>
       </c>
       <c r="I38" t="s">
-        <v>183</v>
+        <v>174</v>
       </c>
       <c r="N38">
         <f t="shared" si="5"/>
         <v>5</v>
       </c>
       <c r="P38" t="s">
-        <v>185</v>
+        <v>176</v>
       </c>
     </row>
     <row r="39" spans="1:16">
@@ -2419,14 +2404,14 @@
         <v>Low demand</v>
       </c>
       <c r="I39" t="s">
-        <v>183</v>
+        <v>174</v>
       </c>
       <c r="N39">
         <f t="shared" si="5"/>
         <v>6</v>
       </c>
       <c r="P39" t="s">
-        <v>185</v>
+        <v>176</v>
       </c>
     </row>
     <row r="40" spans="1:16">
@@ -2447,14 +2432,14 @@
         <v>Fragmented World</v>
       </c>
       <c r="I40" t="s">
-        <v>183</v>
+        <v>174</v>
       </c>
       <c r="N40">
         <f t="shared" si="5"/>
         <v>7</v>
       </c>
       <c r="P40" t="s">
-        <v>185</v>
+        <v>176</v>
       </c>
     </row>
   </sheetData>
@@ -2484,33 +2469,33 @@
   <sheetData>
     <row r="1" spans="1:8">
       <c r="A1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="2" spans="1:8">
       <c r="A2" t="s">
+        <v>54</v>
+      </c>
+      <c r="B2" t="s">
+        <v>55</v>
+      </c>
+      <c r="C2" t="s">
         <v>56</v>
       </c>
-      <c r="B2" t="s">
-        <v>57</v>
-      </c>
-      <c r="C2" t="s">
-        <v>58</v>
-      </c>
       <c r="D2" t="s">
+        <v>75</v>
+      </c>
+      <c r="E2" t="s">
+        <v>76</v>
+      </c>
+      <c r="F2" t="s">
+        <v>78</v>
+      </c>
+      <c r="G2" t="s">
         <v>77</v>
       </c>
-      <c r="E2" t="s">
-        <v>78</v>
-      </c>
-      <c r="F2" t="s">
-        <v>80</v>
-      </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>79</v>
-      </c>
-      <c r="H2" t="s">
-        <v>81</v>
       </c>
     </row>
   </sheetData>
@@ -2532,30 +2517,30 @@
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="2" spans="1:7">
       <c r="A2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C2" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D2" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="E2" t="s">
         <v>0</v>
       </c>
       <c r="F2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="G2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -2590,32 +2575,32 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="D2" s="1" t="s">
         <v>35</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B3" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C3" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D3">
         <f>1/8.76</f>
@@ -2624,13 +2609,13 @@
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B4" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="C4" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="D4">
         <f>1/8.76*100</f>
@@ -2639,13 +2624,13 @@
     </row>
     <row r="5" spans="1:4">
       <c r="A5" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B5" t="s">
-        <v>149</v>
+        <v>140</v>
       </c>
       <c r="C5" t="s">
-        <v>153</v>
+        <v>144</v>
       </c>
       <c r="D5">
         <v>1E-3</v>
@@ -2653,13 +2638,13 @@
     </row>
     <row r="6" spans="1:4">
       <c r="A6" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B6" t="s">
-        <v>150</v>
+        <v>141</v>
       </c>
       <c r="C6" t="s">
-        <v>153</v>
+        <v>144</v>
       </c>
       <c r="D6">
         <v>-1E-3</v>
@@ -2667,13 +2652,13 @@
     </row>
     <row r="7" spans="1:4">
       <c r="A7" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B7" t="s">
-        <v>163</v>
+        <v>154</v>
       </c>
       <c r="C7" t="s">
-        <v>165</v>
+        <v>156</v>
       </c>
       <c r="D7">
         <v>-1000</v>
@@ -2722,48 +2707,48 @@
   <sheetData>
     <row r="1" spans="1:21" ht="17.25" thickBot="1">
       <c r="A1" s="5" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:21" ht="15" thickTop="1" thickBot="1">
       <c r="A2" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="B2" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="C2" s="6" t="s">
+      <c r="E2" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="F2" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="G2" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="H2" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="I2" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="E2" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="F2" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="G2" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="H2" s="6" t="s">
+      <c r="J2" s="6" t="s">
         <v>16</v>
-      </c>
-      <c r="I2" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="J2" s="6" t="s">
-        <v>18</v>
       </c>
       <c r="K2" s="6" t="s">
         <v>0</v>
       </c>
       <c r="L2" s="6" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="M2" s="6" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="N2" s="6" t="s">
         <v>2</v>
@@ -2772,226 +2757,226 @@
         <v>1</v>
       </c>
       <c r="P2" s="6" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="Q2" s="6" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="R2" s="6" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="3" spans="1:21">
       <c r="A3" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C3" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>186</v>
+        <v>177</v>
       </c>
       <c r="K3" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="N3" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="4" spans="1:21">
       <c r="A4" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C4" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>186</v>
+        <v>177</v>
       </c>
       <c r="K4" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="N4" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="T4" s="8" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="U4" s="8"/>
     </row>
     <row r="5" spans="1:21">
       <c r="A5" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C5" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>186</v>
+        <v>177</v>
       </c>
       <c r="I5" t="s">
-        <v>187</v>
+        <v>178</v>
       </c>
       <c r="K5" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="N5" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="T5" s="3" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="U5" s="3" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="6" spans="1:21">
       <c r="A6" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C6" t="s">
-        <v>166</v>
+        <v>157</v>
       </c>
       <c r="D6" s="2"/>
       <c r="H6" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="I6" s="2" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="K6" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="N6" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="Q6" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="T6" s="3"/>
       <c r="U6" s="3"/>
     </row>
     <row r="7" spans="1:21">
       <c r="A7" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="I7" s="2" t="s">
-        <v>147</v>
+        <v>138</v>
       </c>
       <c r="K7" t="s">
-        <v>149</v>
+        <v>140</v>
       </c>
       <c r="N7" t="s">
-        <v>151</v>
+        <v>142</v>
       </c>
       <c r="T7" s="3"/>
       <c r="U7" s="3"/>
     </row>
     <row r="8" spans="1:21">
       <c r="A8" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="I8" s="2" t="s">
-        <v>148</v>
+        <v>139</v>
       </c>
       <c r="K8" t="s">
-        <v>150</v>
+        <v>141</v>
       </c>
       <c r="N8" t="s">
-        <v>152</v>
+        <v>143</v>
       </c>
       <c r="T8" s="3"/>
       <c r="U8" s="3"/>
     </row>
     <row r="9" spans="1:21">
       <c r="A9" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C9" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="K9" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="N9" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="10" spans="1:21">
       <c r="A10" s="4" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="H10" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="K10" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="N10" t="s">
+        <v>46</v>
+      </c>
+      <c r="P10" t="s">
+        <v>47</v>
+      </c>
+      <c r="Q10" t="s">
         <v>48</v>
-      </c>
-      <c r="P10" t="s">
-        <v>49</v>
-      </c>
-      <c r="Q10" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="11" spans="1:21">
       <c r="A11" s="4" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="I11" t="s">
-        <v>162</v>
+        <v>153</v>
       </c>
       <c r="K11" t="s">
-        <v>163</v>
+        <v>154</v>
       </c>
       <c r="N11" t="s">
-        <v>164</v>
+        <v>155</v>
       </c>
     </row>
     <row r="12" spans="1:21">
       <c r="A12" t="s">
+        <v>49</v>
+      </c>
+      <c r="K12" t="s">
+        <v>85</v>
+      </c>
+      <c r="N12" t="s">
+        <v>50</v>
+      </c>
+      <c r="P12" t="s">
+        <v>52</v>
+      </c>
+      <c r="Q12" t="s">
         <v>51</v>
-      </c>
-      <c r="K12" t="s">
-        <v>87</v>
-      </c>
-      <c r="N12" t="s">
-        <v>52</v>
-      </c>
-      <c r="P12" t="s">
-        <v>54</v>
-      </c>
-      <c r="Q12" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="13" spans="1:21">
       <c r="A13" s="4" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="K13" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="N13" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="Q13" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
   </sheetData>
@@ -3026,15 +3011,15 @@
   <sheetData>
     <row r="1" spans="3:11">
       <c r="C1" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
     </row>
     <row r="2" spans="3:11">
       <c r="C2" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="D2" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>2</v>
@@ -3043,42 +3028,42 @@
         <v>0</v>
       </c>
       <c r="G2" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="H2" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="I2" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="J2" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="K2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3" spans="3:11">
       <c r="C3" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D3" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="E3" s="7" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="F3" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="G3" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="I3" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="J3" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
   </sheetData>
@@ -3121,45 +3106,45 @@
   <sheetData>
     <row r="3" spans="1:19" ht="17.25" thickBot="1">
       <c r="A3" s="5" t="s">
-        <v>191</v>
+        <v>181</v>
       </c>
     </row>
     <row r="4" spans="1:19" ht="15" thickTop="1" thickBot="1">
       <c r="A4" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="B4" s="6" t="s">
+      <c r="D4" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="E4" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="F4" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="G4" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="C4" s="6" t="s">
+      <c r="H4" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="D4" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="E4" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="F4" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="G4" s="6" t="s">
+      <c r="I4" s="6" t="s">
         <v>16</v>
-      </c>
-      <c r="H4" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="I4" s="6" t="s">
-        <v>18</v>
       </c>
       <c r="J4" s="6" t="s">
         <v>0</v>
       </c>
       <c r="K4" s="6" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="L4" s="6" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="M4" s="6" t="s">
         <v>2</v>
@@ -3168,24 +3153,24 @@
         <v>1</v>
       </c>
       <c r="O4" s="6" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="P4" s="6" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="Q4" s="6" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="R4" s="6" t="s">
-        <v>189</v>
+        <v>179</v>
       </c>
       <c r="S4" s="6" t="s">
-        <v>190</v>
+        <v>180</v>
       </c>
     </row>
     <row r="5" spans="1:19">
       <c r="A5" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B5" t="str">
         <f>_xlfn.TEXTJOIN(",",TRUE,PSet_MAP!$A$3:$A$49)</f>
@@ -3196,10 +3181,10 @@
         <v>Elec-220V,Elec-400V,Elec-380V,Elec-225V,Elec-330V,Elec-275V,Elec-420V,Elec-300V,Elec-500V,Elec-750V,Elec-450V,Elec-515V,Elec-525V,Elec-320V,Elec-150V,Elec-270V,Elec-350V,Elec-250V,Elec-200V,Elec-236V,Elec-600V,Solar elec,Wind elec,fossil,renewable,bioenergy,hydrogen,nuclear,ELC,buildings,industry,transport,EVs</v>
       </c>
       <c r="J5" t="s">
-        <v>192</v>
+        <v>182</v>
       </c>
       <c r="M5" t="s">
-        <v>224</v>
+        <v>214</v>
       </c>
       <c r="S5">
         <v>-1</v>
@@ -3207,7 +3192,7 @@
     </row>
     <row r="6" spans="1:19">
       <c r="A6" t="s">
-        <v>193</v>
+        <v>183</v>
       </c>
       <c r="B6" t="str">
         <f>_xlfn.TEXTJOIN(",",TRUE,PSet_MAP!$A$3:$A$49)</f>
@@ -3218,10 +3203,10 @@
         <v>Elec-220V,Elec-400V,Elec-380V,Elec-225V,Elec-330V,Elec-275V,Elec-420V,Elec-300V,Elec-500V,Elec-750V,Elec-450V,Elec-515V,Elec-525V,Elec-320V,Elec-150V,Elec-270V,Elec-350V,Elec-250V,Elec-200V,Elec-236V,Elec-600V,Solar elec,Wind elec,fossil,renewable,bioenergy,hydrogen,nuclear,ELC,buildings,industry,transport,EVs</v>
       </c>
       <c r="J6" t="s">
-        <v>192</v>
+        <v>182</v>
       </c>
       <c r="M6" t="s">
-        <v>225</v>
+        <v>215</v>
       </c>
       <c r="S6">
         <v>-1</v>
@@ -3237,8 +3222,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:C47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="B36" sqref="B36"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:A47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25"/>
@@ -3250,23 +3235,23 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B2" t="s">
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B3" t="str">
         <f>A3</f>
@@ -3275,7 +3260,7 @@
     </row>
     <row r="4" spans="1:3">
       <c r="A4" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B4" t="str">
         <f t="shared" ref="B4:B47" si="0">A4</f>
@@ -3284,7 +3269,7 @@
     </row>
     <row r="5" spans="1:3">
       <c r="A5" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B5" t="str">
         <f t="shared" si="0"/>
@@ -3293,7 +3278,7 @@
     </row>
     <row r="6" spans="1:3">
       <c r="A6" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B6" t="str">
         <f t="shared" si="0"/>
@@ -3302,7 +3287,7 @@
     </row>
     <row r="7" spans="1:3">
       <c r="A7" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B7" t="str">
         <f t="shared" si="0"/>
@@ -3311,7 +3296,7 @@
     </row>
     <row r="8" spans="1:3">
       <c r="A8" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B8" t="str">
         <f t="shared" si="0"/>
@@ -3320,7 +3305,7 @@
     </row>
     <row r="9" spans="1:3">
       <c r="A9" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B9" t="str">
         <f t="shared" si="0"/>
@@ -3329,7 +3314,7 @@
     </row>
     <row r="10" spans="1:3">
       <c r="A10" t="s">
-        <v>227</v>
+        <v>217</v>
       </c>
       <c r="B10" t="str">
         <f t="shared" si="0"/>
@@ -3338,7 +3323,7 @@
     </row>
     <row r="11" spans="1:3">
       <c r="A11" t="s">
-        <v>228</v>
+        <v>218</v>
       </c>
       <c r="B11" t="str">
         <f t="shared" si="0"/>
@@ -3347,7 +3332,7 @@
     </row>
     <row r="12" spans="1:3">
       <c r="A12" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B12" t="str">
         <f t="shared" si="0"/>
@@ -3356,7 +3341,7 @@
     </row>
     <row r="13" spans="1:3">
       <c r="A13" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B13" t="str">
         <f t="shared" si="0"/>
@@ -3365,7 +3350,7 @@
     </row>
     <row r="14" spans="1:3">
       <c r="A14" t="s">
-        <v>229</v>
+        <v>219</v>
       </c>
       <c r="B14" t="str">
         <f t="shared" si="0"/>
@@ -3374,7 +3359,7 @@
     </row>
     <row r="15" spans="1:3">
       <c r="A15" t="s">
-        <v>233</v>
+        <v>223</v>
       </c>
       <c r="B15" t="str">
         <f t="shared" si="0"/>
@@ -3383,7 +3368,7 @@
     </row>
     <row r="16" spans="1:3">
       <c r="A16" t="s">
-        <v>230</v>
+        <v>220</v>
       </c>
       <c r="B16" t="str">
         <f t="shared" si="0"/>
@@ -3392,7 +3377,7 @@
     </row>
     <row r="17" spans="1:2">
       <c r="A17" t="s">
-        <v>231</v>
+        <v>221</v>
       </c>
       <c r="B17" t="str">
         <f t="shared" si="0"/>
@@ -3401,7 +3386,7 @@
     </row>
     <row r="18" spans="1:2">
       <c r="A18" t="s">
-        <v>232</v>
+        <v>222</v>
       </c>
       <c r="B18" t="str">
         <f t="shared" si="0"/>
@@ -3410,7 +3395,7 @@
     </row>
     <row r="19" spans="1:2">
       <c r="A19" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="B19" t="str">
         <f t="shared" si="0"/>
@@ -3419,7 +3404,7 @@
     </row>
     <row r="20" spans="1:2">
       <c r="A20" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="B20" t="str">
         <f t="shared" si="0"/>
@@ -3428,7 +3413,7 @@
     </row>
     <row r="21" spans="1:2">
       <c r="A21" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="B21" t="str">
         <f t="shared" si="0"/>
@@ -3437,7 +3422,7 @@
     </row>
     <row r="22" spans="1:2">
       <c r="A22" t="s">
-        <v>194</v>
+        <v>184</v>
       </c>
       <c r="B22" t="str">
         <f t="shared" si="0"/>
@@ -3446,7 +3431,7 @@
     </row>
     <row r="23" spans="1:2">
       <c r="A23" t="s">
-        <v>260</v>
+        <v>250</v>
       </c>
       <c r="B23" t="str">
         <f t="shared" si="0"/>
@@ -3455,7 +3440,7 @@
     </row>
     <row r="24" spans="1:2">
       <c r="A24" t="s">
-        <v>261</v>
+        <v>251</v>
       </c>
       <c r="B24" t="str">
         <f t="shared" si="0"/>
@@ -3464,7 +3449,7 @@
     </row>
     <row r="25" spans="1:2">
       <c r="A25" t="s">
-        <v>237</v>
+        <v>227</v>
       </c>
       <c r="B25" t="str">
         <f t="shared" si="0"/>
@@ -3473,7 +3458,7 @@
     </row>
     <row r="26" spans="1:2">
       <c r="A26" t="s">
-        <v>238</v>
+        <v>228</v>
       </c>
       <c r="B26" t="str">
         <f t="shared" si="0"/>
@@ -3482,7 +3467,7 @@
     </row>
     <row r="27" spans="1:2">
       <c r="A27" t="s">
-        <v>239</v>
+        <v>229</v>
       </c>
       <c r="B27" t="str">
         <f t="shared" si="0"/>
@@ -3491,7 +3476,7 @@
     </row>
     <row r="28" spans="1:2">
       <c r="A28" t="s">
-        <v>240</v>
+        <v>230</v>
       </c>
       <c r="B28" t="str">
         <f t="shared" si="0"/>
@@ -3500,7 +3485,7 @@
     </row>
     <row r="29" spans="1:2">
       <c r="A29" t="s">
-        <v>241</v>
+        <v>231</v>
       </c>
       <c r="B29" t="str">
         <f t="shared" si="0"/>
@@ -3509,7 +3494,7 @@
     </row>
     <row r="30" spans="1:2">
       <c r="A30" t="s">
-        <v>242</v>
+        <v>232</v>
       </c>
       <c r="B30" t="str">
         <f t="shared" si="0"/>
@@ -3518,7 +3503,7 @@
     </row>
     <row r="31" spans="1:2">
       <c r="A31" t="s">
-        <v>243</v>
+        <v>233</v>
       </c>
       <c r="B31" t="str">
         <f t="shared" si="0"/>
@@ -3527,7 +3512,7 @@
     </row>
     <row r="32" spans="1:2">
       <c r="A32" t="s">
-        <v>244</v>
+        <v>234</v>
       </c>
       <c r="B32" t="str">
         <f t="shared" si="0"/>
@@ -3536,7 +3521,7 @@
     </row>
     <row r="33" spans="1:2">
       <c r="A33" t="s">
-        <v>245</v>
+        <v>235</v>
       </c>
       <c r="B33" t="str">
         <f t="shared" si="0"/>
@@ -3545,7 +3530,7 @@
     </row>
     <row r="34" spans="1:2">
       <c r="A34" t="s">
-        <v>246</v>
+        <v>236</v>
       </c>
       <c r="B34" t="str">
         <f t="shared" si="0"/>
@@ -3554,7 +3539,7 @@
     </row>
     <row r="35" spans="1:2">
       <c r="A35" t="s">
-        <v>247</v>
+        <v>237</v>
       </c>
       <c r="B35" t="str">
         <f t="shared" si="0"/>
@@ -3563,7 +3548,7 @@
     </row>
     <row r="36" spans="1:2">
       <c r="A36" t="s">
-        <v>248</v>
+        <v>238</v>
       </c>
       <c r="B36" t="str">
         <f t="shared" si="0"/>
@@ -3572,7 +3557,7 @@
     </row>
     <row r="37" spans="1:2">
       <c r="A37" t="s">
-        <v>249</v>
+        <v>239</v>
       </c>
       <c r="B37" t="str">
         <f t="shared" si="0"/>
@@ -3581,7 +3566,7 @@
     </row>
     <row r="38" spans="1:2">
       <c r="A38" t="s">
-        <v>250</v>
+        <v>240</v>
       </c>
       <c r="B38" t="str">
         <f t="shared" si="0"/>
@@ -3590,7 +3575,7 @@
     </row>
     <row r="39" spans="1:2">
       <c r="A39" t="s">
-        <v>251</v>
+        <v>241</v>
       </c>
       <c r="B39" t="str">
         <f t="shared" si="0"/>
@@ -3599,7 +3584,7 @@
     </row>
     <row r="40" spans="1:2">
       <c r="A40" t="s">
-        <v>252</v>
+        <v>242</v>
       </c>
       <c r="B40" t="str">
         <f t="shared" si="0"/>
@@ -3608,7 +3593,7 @@
     </row>
     <row r="41" spans="1:2">
       <c r="A41" t="s">
-        <v>253</v>
+        <v>243</v>
       </c>
       <c r="B41" t="str">
         <f t="shared" si="0"/>
@@ -3617,7 +3602,7 @@
     </row>
     <row r="42" spans="1:2">
       <c r="A42" t="s">
-        <v>254</v>
+        <v>244</v>
       </c>
       <c r="B42" t="str">
         <f t="shared" si="0"/>
@@ -3626,7 +3611,7 @@
     </row>
     <row r="43" spans="1:2">
       <c r="A43" t="s">
-        <v>255</v>
+        <v>245</v>
       </c>
       <c r="B43" t="str">
         <f t="shared" si="0"/>
@@ -3635,7 +3620,7 @@
     </row>
     <row r="44" spans="1:2">
       <c r="A44" t="s">
-        <v>256</v>
+        <v>246</v>
       </c>
       <c r="B44" t="str">
         <f t="shared" si="0"/>
@@ -3644,7 +3629,7 @@
     </row>
     <row r="45" spans="1:2">
       <c r="A45" t="s">
-        <v>257</v>
+        <v>247</v>
       </c>
       <c r="B45" t="str">
         <f t="shared" si="0"/>
@@ -3653,7 +3638,7 @@
     </row>
     <row r="46" spans="1:2">
       <c r="A46" t="s">
-        <v>258</v>
+        <v>248</v>
       </c>
       <c r="B46" t="str">
         <f t="shared" si="0"/>
@@ -3662,7 +3647,7 @@
     </row>
     <row r="47" spans="1:2">
       <c r="A47" t="s">
-        <v>259</v>
+        <v>249</v>
       </c>
       <c r="B47" t="str">
         <f t="shared" si="0"/>
@@ -3690,23 +3675,23 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B2" t="s">
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" t="s">
-        <v>195</v>
+        <v>185</v>
       </c>
       <c r="B3" t="str">
         <f>A3</f>
@@ -3715,7 +3700,7 @@
     </row>
     <row r="4" spans="1:3">
       <c r="A4" t="s">
-        <v>196</v>
+        <v>186</v>
       </c>
       <c r="B4" t="str">
         <f t="shared" ref="B4:B35" si="0">A4</f>
@@ -3724,7 +3709,7 @@
     </row>
     <row r="5" spans="1:3">
       <c r="A5" t="s">
-        <v>197</v>
+        <v>187</v>
       </c>
       <c r="B5" t="str">
         <f t="shared" si="0"/>
@@ -3733,7 +3718,7 @@
     </row>
     <row r="6" spans="1:3">
       <c r="A6" t="s">
-        <v>198</v>
+        <v>188</v>
       </c>
       <c r="B6" t="str">
         <f t="shared" si="0"/>
@@ -3742,7 +3727,7 @@
     </row>
     <row r="7" spans="1:3">
       <c r="A7" t="s">
-        <v>199</v>
+        <v>189</v>
       </c>
       <c r="B7" t="str">
         <f t="shared" si="0"/>
@@ -3751,7 +3736,7 @@
     </row>
     <row r="8" spans="1:3">
       <c r="A8" t="s">
-        <v>200</v>
+        <v>190</v>
       </c>
       <c r="B8" t="str">
         <f t="shared" si="0"/>
@@ -3760,7 +3745,7 @@
     </row>
     <row r="9" spans="1:3">
       <c r="A9" t="s">
-        <v>201</v>
+        <v>191</v>
       </c>
       <c r="B9" t="str">
         <f t="shared" si="0"/>
@@ -3769,7 +3754,7 @@
     </row>
     <row r="10" spans="1:3">
       <c r="A10" t="s">
-        <v>202</v>
+        <v>192</v>
       </c>
       <c r="B10" t="str">
         <f t="shared" si="0"/>
@@ -3778,7 +3763,7 @@
     </row>
     <row r="11" spans="1:3">
       <c r="A11" t="s">
-        <v>203</v>
+        <v>193</v>
       </c>
       <c r="B11" t="str">
         <f t="shared" si="0"/>
@@ -3787,7 +3772,7 @@
     </row>
     <row r="12" spans="1:3">
       <c r="A12" t="s">
-        <v>204</v>
+        <v>194</v>
       </c>
       <c r="B12" t="str">
         <f t="shared" si="0"/>
@@ -3796,7 +3781,7 @@
     </row>
     <row r="13" spans="1:3">
       <c r="A13" t="s">
-        <v>205</v>
+        <v>195</v>
       </c>
       <c r="B13" t="str">
         <f t="shared" si="0"/>
@@ -3805,7 +3790,7 @@
     </row>
     <row r="14" spans="1:3">
       <c r="A14" t="s">
-        <v>206</v>
+        <v>196</v>
       </c>
       <c r="B14" t="str">
         <f t="shared" si="0"/>
@@ -3814,7 +3799,7 @@
     </row>
     <row r="15" spans="1:3">
       <c r="A15" t="s">
-        <v>207</v>
+        <v>197</v>
       </c>
       <c r="B15" t="str">
         <f t="shared" si="0"/>
@@ -3823,7 +3808,7 @@
     </row>
     <row r="16" spans="1:3">
       <c r="A16" t="s">
-        <v>208</v>
+        <v>198</v>
       </c>
       <c r="B16" t="str">
         <f t="shared" si="0"/>
@@ -3832,7 +3817,7 @@
     </row>
     <row r="17" spans="1:2">
       <c r="A17" t="s">
-        <v>209</v>
+        <v>199</v>
       </c>
       <c r="B17" t="str">
         <f t="shared" si="0"/>
@@ -3841,7 +3826,7 @@
     </row>
     <row r="18" spans="1:2">
       <c r="A18" t="s">
-        <v>210</v>
+        <v>200</v>
       </c>
       <c r="B18" t="str">
         <f t="shared" si="0"/>
@@ -3850,7 +3835,7 @@
     </row>
     <row r="19" spans="1:2">
       <c r="A19" t="s">
-        <v>211</v>
+        <v>201</v>
       </c>
       <c r="B19" t="str">
         <f t="shared" si="0"/>
@@ -3859,7 +3844,7 @@
     </row>
     <row r="20" spans="1:2">
       <c r="A20" t="s">
-        <v>212</v>
+        <v>202</v>
       </c>
       <c r="B20" t="str">
         <f t="shared" si="0"/>
@@ -3868,7 +3853,7 @@
     </row>
     <row r="21" spans="1:2">
       <c r="A21" t="s">
-        <v>213</v>
+        <v>203</v>
       </c>
       <c r="B21" t="str">
         <f t="shared" si="0"/>
@@ -3877,7 +3862,7 @@
     </row>
     <row r="22" spans="1:2">
       <c r="A22" t="s">
-        <v>214</v>
+        <v>204</v>
       </c>
       <c r="B22" t="str">
         <f t="shared" si="0"/>
@@ -3886,7 +3871,7 @@
     </row>
     <row r="23" spans="1:2">
       <c r="A23" t="s">
-        <v>215</v>
+        <v>205</v>
       </c>
       <c r="B23" t="str">
         <f t="shared" si="0"/>
@@ -3895,7 +3880,7 @@
     </row>
     <row r="24" spans="1:2">
       <c r="A24" t="s">
-        <v>234</v>
+        <v>224</v>
       </c>
       <c r="B24" t="str">
         <f t="shared" si="0"/>
@@ -3904,7 +3889,7 @@
     </row>
     <row r="25" spans="1:2">
       <c r="A25" t="s">
-        <v>235</v>
+        <v>225</v>
       </c>
       <c r="B25" t="str">
         <f t="shared" si="0"/>
@@ -3913,7 +3898,7 @@
     </row>
     <row r="26" spans="1:2">
       <c r="A26" t="s">
-        <v>226</v>
+        <v>216</v>
       </c>
       <c r="B26" t="str">
         <f t="shared" si="0"/>
@@ -3922,7 +3907,7 @@
     </row>
     <row r="27" spans="1:2">
       <c r="A27" t="s">
-        <v>236</v>
+        <v>226</v>
       </c>
       <c r="B27" t="str">
         <f t="shared" si="0"/>
@@ -3931,7 +3916,7 @@
     </row>
     <row r="28" spans="1:2">
       <c r="A28" t="s">
-        <v>216</v>
+        <v>206</v>
       </c>
       <c r="B28" t="str">
         <f t="shared" si="0"/>
@@ -3940,7 +3925,7 @@
     </row>
     <row r="29" spans="1:2">
       <c r="A29" t="s">
-        <v>217</v>
+        <v>207</v>
       </c>
       <c r="B29" t="str">
         <f t="shared" si="0"/>
@@ -3949,7 +3934,7 @@
     </row>
     <row r="30" spans="1:2">
       <c r="A30" t="s">
-        <v>218</v>
+        <v>208</v>
       </c>
       <c r="B30" t="str">
         <f t="shared" si="0"/>
@@ -3958,7 +3943,7 @@
     </row>
     <row r="31" spans="1:2">
       <c r="A31" t="s">
-        <v>219</v>
+        <v>209</v>
       </c>
       <c r="B31" t="str">
         <f t="shared" si="0"/>
@@ -3967,7 +3952,7 @@
     </row>
     <row r="32" spans="1:2">
       <c r="A32" t="s">
-        <v>220</v>
+        <v>210</v>
       </c>
       <c r="B32" t="str">
         <f t="shared" si="0"/>
@@ -3976,7 +3961,7 @@
     </row>
     <row r="33" spans="1:2">
       <c r="A33" t="s">
-        <v>221</v>
+        <v>211</v>
       </c>
       <c r="B33" t="str">
         <f t="shared" si="0"/>
@@ -3985,7 +3970,7 @@
     </row>
     <row r="34" spans="1:2">
       <c r="A34" t="s">
-        <v>222</v>
+        <v>212</v>
       </c>
       <c r="B34" t="str">
         <f t="shared" si="0"/>
@@ -3994,7 +3979,7 @@
     </row>
     <row r="35" spans="1:2">
       <c r="A35" t="s">
-        <v>223</v>
+        <v>213</v>
       </c>
       <c r="B35" t="str">
         <f t="shared" si="0"/>
@@ -4026,18 +4011,18 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B2" t="s">
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -4064,48 +4049,48 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" t="s">
-        <v>179</v>
+        <v>170</v>
       </c>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" t="s">
+        <v>54</v>
+      </c>
+      <c r="B2" t="s">
+        <v>55</v>
+      </c>
+      <c r="C2" t="s">
         <v>56</v>
-      </c>
-      <c r="B2" t="s">
-        <v>57</v>
-      </c>
-      <c r="C2" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" t="s">
-        <v>171</v>
+        <v>162</v>
       </c>
       <c r="B3" t="s">
-        <v>168</v>
+        <v>159</v>
       </c>
       <c r="C3" t="s">
-        <v>169</v>
+        <v>160</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" t="s">
-        <v>171</v>
+        <v>162</v>
       </c>
       <c r="B4" t="s">
-        <v>167</v>
+        <v>158</v>
       </c>
       <c r="C4" t="s">
-        <v>170</v>
+        <v>161</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" t="s">
-        <v>172</v>
+        <v>163</v>
       </c>
       <c r="B5" t="s">
-        <v>173</v>
+        <v>164</v>
       </c>
       <c r="C5" t="str">
         <f>LEFT(B5,2)</f>
@@ -4114,10 +4099,10 @@
     </row>
     <row r="6" spans="1:3">
       <c r="A6" t="s">
-        <v>172</v>
+        <v>163</v>
       </c>
       <c r="B6" t="s">
-        <v>174</v>
+        <v>165</v>
       </c>
       <c r="C6" t="str">
         <f t="shared" ref="C6:C10" si="0">LEFT(B6,2)</f>
@@ -4126,10 +4111,10 @@
     </row>
     <row r="7" spans="1:3">
       <c r="A7" t="s">
-        <v>172</v>
+        <v>163</v>
       </c>
       <c r="B7" t="s">
-        <v>175</v>
+        <v>166</v>
       </c>
       <c r="C7" t="str">
         <f t="shared" si="0"/>
@@ -4138,10 +4123,10 @@
     </row>
     <row r="8" spans="1:3">
       <c r="A8" t="s">
-        <v>172</v>
+        <v>163</v>
       </c>
       <c r="B8" t="s">
-        <v>176</v>
+        <v>167</v>
       </c>
       <c r="C8" t="str">
         <f t="shared" si="0"/>
@@ -4150,10 +4135,10 @@
     </row>
     <row r="9" spans="1:3">
       <c r="A9" t="s">
-        <v>172</v>
+        <v>163</v>
       </c>
       <c r="B9" t="s">
-        <v>177</v>
+        <v>168</v>
       </c>
       <c r="C9" t="str">
         <f t="shared" si="0"/>
@@ -4162,10 +4147,10 @@
     </row>
     <row r="10" spans="1:3">
       <c r="A10" t="s">
-        <v>172</v>
+        <v>163</v>
       </c>
       <c r="B10" t="s">
-        <v>178</v>
+        <v>169</v>
       </c>
       <c r="C10" t="str">
         <f t="shared" si="0"/>
@@ -4179,10 +4164,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{10ADB714-E6AA-4E3E-B77B-62B65BA0E218}">
-  <dimension ref="A1:G30"/>
+  <dimension ref="A1:G56"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D29" sqref="D29"/>
+      <selection activeCell="D38" sqref="D38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -4197,368 +4182,681 @@
   <sheetData>
     <row r="1" spans="1:7" ht="17.25" thickBot="1">
       <c r="A1" s="5" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="15" thickTop="1" thickBot="1">
       <c r="A2" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="C2" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="B2" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="C2" s="6" t="s">
-        <v>58</v>
-      </c>
       <c r="D2" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="F2" s="6" t="s">
         <v>68</v>
       </c>
-      <c r="E2" s="6" t="s">
+      <c r="G2" s="6" t="s">
         <v>69</v>
-      </c>
-      <c r="F2" s="6" t="s">
-        <v>70</v>
-      </c>
-      <c r="G2" s="6" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="3" spans="1:7">
       <c r="A3" t="s">
-        <v>72</v>
-      </c>
-      <c r="C3" t="str">
-        <f>D3</f>
-        <v>CCGT</v>
-      </c>
-      <c r="D3" t="s">
-        <v>90</v>
+        <v>120</v>
+      </c>
+      <c r="B3" t="s">
+        <v>121</v>
+      </c>
+      <c r="C3" t="s">
+        <v>122</v>
       </c>
     </row>
     <row r="4" spans="1:7">
       <c r="A4" t="s">
-        <v>72</v>
-      </c>
-      <c r="C4" t="str">
-        <f t="shared" ref="C4:C20" si="0">D4</f>
-        <v>Int Comb</v>
-      </c>
-      <c r="D4" t="s">
-        <v>91</v>
+        <v>120</v>
+      </c>
+      <c r="B4" t="s">
+        <v>123</v>
+      </c>
+      <c r="C4" t="s">
+        <v>124</v>
       </c>
     </row>
     <row r="5" spans="1:7">
       <c r="A5" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C5" t="str">
-        <f t="shared" si="0"/>
-        <v>Gas_Oil Steam</v>
+        <f>D5</f>
+        <v>CCGT</v>
       </c>
       <c r="D5" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
     </row>
     <row r="6" spans="1:7">
       <c r="A6" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C6" t="str">
-        <f t="shared" si="0"/>
-        <v>Nuclear</v>
+        <f t="shared" ref="C6:C49" si="0">D6</f>
+        <v>Int Comb</v>
       </c>
       <c r="D6" t="s">
-        <v>4</v>
+        <v>89</v>
       </c>
     </row>
     <row r="7" spans="1:7">
       <c r="A7" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C7" t="str">
         <f t="shared" si="0"/>
-        <v>OCGT (Peaker)</v>
+        <v>Gas_Oil Steam</v>
       </c>
       <c r="D7" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
     </row>
     <row r="8" spans="1:7">
       <c r="A8" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C8" t="str">
         <f t="shared" si="0"/>
-        <v>Subcritical Coal</v>
+        <v>OCGT (Peaker)</v>
       </c>
       <c r="D8" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
     </row>
     <row r="9" spans="1:7">
       <c r="A9" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C9" t="str">
         <f t="shared" si="0"/>
-        <v>Supercritical Coal</v>
+        <v>Subcritical Coal</v>
       </c>
       <c r="D9" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
     </row>
     <row r="10" spans="1:7">
       <c r="A10" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C10" t="str">
         <f t="shared" si="0"/>
-        <v>IGCC</v>
+        <v>Supercritical Coal</v>
       </c>
       <c r="D10" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
     </row>
     <row r="11" spans="1:7">
       <c r="A11" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C11" t="str">
         <f t="shared" si="0"/>
-        <v>Bioenergy</v>
+        <v>IGCC</v>
       </c>
       <c r="D11" t="s">
-        <v>101</v>
+        <v>94</v>
       </c>
     </row>
     <row r="12" spans="1:7">
       <c r="A12" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C12" t="str">
         <f t="shared" si="0"/>
-        <v>Solar</v>
+        <v>Bio Power</v>
       </c>
       <c r="D12" t="s">
-        <v>5</v>
+        <v>217</v>
       </c>
     </row>
     <row r="13" spans="1:7">
       <c r="A13" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C13" t="str">
         <f t="shared" si="0"/>
-        <v>Wind onshore</v>
+        <v>Solar Util</v>
       </c>
       <c r="D13" t="s">
-        <v>97</v>
+        <v>218</v>
       </c>
     </row>
     <row r="14" spans="1:7">
       <c r="A14" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C14" t="str">
         <f t="shared" si="0"/>
-        <v>Wind offshore</v>
+        <v>Wind onshore</v>
       </c>
       <c r="D14" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
     </row>
     <row r="15" spans="1:7">
       <c r="A15" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C15" t="str">
         <f t="shared" si="0"/>
-        <v>Geothermal</v>
+        <v>Wind offshore</v>
       </c>
       <c r="D15" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
     </row>
     <row r="16" spans="1:7">
       <c r="A16" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C16" t="str">
         <f t="shared" si="0"/>
-        <v>Hydro</v>
+        <v>Geothermal P</v>
       </c>
       <c r="D16" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4">
+      <c r="A17" t="s">
+        <v>70</v>
+      </c>
+      <c r="C17" t="str">
+        <f t="shared" si="0"/>
+        <v>Hydro Dam</v>
+      </c>
+      <c r="D17" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4">
+      <c r="A18" t="s">
+        <v>70</v>
+      </c>
+      <c r="C18" t="str">
+        <f t="shared" si="0"/>
+        <v>Hydro RoR</v>
+      </c>
+      <c r="D18" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4">
+      <c r="A19" t="s">
+        <v>70</v>
+      </c>
+      <c r="C19" t="str">
+        <f t="shared" si="0"/>
+        <v>Nuclear P</v>
+      </c>
+      <c r="D19" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4">
+      <c r="A20" t="s">
+        <v>70</v>
+      </c>
+      <c r="C20" t="str">
+        <f t="shared" si="0"/>
+        <v>Nuclear SMR</v>
+      </c>
+      <c r="D20" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4">
+      <c r="A21" t="s">
+        <v>70</v>
+      </c>
+      <c r="C21" t="str">
+        <f t="shared" si="0"/>
+        <v>Hydro pumped stg</v>
+      </c>
+      <c r="D21" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4">
+      <c r="A22" t="s">
+        <v>70</v>
+      </c>
+      <c r="C22" t="str">
+        <f t="shared" si="0"/>
+        <v>Util Batt Stg</v>
+      </c>
+      <c r="D22" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4">
+      <c r="A23" t="s">
+        <v>70</v>
+      </c>
+      <c r="C23" t="str">
+        <f t="shared" si="0"/>
+        <v>EV Batt</v>
+      </c>
+      <c r="D23" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4">
+      <c r="A24" t="s">
+        <v>70</v>
+      </c>
+      <c r="C24" t="str">
+        <f t="shared" si="0"/>
+        <v>Demand</v>
+      </c>
+      <c r="D24" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4">
+      <c r="A25" t="s">
+        <v>70</v>
+      </c>
+      <c r="C25" t="str">
+        <f t="shared" si="0"/>
+        <v>Transformers Dn</v>
+      </c>
+      <c r="D25" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4">
+      <c r="A26" t="s">
+        <v>70</v>
+      </c>
+      <c r="C26" t="str">
+        <f t="shared" si="0"/>
+        <v>Transformers Up</v>
+      </c>
+      <c r="D26" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4">
+      <c r="A27" t="s">
+        <v>70</v>
+      </c>
+      <c r="C27" t="str">
+        <f t="shared" si="0"/>
+        <v>Grid-220V</v>
+      </c>
+      <c r="D27" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4">
+      <c r="A28" t="s">
+        <v>70</v>
+      </c>
+      <c r="C28" t="str">
+        <f t="shared" si="0"/>
+        <v>Grid-400V</v>
+      </c>
+      <c r="D28" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4">
+      <c r="A29" t="s">
+        <v>70</v>
+      </c>
+      <c r="C29" t="str">
+        <f t="shared" si="0"/>
+        <v>Grid-380V</v>
+      </c>
+      <c r="D29" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4">
+      <c r="A30" t="s">
+        <v>70</v>
+      </c>
+      <c r="C30" t="str">
+        <f t="shared" si="0"/>
+        <v>Grid-225V</v>
+      </c>
+      <c r="D30" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4">
+      <c r="A31" t="s">
+        <v>70</v>
+      </c>
+      <c r="C31" t="str">
+        <f t="shared" si="0"/>
+        <v>Grid-330V</v>
+      </c>
+      <c r="D31" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4">
+      <c r="A32" t="s">
+        <v>70</v>
+      </c>
+      <c r="C32" t="str">
+        <f t="shared" si="0"/>
+        <v>Grid-275V</v>
+      </c>
+      <c r="D32" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4">
+      <c r="A33" t="s">
+        <v>70</v>
+      </c>
+      <c r="C33" t="str">
+        <f t="shared" si="0"/>
+        <v>Grid-420V</v>
+      </c>
+      <c r="D33" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4">
+      <c r="A34" t="s">
+        <v>70</v>
+      </c>
+      <c r="C34" t="str">
+        <f t="shared" si="0"/>
+        <v>Grid-300V</v>
+      </c>
+      <c r="D34" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4">
+      <c r="A35" t="s">
+        <v>70</v>
+      </c>
+      <c r="C35" t="str">
+        <f t="shared" si="0"/>
+        <v>Grid-500V</v>
+      </c>
+      <c r="D35" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4">
+      <c r="A36" t="s">
+        <v>70</v>
+      </c>
+      <c r="C36" t="str">
+        <f t="shared" si="0"/>
+        <v>Grid-750V</v>
+      </c>
+      <c r="D36" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4">
+      <c r="A37" t="s">
+        <v>70</v>
+      </c>
+      <c r="C37" t="str">
+        <f t="shared" si="0"/>
+        <v>Grid-450V</v>
+      </c>
+      <c r="D37" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4">
+      <c r="A38" t="s">
+        <v>70</v>
+      </c>
+      <c r="C38" t="str">
+        <f t="shared" si="0"/>
+        <v>Grid-515V</v>
+      </c>
+      <c r="D38" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4">
+      <c r="A39" t="s">
+        <v>70</v>
+      </c>
+      <c r="C39" t="str">
+        <f t="shared" si="0"/>
+        <v>Grid-525V</v>
+      </c>
+      <c r="D39" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4">
+      <c r="A40" t="s">
+        <v>70</v>
+      </c>
+      <c r="C40" t="str">
+        <f t="shared" si="0"/>
+        <v>Grid-320V</v>
+      </c>
+      <c r="D40" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4">
+      <c r="A41" t="s">
+        <v>70</v>
+      </c>
+      <c r="C41" t="str">
+        <f t="shared" si="0"/>
+        <v>Grid-150V</v>
+      </c>
+      <c r="D41" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4">
+      <c r="A42" t="s">
+        <v>70</v>
+      </c>
+      <c r="C42" t="str">
+        <f t="shared" si="0"/>
+        <v>Grid-270V</v>
+      </c>
+      <c r="D42" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4">
+      <c r="A43" t="s">
+        <v>70</v>
+      </c>
+      <c r="C43" t="str">
+        <f t="shared" si="0"/>
+        <v>Grid-350V</v>
+      </c>
+      <c r="D43" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4">
+      <c r="A44" t="s">
+        <v>70</v>
+      </c>
+      <c r="C44" t="str">
+        <f t="shared" si="0"/>
+        <v>Grid-250V</v>
+      </c>
+      <c r="D44" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4">
+      <c r="A45" t="s">
+        <v>70</v>
+      </c>
+      <c r="C45" t="str">
+        <f t="shared" si="0"/>
+        <v>Grid-200V</v>
+      </c>
+      <c r="D45" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4">
+      <c r="A46" t="s">
+        <v>70</v>
+      </c>
+      <c r="C46" t="str">
+        <f t="shared" si="0"/>
+        <v>Grid-236V</v>
+      </c>
+      <c r="D46" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4">
+      <c r="A47" t="s">
+        <v>70</v>
+      </c>
+      <c r="C47" t="str">
+        <f t="shared" si="0"/>
+        <v>Grid-600V</v>
+      </c>
+      <c r="D47" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4">
+      <c r="A48" t="s">
+        <v>70</v>
+      </c>
+      <c r="C48" t="str">
+        <f t="shared" si="0"/>
+        <v>Aggregators</v>
+      </c>
+      <c r="D48" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6">
+      <c r="A49" t="s">
+        <v>70</v>
+      </c>
+      <c r="C49" t="str">
+        <f t="shared" si="0"/>
+        <v>DUMMY_IMP</v>
+      </c>
+      <c r="D49" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6">
+      <c r="A50" t="s">
+        <v>70</v>
+      </c>
+      <c r="C50" t="s">
+        <v>145</v>
+      </c>
+      <c r="E50" t="s">
+        <v>149</v>
+      </c>
+      <c r="F50" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6">
+      <c r="A51" t="s">
+        <v>70</v>
+      </c>
+      <c r="C51" t="s">
+        <v>146</v>
+      </c>
+      <c r="E51" t="s">
+        <v>150</v>
+      </c>
+      <c r="F51" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6">
+      <c r="A52" t="s">
+        <v>70</v>
+      </c>
+      <c r="B52" t="s">
+        <v>152</v>
+      </c>
+      <c r="C52" t="s">
+        <v>147</v>
+      </c>
+      <c r="E52" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6">
+      <c r="A53" t="s">
+        <v>70</v>
+      </c>
+      <c r="B53" t="s">
+        <v>152</v>
+      </c>
+      <c r="C53" t="s">
+        <v>148</v>
+      </c>
+      <c r="E53" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6">
+      <c r="A54" t="s">
+        <v>70</v>
+      </c>
+      <c r="B54" t="s">
+        <v>101</v>
+      </c>
+      <c r="C54" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="17" spans="1:6">
-      <c r="A17" t="s">
-        <v>72</v>
-      </c>
-      <c r="C17" t="str">
-        <f t="shared" si="0"/>
-        <v>Nuclear</v>
-      </c>
-      <c r="D17" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6">
-      <c r="A18" t="s">
-        <v>72</v>
-      </c>
-      <c r="C18" t="str">
-        <f t="shared" si="0"/>
-        <v>Hydro pumped stg</v>
-      </c>
-      <c r="D18" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6">
-      <c r="A19" t="s">
-        <v>72</v>
-      </c>
-      <c r="C19" t="str">
-        <f t="shared" si="0"/>
-        <v>Util Batt Stg</v>
-      </c>
-      <c r="D19" t="s">
+    <row r="55" spans="1:6">
+      <c r="A55" t="s">
+        <v>70</v>
+      </c>
+      <c r="B55" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="20" spans="1:6">
-      <c r="A20" t="s">
-        <v>72</v>
-      </c>
-      <c r="C20" t="str">
-        <f t="shared" si="0"/>
-        <v>EV Batt</v>
-      </c>
-      <c r="D20" t="s">
+      <c r="C55" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="21" spans="1:6">
-      <c r="A21" t="s">
-        <v>72</v>
-      </c>
-      <c r="C21" t="s">
-        <v>154</v>
-      </c>
-      <c r="E21" t="s">
-        <v>158</v>
-      </c>
-      <c r="F21" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6">
-      <c r="A22" t="s">
-        <v>72</v>
-      </c>
-      <c r="C22" t="s">
-        <v>155</v>
-      </c>
-      <c r="E22" t="s">
-        <v>159</v>
-      </c>
-      <c r="F22" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6">
-      <c r="A23" t="s">
-        <v>72</v>
-      </c>
-      <c r="B23" t="s">
-        <v>161</v>
-      </c>
-      <c r="C23" t="s">
-        <v>156</v>
-      </c>
-      <c r="E23" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6">
-      <c r="A24" t="s">
-        <v>72</v>
-      </c>
-      <c r="B24" t="s">
-        <v>161</v>
-      </c>
-      <c r="C24" t="s">
-        <v>157</v>
-      </c>
-      <c r="E24" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6">
-      <c r="A25" t="s">
-        <v>72</v>
-      </c>
-      <c r="B25" t="s">
-        <v>105</v>
-      </c>
-      <c r="C25" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6">
-      <c r="A26" t="s">
-        <v>72</v>
-      </c>
-      <c r="B26" t="s">
-        <v>106</v>
-      </c>
-      <c r="C26" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6">
-      <c r="A27" t="s">
-        <v>72</v>
-      </c>
-      <c r="B27" t="s">
-        <v>118</v>
-      </c>
-      <c r="C27" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6">
-      <c r="A28" t="s">
-        <v>72</v>
-      </c>
-      <c r="C28" t="s">
-        <v>188</v>
-      </c>
-      <c r="D28" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6">
-      <c r="A29" t="s">
-        <v>124</v>
-      </c>
-      <c r="B29" t="s">
-        <v>125</v>
-      </c>
-      <c r="C29" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6">
-      <c r="A30" t="s">
-        <v>124</v>
-      </c>
-      <c r="B30" t="s">
-        <v>127</v>
-      </c>
-      <c r="C30" t="s">
-        <v>128</v>
+    <row r="56" spans="1:6">
+      <c r="A56" t="s">
+        <v>70</v>
+      </c>
+      <c r="B56" t="s">
+        <v>114</v>
+      </c>
+      <c r="C56" t="s">
+        <v>115</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated CHE_grids model - 2025-08-21 08:22
</commit_message>
<xml_diff>
--- a/VerveStacks_CHE_grids/ReportDefs_vervestacks.xlsx
+++ b/VerveStacks_CHE_grids/ReportDefs_vervestacks.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Veda\Veda\Veda_models\vervestacks_models\VerveStacks_CHE_grids\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{769DA10A-C315-4A0D-A006-99CE3B2B2C6D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{AAABF813-F1D5-4A75-BC18-904DA1F7EC76}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="17475" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -82,7 +82,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="966" uniqueCount="415">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1041" uniqueCount="440">
   <si>
     <t>Unit</t>
   </si>
@@ -840,9 +840,6 @@
     <t>Transformers Up</t>
   </si>
   <si>
-    <t>Actual Policies</t>
-  </si>
-  <si>
     <t>Declared NDCs</t>
   </si>
   <si>
@@ -855,6 +852,9 @@
     <t>Target Net Zero 2050</t>
   </si>
   <si>
+    <t>Current Policies</t>
+  </si>
+  <si>
     <t>grid_node</t>
   </si>
   <si>
@@ -1324,6 +1324,81 @@
   </si>
   <si>
     <t>p_w98648381</t>
+  </si>
+  <si>
+    <t>rez_CHE_0</t>
+  </si>
+  <si>
+    <t>rez_CHE_1</t>
+  </si>
+  <si>
+    <t>rez_CHE_10</t>
+  </si>
+  <si>
+    <t>rez_CHE_11</t>
+  </si>
+  <si>
+    <t>rez_CHE_12</t>
+  </si>
+  <si>
+    <t>rez_CHE_13</t>
+  </si>
+  <si>
+    <t>rez_CHE_14</t>
+  </si>
+  <si>
+    <t>rez_CHE_15</t>
+  </si>
+  <si>
+    <t>rez_CHE_17</t>
+  </si>
+  <si>
+    <t>rez_CHE_18</t>
+  </si>
+  <si>
+    <t>rez_CHE_19</t>
+  </si>
+  <si>
+    <t>rez_CHE_2</t>
+  </si>
+  <si>
+    <t>rez_CHE_20</t>
+  </si>
+  <si>
+    <t>rez_CHE_21</t>
+  </si>
+  <si>
+    <t>rez_CHE_22</t>
+  </si>
+  <si>
+    <t>rez_CHE_23</t>
+  </si>
+  <si>
+    <t>rez_CHE_24</t>
+  </si>
+  <si>
+    <t>rez_CHE_25</t>
+  </si>
+  <si>
+    <t>rez_CHE_3</t>
+  </si>
+  <si>
+    <t>rez_CHE_4</t>
+  </si>
+  <si>
+    <t>rez_CHE_5</t>
+  </si>
+  <si>
+    <t>rez_CHE_6</t>
+  </si>
+  <si>
+    <t>rez_CHE_7</t>
+  </si>
+  <si>
+    <t>rez_CHE_8</t>
+  </si>
+  <si>
+    <t>rez_CHE_9</t>
   </si>
   <si>
     <t>VERVESTACKS - the open USE platform · Powered by data · Shaped by vision · Guided by intuition · Fueled by passion</t>
@@ -1619,16 +1694,16 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="18"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="2" xfId="19"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="22" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="19" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="20" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="22" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="19" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="20">
     <cellStyle name="Date" xfId="1" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
@@ -1685,7 +1760,7 @@
         <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B8FF6A91-6B2A-8E2C-1C0E-3D50DB43DBA8}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{399F0054-4F6E-CDD2-7BC0-5DBED7F90602}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2006,12 +2081,10 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{316EBFFF-858A-4D21-973F-9D9013A436BB}">
-  <dimension ref="A1:H159"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{29821C0C-DEBE-47AB-9FC1-CCCC57555E16}">
+  <dimension ref="A1:H184"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
@@ -2020,1747 +2093,2022 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="22.05" customHeight="1">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="9" t="s">
+        <v>439</v>
+      </c>
+      <c r="B1" s="9"/>
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
+      <c r="E1" s="9"/>
+      <c r="F1" s="9"/>
+      <c r="G1" s="9"/>
+      <c r="H1" s="9"/>
+    </row>
+    <row r="2" spans="1:8" ht="14.65" thickBot="1">
+      <c r="B2" s="10" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="15.75" thickBot="1">
+      <c r="B3" s="11" t="s">
+        <v>54</v>
+      </c>
+      <c r="C3" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="D3" s="11" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
+      <c r="B4" s="12" t="s">
+        <v>257</v>
+      </c>
+      <c r="C4" s="12" t="s">
+        <v>258</v>
+      </c>
+      <c r="D4" s="12" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
+      <c r="B5" s="13" t="s">
+        <v>257</v>
+      </c>
+      <c r="C5" s="13" t="s">
+        <v>259</v>
+      </c>
+      <c r="D5" s="13" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
+      <c r="B6" s="12" t="s">
+        <v>257</v>
+      </c>
+      <c r="C6" s="12" t="s">
+        <v>260</v>
+      </c>
+      <c r="D6" s="12" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8">
+      <c r="B7" s="13" t="s">
+        <v>257</v>
+      </c>
+      <c r="C7" s="13" t="s">
+        <v>261</v>
+      </c>
+      <c r="D7" s="13" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8">
+      <c r="B8" s="12" t="s">
+        <v>257</v>
+      </c>
+      <c r="C8" s="12" t="s">
+        <v>262</v>
+      </c>
+      <c r="D8" s="12" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8">
+      <c r="B9" s="13" t="s">
+        <v>257</v>
+      </c>
+      <c r="C9" s="13" t="s">
+        <v>263</v>
+      </c>
+      <c r="D9" s="13" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8">
+      <c r="B10" s="12" t="s">
+        <v>257</v>
+      </c>
+      <c r="C10" s="12" t="s">
+        <v>264</v>
+      </c>
+      <c r="D10" s="12" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8">
+      <c r="B11" s="13" t="s">
+        <v>257</v>
+      </c>
+      <c r="C11" s="13" t="s">
+        <v>265</v>
+      </c>
+      <c r="D11" s="13" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8">
+      <c r="B12" s="12" t="s">
+        <v>257</v>
+      </c>
+      <c r="C12" s="12" t="s">
+        <v>266</v>
+      </c>
+      <c r="D12" s="12" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8">
+      <c r="B13" s="13" t="s">
+        <v>257</v>
+      </c>
+      <c r="C13" s="13" t="s">
+        <v>267</v>
+      </c>
+      <c r="D13" s="13" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8">
+      <c r="B14" s="12" t="s">
+        <v>257</v>
+      </c>
+      <c r="C14" s="12" t="s">
+        <v>268</v>
+      </c>
+      <c r="D14" s="12" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8">
+      <c r="B15" s="13" t="s">
+        <v>257</v>
+      </c>
+      <c r="C15" s="13" t="s">
+        <v>269</v>
+      </c>
+      <c r="D15" s="13" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8">
+      <c r="B16" s="12" t="s">
+        <v>257</v>
+      </c>
+      <c r="C16" s="12" t="s">
+        <v>270</v>
+      </c>
+      <c r="D16" s="12" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="17" spans="2:4">
+      <c r="B17" s="13" t="s">
+        <v>257</v>
+      </c>
+      <c r="C17" s="13" t="s">
+        <v>271</v>
+      </c>
+      <c r="D17" s="13" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="18" spans="2:4">
+      <c r="B18" s="12" t="s">
+        <v>257</v>
+      </c>
+      <c r="C18" s="12" t="s">
+        <v>272</v>
+      </c>
+      <c r="D18" s="12" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="19" spans="2:4">
+      <c r="B19" s="13" t="s">
+        <v>257</v>
+      </c>
+      <c r="C19" s="13" t="s">
+        <v>273</v>
+      </c>
+      <c r="D19" s="13" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="20" spans="2:4">
+      <c r="B20" s="12" t="s">
+        <v>257</v>
+      </c>
+      <c r="C20" s="12" t="s">
+        <v>274</v>
+      </c>
+      <c r="D20" s="12" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="21" spans="2:4">
+      <c r="B21" s="13" t="s">
+        <v>257</v>
+      </c>
+      <c r="C21" s="13" t="s">
+        <v>275</v>
+      </c>
+      <c r="D21" s="13" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="22" spans="2:4">
+      <c r="B22" s="12" t="s">
+        <v>257</v>
+      </c>
+      <c r="C22" s="12" t="s">
+        <v>276</v>
+      </c>
+      <c r="D22" s="12" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="23" spans="2:4">
+      <c r="B23" s="13" t="s">
+        <v>257</v>
+      </c>
+      <c r="C23" s="13" t="s">
+        <v>277</v>
+      </c>
+      <c r="D23" s="13" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="24" spans="2:4">
+      <c r="B24" s="12" t="s">
+        <v>257</v>
+      </c>
+      <c r="C24" s="12" t="s">
+        <v>278</v>
+      </c>
+      <c r="D24" s="12" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="25" spans="2:4">
+      <c r="B25" s="13" t="s">
+        <v>257</v>
+      </c>
+      <c r="C25" s="13" t="s">
+        <v>279</v>
+      </c>
+      <c r="D25" s="13" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="26" spans="2:4">
+      <c r="B26" s="12" t="s">
+        <v>257</v>
+      </c>
+      <c r="C26" s="12" t="s">
+        <v>280</v>
+      </c>
+      <c r="D26" s="12" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="27" spans="2:4">
+      <c r="B27" s="13" t="s">
+        <v>257</v>
+      </c>
+      <c r="C27" s="13" t="s">
+        <v>281</v>
+      </c>
+      <c r="D27" s="13" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="28" spans="2:4">
+      <c r="B28" s="12" t="s">
+        <v>257</v>
+      </c>
+      <c r="C28" s="12" t="s">
+        <v>282</v>
+      </c>
+      <c r="D28" s="12" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="29" spans="2:4">
+      <c r="B29" s="13" t="s">
+        <v>257</v>
+      </c>
+      <c r="C29" s="13" t="s">
+        <v>283</v>
+      </c>
+      <c r="D29" s="13" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="30" spans="2:4">
+      <c r="B30" s="12" t="s">
+        <v>257</v>
+      </c>
+      <c r="C30" s="12" t="s">
+        <v>284</v>
+      </c>
+      <c r="D30" s="12" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="31" spans="2:4">
+      <c r="B31" s="13" t="s">
+        <v>257</v>
+      </c>
+      <c r="C31" s="13" t="s">
+        <v>285</v>
+      </c>
+      <c r="D31" s="13" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="32" spans="2:4">
+      <c r="B32" s="12" t="s">
+        <v>257</v>
+      </c>
+      <c r="C32" s="12" t="s">
+        <v>286</v>
+      </c>
+      <c r="D32" s="12" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="33" spans="2:4">
+      <c r="B33" s="13" t="s">
+        <v>257</v>
+      </c>
+      <c r="C33" s="13" t="s">
+        <v>287</v>
+      </c>
+      <c r="D33" s="13" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="34" spans="2:4">
+      <c r="B34" s="12" t="s">
+        <v>257</v>
+      </c>
+      <c r="C34" s="12" t="s">
+        <v>288</v>
+      </c>
+      <c r="D34" s="12" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="35" spans="2:4">
+      <c r="B35" s="13" t="s">
+        <v>257</v>
+      </c>
+      <c r="C35" s="13" t="s">
+        <v>289</v>
+      </c>
+      <c r="D35" s="13" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="36" spans="2:4">
+      <c r="B36" s="12" t="s">
+        <v>257</v>
+      </c>
+      <c r="C36" s="12" t="s">
+        <v>290</v>
+      </c>
+      <c r="D36" s="12" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="37" spans="2:4">
+      <c r="B37" s="13" t="s">
+        <v>257</v>
+      </c>
+      <c r="C37" s="13" t="s">
+        <v>291</v>
+      </c>
+      <c r="D37" s="13" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="38" spans="2:4">
+      <c r="B38" s="12" t="s">
+        <v>257</v>
+      </c>
+      <c r="C38" s="12" t="s">
+        <v>292</v>
+      </c>
+      <c r="D38" s="12" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="39" spans="2:4">
+      <c r="B39" s="13" t="s">
+        <v>257</v>
+      </c>
+      <c r="C39" s="13" t="s">
+        <v>293</v>
+      </c>
+      <c r="D39" s="13" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="40" spans="2:4">
+      <c r="B40" s="12" t="s">
+        <v>257</v>
+      </c>
+      <c r="C40" s="12" t="s">
+        <v>294</v>
+      </c>
+      <c r="D40" s="12" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="41" spans="2:4">
+      <c r="B41" s="13" t="s">
+        <v>257</v>
+      </c>
+      <c r="C41" s="13" t="s">
+        <v>295</v>
+      </c>
+      <c r="D41" s="13" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="42" spans="2:4">
+      <c r="B42" s="12" t="s">
+        <v>257</v>
+      </c>
+      <c r="C42" s="12" t="s">
+        <v>296</v>
+      </c>
+      <c r="D42" s="12" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="43" spans="2:4">
+      <c r="B43" s="13" t="s">
+        <v>257</v>
+      </c>
+      <c r="C43" s="13" t="s">
+        <v>297</v>
+      </c>
+      <c r="D43" s="13" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="44" spans="2:4">
+      <c r="B44" s="12" t="s">
+        <v>257</v>
+      </c>
+      <c r="C44" s="12" t="s">
+        <v>298</v>
+      </c>
+      <c r="D44" s="12" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="45" spans="2:4">
+      <c r="B45" s="13" t="s">
+        <v>257</v>
+      </c>
+      <c r="C45" s="13" t="s">
+        <v>299</v>
+      </c>
+      <c r="D45" s="13" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="46" spans="2:4">
+      <c r="B46" s="12" t="s">
+        <v>257</v>
+      </c>
+      <c r="C46" s="12" t="s">
+        <v>300</v>
+      </c>
+      <c r="D46" s="12" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="47" spans="2:4">
+      <c r="B47" s="13" t="s">
+        <v>257</v>
+      </c>
+      <c r="C47" s="13" t="s">
+        <v>301</v>
+      </c>
+      <c r="D47" s="13" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="48" spans="2:4">
+      <c r="B48" s="12" t="s">
+        <v>257</v>
+      </c>
+      <c r="C48" s="12" t="s">
+        <v>302</v>
+      </c>
+      <c r="D48" s="12" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="49" spans="2:4">
+      <c r="B49" s="13" t="s">
+        <v>257</v>
+      </c>
+      <c r="C49" s="13" t="s">
+        <v>303</v>
+      </c>
+      <c r="D49" s="13" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="50" spans="2:4">
+      <c r="B50" s="12" t="s">
+        <v>257</v>
+      </c>
+      <c r="C50" s="12" t="s">
+        <v>304</v>
+      </c>
+      <c r="D50" s="12" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="51" spans="2:4">
+      <c r="B51" s="13" t="s">
+        <v>257</v>
+      </c>
+      <c r="C51" s="13" t="s">
+        <v>305</v>
+      </c>
+      <c r="D51" s="13" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="52" spans="2:4">
+      <c r="B52" s="12" t="s">
+        <v>257</v>
+      </c>
+      <c r="C52" s="12" t="s">
+        <v>306</v>
+      </c>
+      <c r="D52" s="12" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="53" spans="2:4">
+      <c r="B53" s="13" t="s">
+        <v>257</v>
+      </c>
+      <c r="C53" s="13" t="s">
+        <v>307</v>
+      </c>
+      <c r="D53" s="13" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="54" spans="2:4">
+      <c r="B54" s="12" t="s">
+        <v>257</v>
+      </c>
+      <c r="C54" s="12" t="s">
+        <v>308</v>
+      </c>
+      <c r="D54" s="12" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="55" spans="2:4">
+      <c r="B55" s="13" t="s">
+        <v>257</v>
+      </c>
+      <c r="C55" s="13" t="s">
+        <v>309</v>
+      </c>
+      <c r="D55" s="13" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="56" spans="2:4">
+      <c r="B56" s="12" t="s">
+        <v>257</v>
+      </c>
+      <c r="C56" s="12" t="s">
+        <v>310</v>
+      </c>
+      <c r="D56" s="12" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="57" spans="2:4">
+      <c r="B57" s="13" t="s">
+        <v>257</v>
+      </c>
+      <c r="C57" s="13" t="s">
+        <v>311</v>
+      </c>
+      <c r="D57" s="13" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="58" spans="2:4">
+      <c r="B58" s="12" t="s">
+        <v>257</v>
+      </c>
+      <c r="C58" s="12" t="s">
+        <v>312</v>
+      </c>
+      <c r="D58" s="12" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="59" spans="2:4">
+      <c r="B59" s="13" t="s">
+        <v>257</v>
+      </c>
+      <c r="C59" s="13" t="s">
+        <v>313</v>
+      </c>
+      <c r="D59" s="13" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="60" spans="2:4">
+      <c r="B60" s="12" t="s">
+        <v>257</v>
+      </c>
+      <c r="C60" s="12" t="s">
+        <v>314</v>
+      </c>
+      <c r="D60" s="12" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="61" spans="2:4">
+      <c r="B61" s="13" t="s">
+        <v>257</v>
+      </c>
+      <c r="C61" s="13" t="s">
+        <v>315</v>
+      </c>
+      <c r="D61" s="13" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="62" spans="2:4">
+      <c r="B62" s="12" t="s">
+        <v>257</v>
+      </c>
+      <c r="C62" s="12" t="s">
+        <v>316</v>
+      </c>
+      <c r="D62" s="12" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="63" spans="2:4">
+      <c r="B63" s="13" t="s">
+        <v>257</v>
+      </c>
+      <c r="C63" s="13" t="s">
+        <v>317</v>
+      </c>
+      <c r="D63" s="13" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="64" spans="2:4">
+      <c r="B64" s="12" t="s">
+        <v>257</v>
+      </c>
+      <c r="C64" s="12" t="s">
+        <v>318</v>
+      </c>
+      <c r="D64" s="12" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="65" spans="2:4">
+      <c r="B65" s="13" t="s">
+        <v>257</v>
+      </c>
+      <c r="C65" s="13" t="s">
+        <v>319</v>
+      </c>
+      <c r="D65" s="13" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="66" spans="2:4">
+      <c r="B66" s="12" t="s">
+        <v>257</v>
+      </c>
+      <c r="C66" s="12" t="s">
+        <v>320</v>
+      </c>
+      <c r="D66" s="12" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="67" spans="2:4">
+      <c r="B67" s="13" t="s">
+        <v>257</v>
+      </c>
+      <c r="C67" s="13" t="s">
+        <v>321</v>
+      </c>
+      <c r="D67" s="13" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="68" spans="2:4">
+      <c r="B68" s="12" t="s">
+        <v>257</v>
+      </c>
+      <c r="C68" s="12" t="s">
+        <v>322</v>
+      </c>
+      <c r="D68" s="12" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="69" spans="2:4">
+      <c r="B69" s="13" t="s">
+        <v>257</v>
+      </c>
+      <c r="C69" s="13" t="s">
+        <v>323</v>
+      </c>
+      <c r="D69" s="13" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="70" spans="2:4">
+      <c r="B70" s="12" t="s">
+        <v>257</v>
+      </c>
+      <c r="C70" s="12" t="s">
+        <v>324</v>
+      </c>
+      <c r="D70" s="12" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="71" spans="2:4">
+      <c r="B71" s="13" t="s">
+        <v>257</v>
+      </c>
+      <c r="C71" s="13" t="s">
+        <v>325</v>
+      </c>
+      <c r="D71" s="13" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="72" spans="2:4">
+      <c r="B72" s="12" t="s">
+        <v>257</v>
+      </c>
+      <c r="C72" s="12" t="s">
+        <v>326</v>
+      </c>
+      <c r="D72" s="12" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="73" spans="2:4">
+      <c r="B73" s="13" t="s">
+        <v>257</v>
+      </c>
+      <c r="C73" s="13" t="s">
+        <v>327</v>
+      </c>
+      <c r="D73" s="13" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="74" spans="2:4">
+      <c r="B74" s="12" t="s">
+        <v>257</v>
+      </c>
+      <c r="C74" s="12" t="s">
+        <v>328</v>
+      </c>
+      <c r="D74" s="12" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="75" spans="2:4">
+      <c r="B75" s="13" t="s">
+        <v>257</v>
+      </c>
+      <c r="C75" s="13" t="s">
+        <v>329</v>
+      </c>
+      <c r="D75" s="13" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="76" spans="2:4">
+      <c r="B76" s="12" t="s">
+        <v>257</v>
+      </c>
+      <c r="C76" s="12" t="s">
+        <v>330</v>
+      </c>
+      <c r="D76" s="12" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="77" spans="2:4">
+      <c r="B77" s="13" t="s">
+        <v>257</v>
+      </c>
+      <c r="C77" s="13" t="s">
+        <v>331</v>
+      </c>
+      <c r="D77" s="13" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="78" spans="2:4">
+      <c r="B78" s="12" t="s">
+        <v>257</v>
+      </c>
+      <c r="C78" s="12" t="s">
+        <v>332</v>
+      </c>
+      <c r="D78" s="12" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="79" spans="2:4">
+      <c r="B79" s="13" t="s">
+        <v>257</v>
+      </c>
+      <c r="C79" s="13" t="s">
+        <v>333</v>
+      </c>
+      <c r="D79" s="13" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="80" spans="2:4">
+      <c r="B80" s="12" t="s">
+        <v>257</v>
+      </c>
+      <c r="C80" s="12" t="s">
+        <v>334</v>
+      </c>
+      <c r="D80" s="12" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="81" spans="2:4">
+      <c r="B81" s="13" t="s">
+        <v>257</v>
+      </c>
+      <c r="C81" s="13" t="s">
+        <v>335</v>
+      </c>
+      <c r="D81" s="13" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="82" spans="2:4">
+      <c r="B82" s="12" t="s">
+        <v>257</v>
+      </c>
+      <c r="C82" s="12" t="s">
+        <v>336</v>
+      </c>
+      <c r="D82" s="12" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="83" spans="2:4">
+      <c r="B83" s="13" t="s">
+        <v>257</v>
+      </c>
+      <c r="C83" s="13" t="s">
+        <v>337</v>
+      </c>
+      <c r="D83" s="13" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="84" spans="2:4">
+      <c r="B84" s="12" t="s">
+        <v>257</v>
+      </c>
+      <c r="C84" s="12" t="s">
+        <v>338</v>
+      </c>
+      <c r="D84" s="12" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="85" spans="2:4">
+      <c r="B85" s="13" t="s">
+        <v>257</v>
+      </c>
+      <c r="C85" s="13" t="s">
+        <v>339</v>
+      </c>
+      <c r="D85" s="13" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="86" spans="2:4">
+      <c r="B86" s="12" t="s">
+        <v>257</v>
+      </c>
+      <c r="C86" s="12" t="s">
+        <v>340</v>
+      </c>
+      <c r="D86" s="12" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="87" spans="2:4">
+      <c r="B87" s="13" t="s">
+        <v>257</v>
+      </c>
+      <c r="C87" s="13" t="s">
+        <v>341</v>
+      </c>
+      <c r="D87" s="13" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="88" spans="2:4">
+      <c r="B88" s="12" t="s">
+        <v>257</v>
+      </c>
+      <c r="C88" s="12" t="s">
+        <v>342</v>
+      </c>
+      <c r="D88" s="12" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="89" spans="2:4">
+      <c r="B89" s="13" t="s">
+        <v>257</v>
+      </c>
+      <c r="C89" s="13" t="s">
+        <v>343</v>
+      </c>
+      <c r="D89" s="13" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="90" spans="2:4">
+      <c r="B90" s="12" t="s">
+        <v>257</v>
+      </c>
+      <c r="C90" s="12" t="s">
+        <v>344</v>
+      </c>
+      <c r="D90" s="12" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="91" spans="2:4">
+      <c r="B91" s="13" t="s">
+        <v>257</v>
+      </c>
+      <c r="C91" s="13" t="s">
+        <v>345</v>
+      </c>
+      <c r="D91" s="13" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="92" spans="2:4">
+      <c r="B92" s="12" t="s">
+        <v>257</v>
+      </c>
+      <c r="C92" s="12" t="s">
+        <v>346</v>
+      </c>
+      <c r="D92" s="12" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="93" spans="2:4">
+      <c r="B93" s="13" t="s">
+        <v>257</v>
+      </c>
+      <c r="C93" s="13" t="s">
+        <v>347</v>
+      </c>
+      <c r="D93" s="13" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="94" spans="2:4">
+      <c r="B94" s="12" t="s">
+        <v>257</v>
+      </c>
+      <c r="C94" s="12" t="s">
+        <v>348</v>
+      </c>
+      <c r="D94" s="12" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="95" spans="2:4">
+      <c r="B95" s="13" t="s">
+        <v>257</v>
+      </c>
+      <c r="C95" s="13" t="s">
+        <v>349</v>
+      </c>
+      <c r="D95" s="13" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="96" spans="2:4">
+      <c r="B96" s="12" t="s">
+        <v>257</v>
+      </c>
+      <c r="C96" s="12" t="s">
+        <v>350</v>
+      </c>
+      <c r="D96" s="12" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="97" spans="2:4">
+      <c r="B97" s="13" t="s">
+        <v>257</v>
+      </c>
+      <c r="C97" s="13" t="s">
+        <v>351</v>
+      </c>
+      <c r="D97" s="13" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="98" spans="2:4">
+      <c r="B98" s="12" t="s">
+        <v>257</v>
+      </c>
+      <c r="C98" s="12" t="s">
+        <v>352</v>
+      </c>
+      <c r="D98" s="12" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="99" spans="2:4">
+      <c r="B99" s="13" t="s">
+        <v>257</v>
+      </c>
+      <c r="C99" s="13" t="s">
+        <v>353</v>
+      </c>
+      <c r="D99" s="13" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="100" spans="2:4">
+      <c r="B100" s="12" t="s">
+        <v>257</v>
+      </c>
+      <c r="C100" s="12" t="s">
+        <v>354</v>
+      </c>
+      <c r="D100" s="12" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="101" spans="2:4">
+      <c r="B101" s="13" t="s">
+        <v>257</v>
+      </c>
+      <c r="C101" s="13" t="s">
+        <v>355</v>
+      </c>
+      <c r="D101" s="13" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="102" spans="2:4">
+      <c r="B102" s="12" t="s">
+        <v>257</v>
+      </c>
+      <c r="C102" s="12" t="s">
+        <v>356</v>
+      </c>
+      <c r="D102" s="12" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="103" spans="2:4">
+      <c r="B103" s="13" t="s">
+        <v>257</v>
+      </c>
+      <c r="C103" s="13" t="s">
+        <v>357</v>
+      </c>
+      <c r="D103" s="13" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="104" spans="2:4">
+      <c r="B104" s="12" t="s">
+        <v>257</v>
+      </c>
+      <c r="C104" s="12" t="s">
+        <v>358</v>
+      </c>
+      <c r="D104" s="12" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="105" spans="2:4">
+      <c r="B105" s="13" t="s">
+        <v>257</v>
+      </c>
+      <c r="C105" s="13" t="s">
+        <v>359</v>
+      </c>
+      <c r="D105" s="13" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="106" spans="2:4">
+      <c r="B106" s="12" t="s">
+        <v>257</v>
+      </c>
+      <c r="C106" s="12" t="s">
+        <v>360</v>
+      </c>
+      <c r="D106" s="12" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="107" spans="2:4">
+      <c r="B107" s="13" t="s">
+        <v>257</v>
+      </c>
+      <c r="C107" s="13" t="s">
+        <v>361</v>
+      </c>
+      <c r="D107" s="13" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="108" spans="2:4">
+      <c r="B108" s="12" t="s">
+        <v>257</v>
+      </c>
+      <c r="C108" s="12" t="s">
+        <v>362</v>
+      </c>
+      <c r="D108" s="12" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="109" spans="2:4">
+      <c r="B109" s="13" t="s">
+        <v>257</v>
+      </c>
+      <c r="C109" s="13" t="s">
+        <v>363</v>
+      </c>
+      <c r="D109" s="13" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="110" spans="2:4">
+      <c r="B110" s="12" t="s">
+        <v>257</v>
+      </c>
+      <c r="C110" s="12" t="s">
+        <v>364</v>
+      </c>
+      <c r="D110" s="12" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="111" spans="2:4">
+      <c r="B111" s="13" t="s">
+        <v>257</v>
+      </c>
+      <c r="C111" s="13" t="s">
+        <v>365</v>
+      </c>
+      <c r="D111" s="13" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="112" spans="2:4">
+      <c r="B112" s="12" t="s">
+        <v>257</v>
+      </c>
+      <c r="C112" s="12" t="s">
+        <v>366</v>
+      </c>
+      <c r="D112" s="12" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="113" spans="2:4">
+      <c r="B113" s="13" t="s">
+        <v>257</v>
+      </c>
+      <c r="C113" s="13" t="s">
+        <v>367</v>
+      </c>
+      <c r="D113" s="13" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="114" spans="2:4">
+      <c r="B114" s="12" t="s">
+        <v>257</v>
+      </c>
+      <c r="C114" s="12" t="s">
+        <v>368</v>
+      </c>
+      <c r="D114" s="12" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="115" spans="2:4">
+      <c r="B115" s="13" t="s">
+        <v>257</v>
+      </c>
+      <c r="C115" s="13" t="s">
+        <v>369</v>
+      </c>
+      <c r="D115" s="13" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="116" spans="2:4">
+      <c r="B116" s="12" t="s">
+        <v>257</v>
+      </c>
+      <c r="C116" s="12" t="s">
+        <v>370</v>
+      </c>
+      <c r="D116" s="12" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="117" spans="2:4">
+      <c r="B117" s="13" t="s">
+        <v>257</v>
+      </c>
+      <c r="C117" s="13" t="s">
+        <v>371</v>
+      </c>
+      <c r="D117" s="13" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="118" spans="2:4">
+      <c r="B118" s="12" t="s">
+        <v>257</v>
+      </c>
+      <c r="C118" s="12" t="s">
+        <v>372</v>
+      </c>
+      <c r="D118" s="12" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="119" spans="2:4">
+      <c r="B119" s="13" t="s">
+        <v>257</v>
+      </c>
+      <c r="C119" s="13" t="s">
+        <v>373</v>
+      </c>
+      <c r="D119" s="13" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="120" spans="2:4">
+      <c r="B120" s="12" t="s">
+        <v>257</v>
+      </c>
+      <c r="C120" s="12" t="s">
+        <v>374</v>
+      </c>
+      <c r="D120" s="12" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="121" spans="2:4">
+      <c r="B121" s="13" t="s">
+        <v>257</v>
+      </c>
+      <c r="C121" s="13" t="s">
+        <v>375</v>
+      </c>
+      <c r="D121" s="13" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="122" spans="2:4">
+      <c r="B122" s="12" t="s">
+        <v>257</v>
+      </c>
+      <c r="C122" s="12" t="s">
+        <v>376</v>
+      </c>
+      <c r="D122" s="12" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="123" spans="2:4">
+      <c r="B123" s="13" t="s">
+        <v>257</v>
+      </c>
+      <c r="C123" s="13" t="s">
+        <v>377</v>
+      </c>
+      <c r="D123" s="13" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="124" spans="2:4">
+      <c r="B124" s="12" t="s">
+        <v>257</v>
+      </c>
+      <c r="C124" s="12" t="s">
+        <v>378</v>
+      </c>
+      <c r="D124" s="12" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="125" spans="2:4">
+      <c r="B125" s="13" t="s">
+        <v>257</v>
+      </c>
+      <c r="C125" s="13" t="s">
+        <v>379</v>
+      </c>
+      <c r="D125" s="13" t="s">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="126" spans="2:4">
+      <c r="B126" s="12" t="s">
+        <v>257</v>
+      </c>
+      <c r="C126" s="12" t="s">
+        <v>380</v>
+      </c>
+      <c r="D126" s="12" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="127" spans="2:4">
+      <c r="B127" s="13" t="s">
+        <v>257</v>
+      </c>
+      <c r="C127" s="13" t="s">
+        <v>381</v>
+      </c>
+      <c r="D127" s="13" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="128" spans="2:4">
+      <c r="B128" s="12" t="s">
+        <v>257</v>
+      </c>
+      <c r="C128" s="12" t="s">
+        <v>382</v>
+      </c>
+      <c r="D128" s="12" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="129" spans="2:4">
+      <c r="B129" s="13" t="s">
+        <v>257</v>
+      </c>
+      <c r="C129" s="13" t="s">
+        <v>383</v>
+      </c>
+      <c r="D129" s="13" t="s">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="130" spans="2:4">
+      <c r="B130" s="12" t="s">
+        <v>257</v>
+      </c>
+      <c r="C130" s="12" t="s">
+        <v>384</v>
+      </c>
+      <c r="D130" s="12" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="131" spans="2:4">
+      <c r="B131" s="13" t="s">
+        <v>257</v>
+      </c>
+      <c r="C131" s="13" t="s">
+        <v>385</v>
+      </c>
+      <c r="D131" s="13" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="132" spans="2:4">
+      <c r="B132" s="12" t="s">
+        <v>257</v>
+      </c>
+      <c r="C132" s="12" t="s">
+        <v>386</v>
+      </c>
+      <c r="D132" s="12" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="133" spans="2:4">
+      <c r="B133" s="13" t="s">
+        <v>257</v>
+      </c>
+      <c r="C133" s="13" t="s">
+        <v>387</v>
+      </c>
+      <c r="D133" s="13" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="134" spans="2:4">
+      <c r="B134" s="12" t="s">
+        <v>257</v>
+      </c>
+      <c r="C134" s="12" t="s">
+        <v>388</v>
+      </c>
+      <c r="D134" s="12" t="s">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="135" spans="2:4">
+      <c r="B135" s="13" t="s">
+        <v>257</v>
+      </c>
+      <c r="C135" s="13" t="s">
+        <v>389</v>
+      </c>
+      <c r="D135" s="13" t="s">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="136" spans="2:4">
+      <c r="B136" s="12" t="s">
+        <v>257</v>
+      </c>
+      <c r="C136" s="12" t="s">
+        <v>390</v>
+      </c>
+      <c r="D136" s="12" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="137" spans="2:4">
+      <c r="B137" s="13" t="s">
+        <v>257</v>
+      </c>
+      <c r="C137" s="13" t="s">
+        <v>391</v>
+      </c>
+      <c r="D137" s="13" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="138" spans="2:4">
+      <c r="B138" s="12" t="s">
+        <v>257</v>
+      </c>
+      <c r="C138" s="12" t="s">
+        <v>392</v>
+      </c>
+      <c r="D138" s="12" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="139" spans="2:4">
+      <c r="B139" s="13" t="s">
+        <v>257</v>
+      </c>
+      <c r="C139" s="13" t="s">
+        <v>393</v>
+      </c>
+      <c r="D139" s="13" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="140" spans="2:4">
+      <c r="B140" s="12" t="s">
+        <v>257</v>
+      </c>
+      <c r="C140" s="12" t="s">
+        <v>394</v>
+      </c>
+      <c r="D140" s="12" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="141" spans="2:4">
+      <c r="B141" s="13" t="s">
+        <v>257</v>
+      </c>
+      <c r="C141" s="13" t="s">
+        <v>395</v>
+      </c>
+      <c r="D141" s="13" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="142" spans="2:4">
+      <c r="B142" s="12" t="s">
+        <v>257</v>
+      </c>
+      <c r="C142" s="12" t="s">
+        <v>396</v>
+      </c>
+      <c r="D142" s="12" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="143" spans="2:4">
+      <c r="B143" s="13" t="s">
+        <v>257</v>
+      </c>
+      <c r="C143" s="13" t="s">
+        <v>397</v>
+      </c>
+      <c r="D143" s="13" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="144" spans="2:4">
+      <c r="B144" s="12" t="s">
+        <v>257</v>
+      </c>
+      <c r="C144" s="12" t="s">
+        <v>398</v>
+      </c>
+      <c r="D144" s="12" t="s">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="145" spans="2:4">
+      <c r="B145" s="13" t="s">
+        <v>257</v>
+      </c>
+      <c r="C145" s="13" t="s">
+        <v>399</v>
+      </c>
+      <c r="D145" s="13" t="s">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="146" spans="2:4">
+      <c r="B146" s="12" t="s">
+        <v>257</v>
+      </c>
+      <c r="C146" s="12" t="s">
+        <v>400</v>
+      </c>
+      <c r="D146" s="12" t="s">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="147" spans="2:4">
+      <c r="B147" s="13" t="s">
+        <v>257</v>
+      </c>
+      <c r="C147" s="13" t="s">
+        <v>401</v>
+      </c>
+      <c r="D147" s="13" t="s">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="148" spans="2:4">
+      <c r="B148" s="12" t="s">
+        <v>257</v>
+      </c>
+      <c r="C148" s="12" t="s">
+        <v>402</v>
+      </c>
+      <c r="D148" s="12" t="s">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="149" spans="2:4">
+      <c r="B149" s="13" t="s">
+        <v>257</v>
+      </c>
+      <c r="C149" s="13" t="s">
+        <v>403</v>
+      </c>
+      <c r="D149" s="13" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="150" spans="2:4">
+      <c r="B150" s="12" t="s">
+        <v>257</v>
+      </c>
+      <c r="C150" s="12" t="s">
+        <v>404</v>
+      </c>
+      <c r="D150" s="12" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="151" spans="2:4">
+      <c r="B151" s="13" t="s">
+        <v>257</v>
+      </c>
+      <c r="C151" s="13" t="s">
+        <v>405</v>
+      </c>
+      <c r="D151" s="13" t="s">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="152" spans="2:4">
+      <c r="B152" s="12" t="s">
+        <v>257</v>
+      </c>
+      <c r="C152" s="12" t="s">
+        <v>406</v>
+      </c>
+      <c r="D152" s="12" t="s">
+        <v>406</v>
+      </c>
+    </row>
+    <row r="153" spans="2:4">
+      <c r="B153" s="13" t="s">
+        <v>257</v>
+      </c>
+      <c r="C153" s="13" t="s">
+        <v>407</v>
+      </c>
+      <c r="D153" s="13" t="s">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="154" spans="2:4">
+      <c r="B154" s="12" t="s">
+        <v>257</v>
+      </c>
+      <c r="C154" s="12" t="s">
+        <v>408</v>
+      </c>
+      <c r="D154" s="12" t="s">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="155" spans="2:4">
+      <c r="B155" s="13" t="s">
+        <v>257</v>
+      </c>
+      <c r="C155" s="13" t="s">
+        <v>409</v>
+      </c>
+      <c r="D155" s="13" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="156" spans="2:4">
+      <c r="B156" s="12" t="s">
+        <v>257</v>
+      </c>
+      <c r="C156" s="12" t="s">
+        <v>410</v>
+      </c>
+      <c r="D156" s="12" t="s">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="157" spans="2:4">
+      <c r="B157" s="13" t="s">
+        <v>257</v>
+      </c>
+      <c r="C157" s="13" t="s">
+        <v>411</v>
+      </c>
+      <c r="D157" s="13" t="s">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="158" spans="2:4">
+      <c r="B158" s="12" t="s">
+        <v>257</v>
+      </c>
+      <c r="C158" s="12" t="s">
+        <v>412</v>
+      </c>
+      <c r="D158" s="12" t="s">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="159" spans="2:4">
+      <c r="B159" s="13" t="s">
+        <v>257</v>
+      </c>
+      <c r="C159" s="13" t="s">
+        <v>413</v>
+      </c>
+      <c r="D159" s="13" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="160" spans="2:4">
+      <c r="B160" s="12" t="s">
+        <v>257</v>
+      </c>
+      <c r="C160" s="12" t="s">
         <v>414</v>
       </c>
-      <c r="B1" s="12"/>
-      <c r="C1" s="12"/>
-      <c r="D1" s="12"/>
-      <c r="E1" s="12"/>
-      <c r="F1" s="12"/>
-      <c r="G1" s="12"/>
-      <c r="H1" s="12"/>
-    </row>
-    <row r="2" spans="1:8" ht="14.65" thickBot="1">
-      <c r="B2" s="8" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" ht="15.75" thickBot="1">
-      <c r="B3" s="9" t="s">
-        <v>54</v>
-      </c>
-      <c r="C3" s="9" t="s">
-        <v>56</v>
-      </c>
-      <c r="D3" s="9" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8">
-      <c r="B4" s="10" t="s">
-        <v>257</v>
-      </c>
-      <c r="C4" s="10" t="s">
-        <v>258</v>
-      </c>
-      <c r="D4" s="10" t="s">
-        <v>258</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8">
-      <c r="B5" s="11" t="s">
-        <v>257</v>
-      </c>
-      <c r="C5" s="11" t="s">
-        <v>259</v>
-      </c>
-      <c r="D5" s="11" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8">
-      <c r="B6" s="10" t="s">
-        <v>257</v>
-      </c>
-      <c r="C6" s="10" t="s">
-        <v>260</v>
-      </c>
-      <c r="D6" s="10" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8">
-      <c r="B7" s="11" t="s">
-        <v>257</v>
-      </c>
-      <c r="C7" s="11" t="s">
-        <v>261</v>
-      </c>
-      <c r="D7" s="11" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8">
-      <c r="B8" s="10" t="s">
-        <v>257</v>
-      </c>
-      <c r="C8" s="10" t="s">
-        <v>262</v>
-      </c>
-      <c r="D8" s="10" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8">
-      <c r="B9" s="11" t="s">
-        <v>257</v>
-      </c>
-      <c r="C9" s="11" t="s">
-        <v>263</v>
-      </c>
-      <c r="D9" s="11" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8">
-      <c r="B10" s="10" t="s">
-        <v>257</v>
-      </c>
-      <c r="C10" s="10" t="s">
-        <v>264</v>
-      </c>
-      <c r="D10" s="10" t="s">
-        <v>264</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8">
-      <c r="B11" s="11" t="s">
-        <v>257</v>
-      </c>
-      <c r="C11" s="11" t="s">
-        <v>265</v>
-      </c>
-      <c r="D11" s="11" t="s">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8">
-      <c r="B12" s="10" t="s">
-        <v>257</v>
-      </c>
-      <c r="C12" s="10" t="s">
-        <v>266</v>
-      </c>
-      <c r="D12" s="10" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8">
-      <c r="B13" s="11" t="s">
-        <v>257</v>
-      </c>
-      <c r="C13" s="11" t="s">
-        <v>267</v>
-      </c>
-      <c r="D13" s="11" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8">
-      <c r="B14" s="10" t="s">
-        <v>257</v>
-      </c>
-      <c r="C14" s="10" t="s">
-        <v>268</v>
-      </c>
-      <c r="D14" s="10" t="s">
-        <v>268</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8">
-      <c r="B15" s="11" t="s">
-        <v>257</v>
-      </c>
-      <c r="C15" s="11" t="s">
-        <v>269</v>
-      </c>
-      <c r="D15" s="11" t="s">
-        <v>269</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8">
-      <c r="B16" s="10" t="s">
-        <v>257</v>
-      </c>
-      <c r="C16" s="10" t="s">
-        <v>270</v>
-      </c>
-      <c r="D16" s="10" t="s">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="17" spans="2:4">
-      <c r="B17" s="11" t="s">
-        <v>257</v>
-      </c>
-      <c r="C17" s="11" t="s">
-        <v>271</v>
-      </c>
-      <c r="D17" s="11" t="s">
-        <v>271</v>
-      </c>
-    </row>
-    <row r="18" spans="2:4">
-      <c r="B18" s="10" t="s">
-        <v>257</v>
-      </c>
-      <c r="C18" s="10" t="s">
-        <v>272</v>
-      </c>
-      <c r="D18" s="10" t="s">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="19" spans="2:4">
-      <c r="B19" s="11" t="s">
-        <v>257</v>
-      </c>
-      <c r="C19" s="11" t="s">
-        <v>273</v>
-      </c>
-      <c r="D19" s="11" t="s">
-        <v>273</v>
-      </c>
-    </row>
-    <row r="20" spans="2:4">
-      <c r="B20" s="10" t="s">
-        <v>257</v>
-      </c>
-      <c r="C20" s="10" t="s">
-        <v>274</v>
-      </c>
-      <c r="D20" s="10" t="s">
-        <v>274</v>
-      </c>
-    </row>
-    <row r="21" spans="2:4">
-      <c r="B21" s="11" t="s">
-        <v>257</v>
-      </c>
-      <c r="C21" s="11" t="s">
-        <v>275</v>
-      </c>
-      <c r="D21" s="11" t="s">
-        <v>275</v>
-      </c>
-    </row>
-    <row r="22" spans="2:4">
-      <c r="B22" s="10" t="s">
-        <v>257</v>
-      </c>
-      <c r="C22" s="10" t="s">
-        <v>276</v>
-      </c>
-      <c r="D22" s="10" t="s">
-        <v>276</v>
-      </c>
-    </row>
-    <row r="23" spans="2:4">
-      <c r="B23" s="11" t="s">
-        <v>257</v>
-      </c>
-      <c r="C23" s="11" t="s">
-        <v>277</v>
-      </c>
-      <c r="D23" s="11" t="s">
-        <v>277</v>
-      </c>
-    </row>
-    <row r="24" spans="2:4">
-      <c r="B24" s="10" t="s">
-        <v>257</v>
-      </c>
-      <c r="C24" s="10" t="s">
-        <v>278</v>
-      </c>
-      <c r="D24" s="10" t="s">
-        <v>278</v>
-      </c>
-    </row>
-    <row r="25" spans="2:4">
-      <c r="B25" s="11" t="s">
-        <v>257</v>
-      </c>
-      <c r="C25" s="11" t="s">
-        <v>279</v>
-      </c>
-      <c r="D25" s="11" t="s">
-        <v>279</v>
-      </c>
-    </row>
-    <row r="26" spans="2:4">
-      <c r="B26" s="10" t="s">
-        <v>257</v>
-      </c>
-      <c r="C26" s="10" t="s">
-        <v>280</v>
-      </c>
-      <c r="D26" s="10" t="s">
-        <v>280</v>
-      </c>
-    </row>
-    <row r="27" spans="2:4">
-      <c r="B27" s="11" t="s">
-        <v>257</v>
-      </c>
-      <c r="C27" s="11" t="s">
-        <v>281</v>
-      </c>
-      <c r="D27" s="11" t="s">
-        <v>281</v>
-      </c>
-    </row>
-    <row r="28" spans="2:4">
-      <c r="B28" s="10" t="s">
-        <v>257</v>
-      </c>
-      <c r="C28" s="10" t="s">
-        <v>282</v>
-      </c>
-      <c r="D28" s="10" t="s">
-        <v>282</v>
-      </c>
-    </row>
-    <row r="29" spans="2:4">
-      <c r="B29" s="11" t="s">
-        <v>257</v>
-      </c>
-      <c r="C29" s="11" t="s">
-        <v>283</v>
-      </c>
-      <c r="D29" s="11" t="s">
-        <v>283</v>
-      </c>
-    </row>
-    <row r="30" spans="2:4">
-      <c r="B30" s="10" t="s">
-        <v>257</v>
-      </c>
-      <c r="C30" s="10" t="s">
-        <v>284</v>
-      </c>
-      <c r="D30" s="10" t="s">
-        <v>284</v>
-      </c>
-    </row>
-    <row r="31" spans="2:4">
-      <c r="B31" s="11" t="s">
-        <v>257</v>
-      </c>
-      <c r="C31" s="11" t="s">
-        <v>285</v>
-      </c>
-      <c r="D31" s="11" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="32" spans="2:4">
-      <c r="B32" s="10" t="s">
-        <v>257</v>
-      </c>
-      <c r="C32" s="10" t="s">
-        <v>286</v>
-      </c>
-      <c r="D32" s="10" t="s">
-        <v>286</v>
-      </c>
-    </row>
-    <row r="33" spans="2:4">
-      <c r="B33" s="11" t="s">
-        <v>257</v>
-      </c>
-      <c r="C33" s="11" t="s">
-        <v>287</v>
-      </c>
-      <c r="D33" s="11" t="s">
-        <v>287</v>
-      </c>
-    </row>
-    <row r="34" spans="2:4">
-      <c r="B34" s="10" t="s">
-        <v>257</v>
-      </c>
-      <c r="C34" s="10" t="s">
-        <v>288</v>
-      </c>
-      <c r="D34" s="10" t="s">
-        <v>288</v>
-      </c>
-    </row>
-    <row r="35" spans="2:4">
-      <c r="B35" s="11" t="s">
-        <v>257</v>
-      </c>
-      <c r="C35" s="11" t="s">
-        <v>289</v>
-      </c>
-      <c r="D35" s="11" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="36" spans="2:4">
-      <c r="B36" s="10" t="s">
-        <v>257</v>
-      </c>
-      <c r="C36" s="10" t="s">
-        <v>290</v>
-      </c>
-      <c r="D36" s="10" t="s">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="37" spans="2:4">
-      <c r="B37" s="11" t="s">
-        <v>257</v>
-      </c>
-      <c r="C37" s="11" t="s">
-        <v>291</v>
-      </c>
-      <c r="D37" s="11" t="s">
-        <v>291</v>
-      </c>
-    </row>
-    <row r="38" spans="2:4">
-      <c r="B38" s="10" t="s">
-        <v>257</v>
-      </c>
-      <c r="C38" s="10" t="s">
-        <v>292</v>
-      </c>
-      <c r="D38" s="10" t="s">
-        <v>292</v>
-      </c>
-    </row>
-    <row r="39" spans="2:4">
-      <c r="B39" s="11" t="s">
-        <v>257</v>
-      </c>
-      <c r="C39" s="11" t="s">
-        <v>293</v>
-      </c>
-      <c r="D39" s="11" t="s">
-        <v>293</v>
-      </c>
-    </row>
-    <row r="40" spans="2:4">
-      <c r="B40" s="10" t="s">
-        <v>257</v>
-      </c>
-      <c r="C40" s="10" t="s">
-        <v>294</v>
-      </c>
-      <c r="D40" s="10" t="s">
-        <v>294</v>
-      </c>
-    </row>
-    <row r="41" spans="2:4">
-      <c r="B41" s="11" t="s">
-        <v>257</v>
-      </c>
-      <c r="C41" s="11" t="s">
-        <v>295</v>
-      </c>
-      <c r="D41" s="11" t="s">
-        <v>295</v>
-      </c>
-    </row>
-    <row r="42" spans="2:4">
-      <c r="B42" s="10" t="s">
-        <v>257</v>
-      </c>
-      <c r="C42" s="10" t="s">
-        <v>296</v>
-      </c>
-      <c r="D42" s="10" t="s">
-        <v>296</v>
-      </c>
-    </row>
-    <row r="43" spans="2:4">
-      <c r="B43" s="11" t="s">
-        <v>257</v>
-      </c>
-      <c r="C43" s="11" t="s">
-        <v>297</v>
-      </c>
-      <c r="D43" s="11" t="s">
-        <v>297</v>
-      </c>
-    </row>
-    <row r="44" spans="2:4">
-      <c r="B44" s="10" t="s">
-        <v>257</v>
-      </c>
-      <c r="C44" s="10" t="s">
-        <v>298</v>
-      </c>
-      <c r="D44" s="10" t="s">
-        <v>298</v>
-      </c>
-    </row>
-    <row r="45" spans="2:4">
-      <c r="B45" s="11" t="s">
-        <v>257</v>
-      </c>
-      <c r="C45" s="11" t="s">
-        <v>299</v>
-      </c>
-      <c r="D45" s="11" t="s">
-        <v>299</v>
-      </c>
-    </row>
-    <row r="46" spans="2:4">
-      <c r="B46" s="10" t="s">
-        <v>257</v>
-      </c>
-      <c r="C46" s="10" t="s">
-        <v>300</v>
-      </c>
-      <c r="D46" s="10" t="s">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="47" spans="2:4">
-      <c r="B47" s="11" t="s">
-        <v>257</v>
-      </c>
-      <c r="C47" s="11" t="s">
-        <v>301</v>
-      </c>
-      <c r="D47" s="11" t="s">
-        <v>301</v>
-      </c>
-    </row>
-    <row r="48" spans="2:4">
-      <c r="B48" s="10" t="s">
-        <v>257</v>
-      </c>
-      <c r="C48" s="10" t="s">
-        <v>302</v>
-      </c>
-      <c r="D48" s="10" t="s">
-        <v>302</v>
-      </c>
-    </row>
-    <row r="49" spans="2:4">
-      <c r="B49" s="11" t="s">
-        <v>257</v>
-      </c>
-      <c r="C49" s="11" t="s">
-        <v>303</v>
-      </c>
-      <c r="D49" s="11" t="s">
-        <v>303</v>
-      </c>
-    </row>
-    <row r="50" spans="2:4">
-      <c r="B50" s="10" t="s">
-        <v>257</v>
-      </c>
-      <c r="C50" s="10" t="s">
-        <v>304</v>
-      </c>
-      <c r="D50" s="10" t="s">
-        <v>304</v>
-      </c>
-    </row>
-    <row r="51" spans="2:4">
-      <c r="B51" s="11" t="s">
-        <v>257</v>
-      </c>
-      <c r="C51" s="11" t="s">
-        <v>305</v>
-      </c>
-      <c r="D51" s="11" t="s">
-        <v>305</v>
-      </c>
-    </row>
-    <row r="52" spans="2:4">
-      <c r="B52" s="10" t="s">
-        <v>257</v>
-      </c>
-      <c r="C52" s="10" t="s">
-        <v>306</v>
-      </c>
-      <c r="D52" s="10" t="s">
-        <v>306</v>
-      </c>
-    </row>
-    <row r="53" spans="2:4">
-      <c r="B53" s="11" t="s">
-        <v>257</v>
-      </c>
-      <c r="C53" s="11" t="s">
-        <v>307</v>
-      </c>
-      <c r="D53" s="11" t="s">
-        <v>307</v>
-      </c>
-    </row>
-    <row r="54" spans="2:4">
-      <c r="B54" s="10" t="s">
-        <v>257</v>
-      </c>
-      <c r="C54" s="10" t="s">
-        <v>308</v>
-      </c>
-      <c r="D54" s="10" t="s">
-        <v>308</v>
-      </c>
-    </row>
-    <row r="55" spans="2:4">
-      <c r="B55" s="11" t="s">
-        <v>257</v>
-      </c>
-      <c r="C55" s="11" t="s">
-        <v>309</v>
-      </c>
-      <c r="D55" s="11" t="s">
-        <v>309</v>
-      </c>
-    </row>
-    <row r="56" spans="2:4">
-      <c r="B56" s="10" t="s">
-        <v>257</v>
-      </c>
-      <c r="C56" s="10" t="s">
-        <v>310</v>
-      </c>
-      <c r="D56" s="10" t="s">
-        <v>310</v>
-      </c>
-    </row>
-    <row r="57" spans="2:4">
-      <c r="B57" s="11" t="s">
-        <v>257</v>
-      </c>
-      <c r="C57" s="11" t="s">
-        <v>311</v>
-      </c>
-      <c r="D57" s="11" t="s">
-        <v>311</v>
-      </c>
-    </row>
-    <row r="58" spans="2:4">
-      <c r="B58" s="10" t="s">
-        <v>257</v>
-      </c>
-      <c r="C58" s="10" t="s">
-        <v>312</v>
-      </c>
-      <c r="D58" s="10" t="s">
-        <v>312</v>
-      </c>
-    </row>
-    <row r="59" spans="2:4">
-      <c r="B59" s="11" t="s">
-        <v>257</v>
-      </c>
-      <c r="C59" s="11" t="s">
-        <v>313</v>
-      </c>
-      <c r="D59" s="11" t="s">
-        <v>313</v>
-      </c>
-    </row>
-    <row r="60" spans="2:4">
-      <c r="B60" s="10" t="s">
-        <v>257</v>
-      </c>
-      <c r="C60" s="10" t="s">
-        <v>314</v>
-      </c>
-      <c r="D60" s="10" t="s">
-        <v>314</v>
-      </c>
-    </row>
-    <row r="61" spans="2:4">
-      <c r="B61" s="11" t="s">
-        <v>257</v>
-      </c>
-      <c r="C61" s="11" t="s">
-        <v>315</v>
-      </c>
-      <c r="D61" s="11" t="s">
-        <v>315</v>
-      </c>
-    </row>
-    <row r="62" spans="2:4">
-      <c r="B62" s="10" t="s">
-        <v>257</v>
-      </c>
-      <c r="C62" s="10" t="s">
-        <v>316</v>
-      </c>
-      <c r="D62" s="10" t="s">
-        <v>316</v>
-      </c>
-    </row>
-    <row r="63" spans="2:4">
-      <c r="B63" s="11" t="s">
-        <v>257</v>
-      </c>
-      <c r="C63" s="11" t="s">
-        <v>317</v>
-      </c>
-      <c r="D63" s="11" t="s">
-        <v>317</v>
-      </c>
-    </row>
-    <row r="64" spans="2:4">
-      <c r="B64" s="10" t="s">
-        <v>257</v>
-      </c>
-      <c r="C64" s="10" t="s">
-        <v>318</v>
-      </c>
-      <c r="D64" s="10" t="s">
-        <v>318</v>
-      </c>
-    </row>
-    <row r="65" spans="2:4">
-      <c r="B65" s="11" t="s">
-        <v>257</v>
-      </c>
-      <c r="C65" s="11" t="s">
-        <v>319</v>
-      </c>
-      <c r="D65" s="11" t="s">
-        <v>319</v>
-      </c>
-    </row>
-    <row r="66" spans="2:4">
-      <c r="B66" s="10" t="s">
-        <v>257</v>
-      </c>
-      <c r="C66" s="10" t="s">
-        <v>320</v>
-      </c>
-      <c r="D66" s="10" t="s">
-        <v>320</v>
-      </c>
-    </row>
-    <row r="67" spans="2:4">
-      <c r="B67" s="11" t="s">
-        <v>257</v>
-      </c>
-      <c r="C67" s="11" t="s">
-        <v>321</v>
-      </c>
-      <c r="D67" s="11" t="s">
-        <v>321</v>
-      </c>
-    </row>
-    <row r="68" spans="2:4">
-      <c r="B68" s="10" t="s">
-        <v>257</v>
-      </c>
-      <c r="C68" s="10" t="s">
-        <v>322</v>
-      </c>
-      <c r="D68" s="10" t="s">
-        <v>322</v>
-      </c>
-    </row>
-    <row r="69" spans="2:4">
-      <c r="B69" s="11" t="s">
-        <v>257</v>
-      </c>
-      <c r="C69" s="11" t="s">
-        <v>323</v>
-      </c>
-      <c r="D69" s="11" t="s">
-        <v>323</v>
-      </c>
-    </row>
-    <row r="70" spans="2:4">
-      <c r="B70" s="10" t="s">
-        <v>257</v>
-      </c>
-      <c r="C70" s="10" t="s">
-        <v>324</v>
-      </c>
-      <c r="D70" s="10" t="s">
-        <v>324</v>
-      </c>
-    </row>
-    <row r="71" spans="2:4">
-      <c r="B71" s="11" t="s">
-        <v>257</v>
-      </c>
-      <c r="C71" s="11" t="s">
-        <v>325</v>
-      </c>
-      <c r="D71" s="11" t="s">
-        <v>325</v>
-      </c>
-    </row>
-    <row r="72" spans="2:4">
-      <c r="B72" s="10" t="s">
-        <v>257</v>
-      </c>
-      <c r="C72" s="10" t="s">
-        <v>326</v>
-      </c>
-      <c r="D72" s="10" t="s">
-        <v>326</v>
-      </c>
-    </row>
-    <row r="73" spans="2:4">
-      <c r="B73" s="11" t="s">
-        <v>257</v>
-      </c>
-      <c r="C73" s="11" t="s">
-        <v>327</v>
-      </c>
-      <c r="D73" s="11" t="s">
-        <v>327</v>
-      </c>
-    </row>
-    <row r="74" spans="2:4">
-      <c r="B74" s="10" t="s">
-        <v>257</v>
-      </c>
-      <c r="C74" s="10" t="s">
-        <v>328</v>
-      </c>
-      <c r="D74" s="10" t="s">
-        <v>328</v>
-      </c>
-    </row>
-    <row r="75" spans="2:4">
-      <c r="B75" s="11" t="s">
-        <v>257</v>
-      </c>
-      <c r="C75" s="11" t="s">
-        <v>329</v>
-      </c>
-      <c r="D75" s="11" t="s">
-        <v>329</v>
-      </c>
-    </row>
-    <row r="76" spans="2:4">
-      <c r="B76" s="10" t="s">
-        <v>257</v>
-      </c>
-      <c r="C76" s="10" t="s">
-        <v>330</v>
-      </c>
-      <c r="D76" s="10" t="s">
-        <v>330</v>
-      </c>
-    </row>
-    <row r="77" spans="2:4">
-      <c r="B77" s="11" t="s">
-        <v>257</v>
-      </c>
-      <c r="C77" s="11" t="s">
-        <v>331</v>
-      </c>
-      <c r="D77" s="11" t="s">
-        <v>331</v>
-      </c>
-    </row>
-    <row r="78" spans="2:4">
-      <c r="B78" s="10" t="s">
-        <v>257</v>
-      </c>
-      <c r="C78" s="10" t="s">
-        <v>332</v>
-      </c>
-      <c r="D78" s="10" t="s">
-        <v>332</v>
-      </c>
-    </row>
-    <row r="79" spans="2:4">
-      <c r="B79" s="11" t="s">
-        <v>257</v>
-      </c>
-      <c r="C79" s="11" t="s">
-        <v>333</v>
-      </c>
-      <c r="D79" s="11" t="s">
-        <v>333</v>
-      </c>
-    </row>
-    <row r="80" spans="2:4">
-      <c r="B80" s="10" t="s">
-        <v>257</v>
-      </c>
-      <c r="C80" s="10" t="s">
-        <v>334</v>
-      </c>
-      <c r="D80" s="10" t="s">
-        <v>334</v>
-      </c>
-    </row>
-    <row r="81" spans="2:4">
-      <c r="B81" s="11" t="s">
-        <v>257</v>
-      </c>
-      <c r="C81" s="11" t="s">
-        <v>335</v>
-      </c>
-      <c r="D81" s="11" t="s">
-        <v>335</v>
-      </c>
-    </row>
-    <row r="82" spans="2:4">
-      <c r="B82" s="10" t="s">
-        <v>257</v>
-      </c>
-      <c r="C82" s="10" t="s">
-        <v>336</v>
-      </c>
-      <c r="D82" s="10" t="s">
-        <v>336</v>
-      </c>
-    </row>
-    <row r="83" spans="2:4">
-      <c r="B83" s="11" t="s">
-        <v>257</v>
-      </c>
-      <c r="C83" s="11" t="s">
-        <v>337</v>
-      </c>
-      <c r="D83" s="11" t="s">
-        <v>337</v>
-      </c>
-    </row>
-    <row r="84" spans="2:4">
-      <c r="B84" s="10" t="s">
-        <v>257</v>
-      </c>
-      <c r="C84" s="10" t="s">
-        <v>338</v>
-      </c>
-      <c r="D84" s="10" t="s">
-        <v>338</v>
-      </c>
-    </row>
-    <row r="85" spans="2:4">
-      <c r="B85" s="11" t="s">
-        <v>257</v>
-      </c>
-      <c r="C85" s="11" t="s">
-        <v>339</v>
-      </c>
-      <c r="D85" s="11" t="s">
-        <v>339</v>
-      </c>
-    </row>
-    <row r="86" spans="2:4">
-      <c r="B86" s="10" t="s">
-        <v>257</v>
-      </c>
-      <c r="C86" s="10" t="s">
-        <v>340</v>
-      </c>
-      <c r="D86" s="10" t="s">
-        <v>340</v>
-      </c>
-    </row>
-    <row r="87" spans="2:4">
-      <c r="B87" s="11" t="s">
-        <v>257</v>
-      </c>
-      <c r="C87" s="11" t="s">
-        <v>341</v>
-      </c>
-      <c r="D87" s="11" t="s">
-        <v>341</v>
-      </c>
-    </row>
-    <row r="88" spans="2:4">
-      <c r="B88" s="10" t="s">
-        <v>257</v>
-      </c>
-      <c r="C88" s="10" t="s">
-        <v>342</v>
-      </c>
-      <c r="D88" s="10" t="s">
-        <v>342</v>
-      </c>
-    </row>
-    <row r="89" spans="2:4">
-      <c r="B89" s="11" t="s">
-        <v>257</v>
-      </c>
-      <c r="C89" s="11" t="s">
-        <v>343</v>
-      </c>
-      <c r="D89" s="11" t="s">
-        <v>343</v>
-      </c>
-    </row>
-    <row r="90" spans="2:4">
-      <c r="B90" s="10" t="s">
-        <v>257</v>
-      </c>
-      <c r="C90" s="10" t="s">
-        <v>344</v>
-      </c>
-      <c r="D90" s="10" t="s">
-        <v>344</v>
-      </c>
-    </row>
-    <row r="91" spans="2:4">
-      <c r="B91" s="11" t="s">
-        <v>257</v>
-      </c>
-      <c r="C91" s="11" t="s">
-        <v>345</v>
-      </c>
-      <c r="D91" s="11" t="s">
-        <v>345</v>
-      </c>
-    </row>
-    <row r="92" spans="2:4">
-      <c r="B92" s="10" t="s">
-        <v>257</v>
-      </c>
-      <c r="C92" s="10" t="s">
-        <v>346</v>
-      </c>
-      <c r="D92" s="10" t="s">
-        <v>346</v>
-      </c>
-    </row>
-    <row r="93" spans="2:4">
-      <c r="B93" s="11" t="s">
-        <v>257</v>
-      </c>
-      <c r="C93" s="11" t="s">
-        <v>347</v>
-      </c>
-      <c r="D93" s="11" t="s">
-        <v>347</v>
-      </c>
-    </row>
-    <row r="94" spans="2:4">
-      <c r="B94" s="10" t="s">
-        <v>257</v>
-      </c>
-      <c r="C94" s="10" t="s">
-        <v>348</v>
-      </c>
-      <c r="D94" s="10" t="s">
-        <v>348</v>
-      </c>
-    </row>
-    <row r="95" spans="2:4">
-      <c r="B95" s="11" t="s">
-        <v>257</v>
-      </c>
-      <c r="C95" s="11" t="s">
-        <v>349</v>
-      </c>
-      <c r="D95" s="11" t="s">
-        <v>349</v>
-      </c>
-    </row>
-    <row r="96" spans="2:4">
-      <c r="B96" s="10" t="s">
-        <v>257</v>
-      </c>
-      <c r="C96" s="10" t="s">
-        <v>350</v>
-      </c>
-      <c r="D96" s="10" t="s">
-        <v>350</v>
-      </c>
-    </row>
-    <row r="97" spans="2:4">
-      <c r="B97" s="11" t="s">
-        <v>257</v>
-      </c>
-      <c r="C97" s="11" t="s">
-        <v>351</v>
-      </c>
-      <c r="D97" s="11" t="s">
-        <v>351</v>
-      </c>
-    </row>
-    <row r="98" spans="2:4">
-      <c r="B98" s="10" t="s">
-        <v>257</v>
-      </c>
-      <c r="C98" s="10" t="s">
-        <v>352</v>
-      </c>
-      <c r="D98" s="10" t="s">
-        <v>352</v>
-      </c>
-    </row>
-    <row r="99" spans="2:4">
-      <c r="B99" s="11" t="s">
-        <v>257</v>
-      </c>
-      <c r="C99" s="11" t="s">
-        <v>353</v>
-      </c>
-      <c r="D99" s="11" t="s">
-        <v>353</v>
-      </c>
-    </row>
-    <row r="100" spans="2:4">
-      <c r="B100" s="10" t="s">
-        <v>257</v>
-      </c>
-      <c r="C100" s="10" t="s">
-        <v>354</v>
-      </c>
-      <c r="D100" s="10" t="s">
-        <v>354</v>
-      </c>
-    </row>
-    <row r="101" spans="2:4">
-      <c r="B101" s="11" t="s">
-        <v>257</v>
-      </c>
-      <c r="C101" s="11" t="s">
-        <v>355</v>
-      </c>
-      <c r="D101" s="11" t="s">
-        <v>355</v>
-      </c>
-    </row>
-    <row r="102" spans="2:4">
-      <c r="B102" s="10" t="s">
-        <v>257</v>
-      </c>
-      <c r="C102" s="10" t="s">
-        <v>356</v>
-      </c>
-      <c r="D102" s="10" t="s">
-        <v>356</v>
-      </c>
-    </row>
-    <row r="103" spans="2:4">
-      <c r="B103" s="11" t="s">
-        <v>257</v>
-      </c>
-      <c r="C103" s="11" t="s">
-        <v>357</v>
-      </c>
-      <c r="D103" s="11" t="s">
-        <v>357</v>
-      </c>
-    </row>
-    <row r="104" spans="2:4">
-      <c r="B104" s="10" t="s">
-        <v>257</v>
-      </c>
-      <c r="C104" s="10" t="s">
-        <v>358</v>
-      </c>
-      <c r="D104" s="10" t="s">
-        <v>358</v>
-      </c>
-    </row>
-    <row r="105" spans="2:4">
-      <c r="B105" s="11" t="s">
-        <v>257</v>
-      </c>
-      <c r="C105" s="11" t="s">
-        <v>359</v>
-      </c>
-      <c r="D105" s="11" t="s">
-        <v>359</v>
-      </c>
-    </row>
-    <row r="106" spans="2:4">
-      <c r="B106" s="10" t="s">
-        <v>257</v>
-      </c>
-      <c r="C106" s="10" t="s">
-        <v>360</v>
-      </c>
-      <c r="D106" s="10" t="s">
-        <v>360</v>
-      </c>
-    </row>
-    <row r="107" spans="2:4">
-      <c r="B107" s="11" t="s">
-        <v>257</v>
-      </c>
-      <c r="C107" s="11" t="s">
-        <v>361</v>
-      </c>
-      <c r="D107" s="11" t="s">
-        <v>361</v>
-      </c>
-    </row>
-    <row r="108" spans="2:4">
-      <c r="B108" s="10" t="s">
-        <v>257</v>
-      </c>
-      <c r="C108" s="10" t="s">
-        <v>362</v>
-      </c>
-      <c r="D108" s="10" t="s">
-        <v>362</v>
-      </c>
-    </row>
-    <row r="109" spans="2:4">
-      <c r="B109" s="11" t="s">
-        <v>257</v>
-      </c>
-      <c r="C109" s="11" t="s">
-        <v>363</v>
-      </c>
-      <c r="D109" s="11" t="s">
-        <v>363</v>
-      </c>
-    </row>
-    <row r="110" spans="2:4">
-      <c r="B110" s="10" t="s">
-        <v>257</v>
-      </c>
-      <c r="C110" s="10" t="s">
-        <v>364</v>
-      </c>
-      <c r="D110" s="10" t="s">
-        <v>364</v>
-      </c>
-    </row>
-    <row r="111" spans="2:4">
-      <c r="B111" s="11" t="s">
-        <v>257</v>
-      </c>
-      <c r="C111" s="11" t="s">
-        <v>365</v>
-      </c>
-      <c r="D111" s="11" t="s">
-        <v>365</v>
-      </c>
-    </row>
-    <row r="112" spans="2:4">
-      <c r="B112" s="10" t="s">
-        <v>257</v>
-      </c>
-      <c r="C112" s="10" t="s">
-        <v>366</v>
-      </c>
-      <c r="D112" s="10" t="s">
-        <v>366</v>
-      </c>
-    </row>
-    <row r="113" spans="2:4">
-      <c r="B113" s="11" t="s">
-        <v>257</v>
-      </c>
-      <c r="C113" s="11" t="s">
-        <v>367</v>
-      </c>
-      <c r="D113" s="11" t="s">
-        <v>367</v>
-      </c>
-    </row>
-    <row r="114" spans="2:4">
-      <c r="B114" s="10" t="s">
-        <v>257</v>
-      </c>
-      <c r="C114" s="10" t="s">
-        <v>368</v>
-      </c>
-      <c r="D114" s="10" t="s">
-        <v>368</v>
-      </c>
-    </row>
-    <row r="115" spans="2:4">
-      <c r="B115" s="11" t="s">
-        <v>257</v>
-      </c>
-      <c r="C115" s="11" t="s">
-        <v>369</v>
-      </c>
-      <c r="D115" s="11" t="s">
-        <v>369</v>
-      </c>
-    </row>
-    <row r="116" spans="2:4">
-      <c r="B116" s="10" t="s">
-        <v>257</v>
-      </c>
-      <c r="C116" s="10" t="s">
-        <v>370</v>
-      </c>
-      <c r="D116" s="10" t="s">
-        <v>370</v>
-      </c>
-    </row>
-    <row r="117" spans="2:4">
-      <c r="B117" s="11" t="s">
-        <v>257</v>
-      </c>
-      <c r="C117" s="11" t="s">
-        <v>371</v>
-      </c>
-      <c r="D117" s="11" t="s">
-        <v>371</v>
-      </c>
-    </row>
-    <row r="118" spans="2:4">
-      <c r="B118" s="10" t="s">
-        <v>257</v>
-      </c>
-      <c r="C118" s="10" t="s">
-        <v>372</v>
-      </c>
-      <c r="D118" s="10" t="s">
-        <v>372</v>
-      </c>
-    </row>
-    <row r="119" spans="2:4">
-      <c r="B119" s="11" t="s">
-        <v>257</v>
-      </c>
-      <c r="C119" s="11" t="s">
-        <v>373</v>
-      </c>
-      <c r="D119" s="11" t="s">
-        <v>373</v>
-      </c>
-    </row>
-    <row r="120" spans="2:4">
-      <c r="B120" s="10" t="s">
-        <v>257</v>
-      </c>
-      <c r="C120" s="10" t="s">
-        <v>374</v>
-      </c>
-      <c r="D120" s="10" t="s">
-        <v>374</v>
-      </c>
-    </row>
-    <row r="121" spans="2:4">
-      <c r="B121" s="11" t="s">
-        <v>257</v>
-      </c>
-      <c r="C121" s="11" t="s">
-        <v>375</v>
-      </c>
-      <c r="D121" s="11" t="s">
-        <v>375</v>
-      </c>
-    </row>
-    <row r="122" spans="2:4">
-      <c r="B122" s="10" t="s">
-        <v>257</v>
-      </c>
-      <c r="C122" s="10" t="s">
-        <v>376</v>
-      </c>
-      <c r="D122" s="10" t="s">
-        <v>376</v>
-      </c>
-    </row>
-    <row r="123" spans="2:4">
-      <c r="B123" s="11" t="s">
-        <v>257</v>
-      </c>
-      <c r="C123" s="11" t="s">
-        <v>377</v>
-      </c>
-      <c r="D123" s="11" t="s">
-        <v>377</v>
-      </c>
-    </row>
-    <row r="124" spans="2:4">
-      <c r="B124" s="10" t="s">
-        <v>257</v>
-      </c>
-      <c r="C124" s="10" t="s">
-        <v>378</v>
-      </c>
-      <c r="D124" s="10" t="s">
-        <v>378</v>
-      </c>
-    </row>
-    <row r="125" spans="2:4">
-      <c r="B125" s="11" t="s">
-        <v>257</v>
-      </c>
-      <c r="C125" s="11" t="s">
-        <v>379</v>
-      </c>
-      <c r="D125" s="11" t="s">
-        <v>379</v>
-      </c>
-    </row>
-    <row r="126" spans="2:4">
-      <c r="B126" s="10" t="s">
-        <v>257</v>
-      </c>
-      <c r="C126" s="10" t="s">
-        <v>380</v>
-      </c>
-      <c r="D126" s="10" t="s">
-        <v>380</v>
-      </c>
-    </row>
-    <row r="127" spans="2:4">
-      <c r="B127" s="11" t="s">
-        <v>257</v>
-      </c>
-      <c r="C127" s="11" t="s">
-        <v>381</v>
-      </c>
-      <c r="D127" s="11" t="s">
-        <v>381</v>
-      </c>
-    </row>
-    <row r="128" spans="2:4">
-      <c r="B128" s="10" t="s">
-        <v>257</v>
-      </c>
-      <c r="C128" s="10" t="s">
-        <v>382</v>
-      </c>
-      <c r="D128" s="10" t="s">
-        <v>382</v>
-      </c>
-    </row>
-    <row r="129" spans="2:4">
-      <c r="B129" s="11" t="s">
-        <v>257</v>
-      </c>
-      <c r="C129" s="11" t="s">
-        <v>383</v>
-      </c>
-      <c r="D129" s="11" t="s">
-        <v>383</v>
-      </c>
-    </row>
-    <row r="130" spans="2:4">
-      <c r="B130" s="10" t="s">
-        <v>257</v>
-      </c>
-      <c r="C130" s="10" t="s">
-        <v>384</v>
-      </c>
-      <c r="D130" s="10" t="s">
-        <v>384</v>
-      </c>
-    </row>
-    <row r="131" spans="2:4">
-      <c r="B131" s="11" t="s">
-        <v>257</v>
-      </c>
-      <c r="C131" s="11" t="s">
-        <v>385</v>
-      </c>
-      <c r="D131" s="11" t="s">
-        <v>385</v>
-      </c>
-    </row>
-    <row r="132" spans="2:4">
-      <c r="B132" s="10" t="s">
-        <v>257</v>
-      </c>
-      <c r="C132" s="10" t="s">
-        <v>386</v>
-      </c>
-      <c r="D132" s="10" t="s">
-        <v>386</v>
-      </c>
-    </row>
-    <row r="133" spans="2:4">
-      <c r="B133" s="11" t="s">
-        <v>257</v>
-      </c>
-      <c r="C133" s="11" t="s">
-        <v>387</v>
-      </c>
-      <c r="D133" s="11" t="s">
-        <v>387</v>
-      </c>
-    </row>
-    <row r="134" spans="2:4">
-      <c r="B134" s="10" t="s">
-        <v>257</v>
-      </c>
-      <c r="C134" s="10" t="s">
-        <v>388</v>
-      </c>
-      <c r="D134" s="10" t="s">
-        <v>388</v>
-      </c>
-    </row>
-    <row r="135" spans="2:4">
-      <c r="B135" s="11" t="s">
-        <v>257</v>
-      </c>
-      <c r="C135" s="11" t="s">
-        <v>389</v>
-      </c>
-      <c r="D135" s="11" t="s">
-        <v>389</v>
-      </c>
-    </row>
-    <row r="136" spans="2:4">
-      <c r="B136" s="10" t="s">
-        <v>257</v>
-      </c>
-      <c r="C136" s="10" t="s">
-        <v>390</v>
-      </c>
-      <c r="D136" s="10" t="s">
-        <v>390</v>
-      </c>
-    </row>
-    <row r="137" spans="2:4">
-      <c r="B137" s="11" t="s">
-        <v>257</v>
-      </c>
-      <c r="C137" s="11" t="s">
-        <v>391</v>
-      </c>
-      <c r="D137" s="11" t="s">
-        <v>391</v>
-      </c>
-    </row>
-    <row r="138" spans="2:4">
-      <c r="B138" s="10" t="s">
-        <v>257</v>
-      </c>
-      <c r="C138" s="10" t="s">
-        <v>392</v>
-      </c>
-      <c r="D138" s="10" t="s">
-        <v>392</v>
-      </c>
-    </row>
-    <row r="139" spans="2:4">
-      <c r="B139" s="11" t="s">
-        <v>257</v>
-      </c>
-      <c r="C139" s="11" t="s">
-        <v>393</v>
-      </c>
-      <c r="D139" s="11" t="s">
-        <v>393</v>
-      </c>
-    </row>
-    <row r="140" spans="2:4">
-      <c r="B140" s="10" t="s">
-        <v>257</v>
-      </c>
-      <c r="C140" s="10" t="s">
-        <v>394</v>
-      </c>
-      <c r="D140" s="10" t="s">
-        <v>394</v>
-      </c>
-    </row>
-    <row r="141" spans="2:4">
-      <c r="B141" s="11" t="s">
-        <v>257</v>
-      </c>
-      <c r="C141" s="11" t="s">
-        <v>395</v>
-      </c>
-      <c r="D141" s="11" t="s">
-        <v>395</v>
-      </c>
-    </row>
-    <row r="142" spans="2:4">
-      <c r="B142" s="10" t="s">
-        <v>257</v>
-      </c>
-      <c r="C142" s="10" t="s">
-        <v>396</v>
-      </c>
-      <c r="D142" s="10" t="s">
-        <v>396</v>
-      </c>
-    </row>
-    <row r="143" spans="2:4">
-      <c r="B143" s="11" t="s">
-        <v>257</v>
-      </c>
-      <c r="C143" s="11" t="s">
-        <v>397</v>
-      </c>
-      <c r="D143" s="11" t="s">
-        <v>397</v>
-      </c>
-    </row>
-    <row r="144" spans="2:4">
-      <c r="B144" s="10" t="s">
-        <v>257</v>
-      </c>
-      <c r="C144" s="10" t="s">
-        <v>398</v>
-      </c>
-      <c r="D144" s="10" t="s">
-        <v>398</v>
-      </c>
-    </row>
-    <row r="145" spans="2:4">
-      <c r="B145" s="11" t="s">
-        <v>257</v>
-      </c>
-      <c r="C145" s="11" t="s">
-        <v>399</v>
-      </c>
-      <c r="D145" s="11" t="s">
-        <v>399</v>
-      </c>
-    </row>
-    <row r="146" spans="2:4">
-      <c r="B146" s="10" t="s">
-        <v>257</v>
-      </c>
-      <c r="C146" s="10" t="s">
-        <v>400</v>
-      </c>
-      <c r="D146" s="10" t="s">
-        <v>400</v>
-      </c>
-    </row>
-    <row r="147" spans="2:4">
-      <c r="B147" s="11" t="s">
-        <v>257</v>
-      </c>
-      <c r="C147" s="11" t="s">
-        <v>401</v>
-      </c>
-      <c r="D147" s="11" t="s">
-        <v>401</v>
-      </c>
-    </row>
-    <row r="148" spans="2:4">
-      <c r="B148" s="10" t="s">
-        <v>257</v>
-      </c>
-      <c r="C148" s="10" t="s">
-        <v>402</v>
-      </c>
-      <c r="D148" s="10" t="s">
-        <v>402</v>
-      </c>
-    </row>
-    <row r="149" spans="2:4">
-      <c r="B149" s="11" t="s">
-        <v>257</v>
-      </c>
-      <c r="C149" s="11" t="s">
-        <v>403</v>
-      </c>
-      <c r="D149" s="11" t="s">
-        <v>403</v>
-      </c>
-    </row>
-    <row r="150" spans="2:4">
-      <c r="B150" s="10" t="s">
-        <v>257</v>
-      </c>
-      <c r="C150" s="10" t="s">
-        <v>404</v>
-      </c>
-      <c r="D150" s="10" t="s">
-        <v>404</v>
-      </c>
-    </row>
-    <row r="151" spans="2:4">
-      <c r="B151" s="11" t="s">
-        <v>257</v>
-      </c>
-      <c r="C151" s="11" t="s">
-        <v>405</v>
-      </c>
-      <c r="D151" s="11" t="s">
-        <v>405</v>
-      </c>
-    </row>
-    <row r="152" spans="2:4">
-      <c r="B152" s="10" t="s">
-        <v>257</v>
-      </c>
-      <c r="C152" s="10" t="s">
-        <v>406</v>
-      </c>
-      <c r="D152" s="10" t="s">
-        <v>406</v>
-      </c>
-    </row>
-    <row r="153" spans="2:4">
-      <c r="B153" s="11" t="s">
-        <v>257</v>
-      </c>
-      <c r="C153" s="11" t="s">
-        <v>407</v>
-      </c>
-      <c r="D153" s="11" t="s">
-        <v>407</v>
-      </c>
-    </row>
-    <row r="154" spans="2:4">
-      <c r="B154" s="10" t="s">
-        <v>257</v>
-      </c>
-      <c r="C154" s="10" t="s">
-        <v>408</v>
-      </c>
-      <c r="D154" s="10" t="s">
-        <v>408</v>
-      </c>
-    </row>
-    <row r="155" spans="2:4">
-      <c r="B155" s="11" t="s">
-        <v>257</v>
-      </c>
-      <c r="C155" s="11" t="s">
-        <v>409</v>
-      </c>
-      <c r="D155" s="11" t="s">
-        <v>409</v>
-      </c>
-    </row>
-    <row r="156" spans="2:4">
-      <c r="B156" s="10" t="s">
-        <v>257</v>
-      </c>
-      <c r="C156" s="10" t="s">
-        <v>410</v>
-      </c>
-      <c r="D156" s="10" t="s">
-        <v>410</v>
-      </c>
-    </row>
-    <row r="157" spans="2:4">
-      <c r="B157" s="11" t="s">
-        <v>257</v>
-      </c>
-      <c r="C157" s="11" t="s">
-        <v>411</v>
-      </c>
-      <c r="D157" s="11" t="s">
-        <v>411</v>
-      </c>
-    </row>
-    <row r="158" spans="2:4">
-      <c r="B158" s="10" t="s">
-        <v>257</v>
-      </c>
-      <c r="C158" s="10" t="s">
-        <v>412</v>
-      </c>
-      <c r="D158" s="10" t="s">
-        <v>412</v>
-      </c>
-    </row>
-    <row r="159" spans="2:4">
-      <c r="B159" s="11" t="s">
-        <v>257</v>
-      </c>
-      <c r="C159" s="11" t="s">
-        <v>413</v>
-      </c>
-      <c r="D159" s="11" t="s">
-        <v>413</v>
+      <c r="D160" s="12" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="161" spans="2:4">
+      <c r="B161" s="13" t="s">
+        <v>257</v>
+      </c>
+      <c r="C161" s="13" t="s">
+        <v>415</v>
+      </c>
+      <c r="D161" s="13" t="s">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="162" spans="2:4">
+      <c r="B162" s="12" t="s">
+        <v>257</v>
+      </c>
+      <c r="C162" s="12" t="s">
+        <v>416</v>
+      </c>
+      <c r="D162" s="12" t="s">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="163" spans="2:4">
+      <c r="B163" s="13" t="s">
+        <v>257</v>
+      </c>
+      <c r="C163" s="13" t="s">
+        <v>417</v>
+      </c>
+      <c r="D163" s="13" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="164" spans="2:4">
+      <c r="B164" s="12" t="s">
+        <v>257</v>
+      </c>
+      <c r="C164" s="12" t="s">
+        <v>418</v>
+      </c>
+      <c r="D164" s="12" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="165" spans="2:4">
+      <c r="B165" s="13" t="s">
+        <v>257</v>
+      </c>
+      <c r="C165" s="13" t="s">
+        <v>419</v>
+      </c>
+      <c r="D165" s="13" t="s">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="166" spans="2:4">
+      <c r="B166" s="12" t="s">
+        <v>257</v>
+      </c>
+      <c r="C166" s="12" t="s">
+        <v>420</v>
+      </c>
+      <c r="D166" s="12" t="s">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="167" spans="2:4">
+      <c r="B167" s="13" t="s">
+        <v>257</v>
+      </c>
+      <c r="C167" s="13" t="s">
+        <v>421</v>
+      </c>
+      <c r="D167" s="13" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="168" spans="2:4">
+      <c r="B168" s="12" t="s">
+        <v>257</v>
+      </c>
+      <c r="C168" s="12" t="s">
+        <v>422</v>
+      </c>
+      <c r="D168" s="12" t="s">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="169" spans="2:4">
+      <c r="B169" s="13" t="s">
+        <v>257</v>
+      </c>
+      <c r="C169" s="13" t="s">
+        <v>423</v>
+      </c>
+      <c r="D169" s="13" t="s">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="170" spans="2:4">
+      <c r="B170" s="12" t="s">
+        <v>257</v>
+      </c>
+      <c r="C170" s="12" t="s">
+        <v>424</v>
+      </c>
+      <c r="D170" s="12" t="s">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="171" spans="2:4">
+      <c r="B171" s="13" t="s">
+        <v>257</v>
+      </c>
+      <c r="C171" s="13" t="s">
+        <v>425</v>
+      </c>
+      <c r="D171" s="13" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="172" spans="2:4">
+      <c r="B172" s="12" t="s">
+        <v>257</v>
+      </c>
+      <c r="C172" s="12" t="s">
+        <v>426</v>
+      </c>
+      <c r="D172" s="12" t="s">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="173" spans="2:4">
+      <c r="B173" s="13" t="s">
+        <v>257</v>
+      </c>
+      <c r="C173" s="13" t="s">
+        <v>427</v>
+      </c>
+      <c r="D173" s="13" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="174" spans="2:4">
+      <c r="B174" s="12" t="s">
+        <v>257</v>
+      </c>
+      <c r="C174" s="12" t="s">
+        <v>428</v>
+      </c>
+      <c r="D174" s="12" t="s">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="175" spans="2:4">
+      <c r="B175" s="13" t="s">
+        <v>257</v>
+      </c>
+      <c r="C175" s="13" t="s">
+        <v>429</v>
+      </c>
+      <c r="D175" s="13" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="176" spans="2:4">
+      <c r="B176" s="12" t="s">
+        <v>257</v>
+      </c>
+      <c r="C176" s="12" t="s">
+        <v>430</v>
+      </c>
+      <c r="D176" s="12" t="s">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="177" spans="2:4">
+      <c r="B177" s="13" t="s">
+        <v>257</v>
+      </c>
+      <c r="C177" s="13" t="s">
+        <v>431</v>
+      </c>
+      <c r="D177" s="13" t="s">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="178" spans="2:4">
+      <c r="B178" s="12" t="s">
+        <v>257</v>
+      </c>
+      <c r="C178" s="12" t="s">
+        <v>432</v>
+      </c>
+      <c r="D178" s="12" t="s">
+        <v>432</v>
+      </c>
+    </row>
+    <row r="179" spans="2:4">
+      <c r="B179" s="13" t="s">
+        <v>257</v>
+      </c>
+      <c r="C179" s="13" t="s">
+        <v>433</v>
+      </c>
+      <c r="D179" s="13" t="s">
+        <v>433</v>
+      </c>
+    </row>
+    <row r="180" spans="2:4">
+      <c r="B180" s="12" t="s">
+        <v>257</v>
+      </c>
+      <c r="C180" s="12" t="s">
+        <v>434</v>
+      </c>
+      <c r="D180" s="12" t="s">
+        <v>434</v>
+      </c>
+    </row>
+    <row r="181" spans="2:4">
+      <c r="B181" s="13" t="s">
+        <v>257</v>
+      </c>
+      <c r="C181" s="13" t="s">
+        <v>435</v>
+      </c>
+      <c r="D181" s="13" t="s">
+        <v>435</v>
+      </c>
+    </row>
+    <row r="182" spans="2:4">
+      <c r="B182" s="12" t="s">
+        <v>257</v>
+      </c>
+      <c r="C182" s="12" t="s">
+        <v>436</v>
+      </c>
+      <c r="D182" s="12" t="s">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="183" spans="2:4">
+      <c r="B183" s="13" t="s">
+        <v>257</v>
+      </c>
+      <c r="C183" s="13" t="s">
+        <v>437</v>
+      </c>
+      <c r="D183" s="13" t="s">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="184" spans="2:4">
+      <c r="B184" s="12" t="s">
+        <v>257</v>
+      </c>
+      <c r="C184" s="12" t="s">
+        <v>438</v>
+      </c>
+      <c r="D184" s="12" t="s">
+        <v>438</v>
       </c>
     </row>
   </sheetData>
@@ -4700,7 +5048,7 @@
   <dimension ref="A1:P40"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L6" sqref="L6"/>
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.73046875" defaultRowHeight="14.25"/>
@@ -4791,7 +5139,7 @@
         <v>Postponed Transition_3d</v>
       </c>
       <c r="H6" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="I6" t="s">
         <v>132</v>
@@ -4817,7 +5165,7 @@
         <v>Target Net Zero 2050_3d</v>
       </c>
       <c r="H7" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="I7" t="s">
         <v>132</v>
@@ -4843,7 +5191,7 @@
         <v>Declared NDCs_3d</v>
       </c>
       <c r="H8" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="I8" t="s">
         <v>132</v>
@@ -4869,7 +5217,7 @@
         <v>Limited to 2 deg_3d</v>
       </c>
       <c r="H9" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="I9" t="s">
         <v>132</v>
@@ -4888,14 +5236,14 @@
       </c>
       <c r="B10" t="str">
         <f t="shared" si="1"/>
-        <v>Actual Policies_3d</v>
+        <v>Current Policies_3d</v>
       </c>
       <c r="G10" t="str">
         <f t="shared" si="2"/>
-        <v>Actual Policies_3d</v>
+        <v>Current Policies_3d</v>
       </c>
       <c r="H10" t="s">
-        <v>252</v>
+        <v>256</v>
       </c>
       <c r="I10" t="s">
         <v>132</v>
@@ -5078,15 +5426,15 @@
       </c>
       <c r="B17" t="str">
         <f t="shared" si="1"/>
-        <v>Actual Policies_15d</v>
+        <v>Current Policies_15d</v>
       </c>
       <c r="G17" t="str">
         <f t="shared" si="2"/>
-        <v>Actual Policies_15d</v>
+        <v>Current Policies_15d</v>
       </c>
       <c r="H17" t="str">
         <f t="shared" si="4"/>
-        <v>Actual Policies</v>
+        <v>Current Policies</v>
       </c>
       <c r="I17" t="s">
         <v>133</v>
@@ -5274,15 +5622,15 @@
       </c>
       <c r="B24" t="str">
         <f t="shared" si="1"/>
-        <v>Actual Policies_2w</v>
+        <v>Current Policies_2w</v>
       </c>
       <c r="G24" t="str">
         <f t="shared" si="2"/>
-        <v>Actual Policies_2w</v>
+        <v>Current Policies_2w</v>
       </c>
       <c r="H24" t="str">
         <f t="shared" si="4"/>
-        <v>Actual Policies</v>
+        <v>Current Policies</v>
       </c>
       <c r="I24" t="s">
         <v>134</v>
@@ -5470,15 +5818,15 @@
       </c>
       <c r="B31" t="str">
         <f t="shared" si="7"/>
-        <v>Actual Policies_16</v>
+        <v>Current Policies_16</v>
       </c>
       <c r="G31" t="str">
         <f t="shared" si="8"/>
-        <v>Actual Policies_16</v>
+        <v>Current Policies_16</v>
       </c>
       <c r="H31" t="str">
         <f t="shared" si="4"/>
-        <v>Actual Policies</v>
+        <v>Current Policies</v>
       </c>
       <c r="I31" t="s">
         <v>173</v>
@@ -5666,15 +6014,15 @@
       </c>
       <c r="B38" t="str">
         <f t="shared" si="7"/>
-        <v>Actual Policies_ann</v>
+        <v>Current Policies_ann</v>
       </c>
       <c r="G38" t="str">
         <f t="shared" si="8"/>
-        <v>Actual Policies_ann</v>
+        <v>Current Policies_ann</v>
       </c>
       <c r="H38" t="str">
         <f t="shared" si="4"/>
-        <v>Actual Policies</v>
+        <v>Current Policies</v>
       </c>
       <c r="I38" t="s">
         <v>174</v>
@@ -5880,10 +6228,10 @@
       <c r="N4" t="s">
         <v>80</v>
       </c>
-      <c r="T4" s="13" t="s">
+      <c r="T4" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="U4" s="13"/>
+      <c r="U4" s="8"/>
     </row>
     <row r="5" spans="1:21">
       <c r="A5" t="s">

</xml_diff>

<commit_message>
Updated CHE_grids model - 2025-08-21 13:06
</commit_message>
<xml_diff>
--- a/VerveStacks_CHE_grids/ReportDefs_vervestacks.xlsx
+++ b/VerveStacks_CHE_grids/ReportDefs_vervestacks.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Veda\Veda\Veda_models\vervestacks_models\VerveStacks_CHE_grids\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{AAABF813-F1D5-4A75-BC18-904DA1F7EC76}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{FC240E1B-644E-4544-BCC0-024415F5F4FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="17475" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1760,7 +1760,7 @@
         <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{399F0054-4F6E-CDD2-7BC0-5DBED7F90602}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{978FD6D0-E608-C29F-ED18-3A24BEADBB8F}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2081,7 +2081,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{29821C0C-DEBE-47AB-9FC1-CCCC57555E16}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{96E0ACFC-6FAF-4892-9830-8FEE9950A2B8}">
   <dimension ref="A1:H184"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>

</xml_diff>

<commit_message>
Updated CHE_grids model - 2025-08-21 14:14
</commit_message>
<xml_diff>
--- a/VerveStacks_CHE_grids/ReportDefs_vervestacks.xlsx
+++ b/VerveStacks_CHE_grids/ReportDefs_vervestacks.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Veda\Veda\Veda_models\vervestacks_models\VerveStacks_CHE_grids\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{273415B3-BC35-4813-AF3C-244F90AD0392}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{3216A7F1-D3BB-4612-9A35-E672C7D73578}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="17475" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1779,7 +1779,7 @@
         <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{717FD10A-AEEE-3956-5451-40FCA534A995}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0A3AF9A7-42C9-57DC-8F09-287091B0C2C5}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1834,7 +1834,7 @@
         <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4EDD798C-CCC9-4F4D-28D4-B81283C0933D}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5BAFFBE3-D1F3-5128-FFE9-576CD3887921}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2155,7 +2155,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B686F040-CC7A-444F-B6D7-DD9B65F0FD46}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D2436C7E-661C-47B8-80FA-79041E8217E8}">
   <dimension ref="A1:H191"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
@@ -5248,7 +5248,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C885BF27-18BA-407C-89D4-B92E513DF7EE}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D2D636E-8DA7-42AD-AD1B-852670D026FD}">
   <dimension ref="A1:H184"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>

<commit_message>
Updated CHE_grids model - 2025-08-21 14:52
</commit_message>
<xml_diff>
--- a/VerveStacks_CHE_grids/ReportDefs_vervestacks.xlsx
+++ b/VerveStacks_CHE_grids/ReportDefs_vervestacks.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Veda\Veda\Veda_models\vervestacks_models\VerveStacks_CHE_grids\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{3216A7F1-D3BB-4612-9A35-E672C7D73578}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{35C31C95-2113-40D2-B737-3845768F8A44}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="17475" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1779,7 +1779,7 @@
         <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0A3AF9A7-42C9-57DC-8F09-287091B0C2C5}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9A8DFCBC-4FCB-B9C0-0BA1-A42F5937C636}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1834,7 +1834,7 @@
         <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5BAFFBE3-D1F3-5128-FFE9-576CD3887921}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{973176DF-5AF3-6452-70C5-AFDF9B268BB3}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2155,7 +2155,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D2436C7E-661C-47B8-80FA-79041E8217E8}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F5DED83B-CA76-4E13-8A01-8EAF25611B5C}">
   <dimension ref="A1:H191"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
@@ -5248,7 +5248,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D2D636E-8DA7-42AD-AD1B-852670D026FD}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{70F2803A-4996-4D01-9E06-4F66553FE6CC}">
   <dimension ref="A1:H184"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>

<commit_message>
Updated CHE_grids model - 2025-08-21 15:23
</commit_message>
<xml_diff>
--- a/VerveStacks_CHE_grids/ReportDefs_vervestacks.xlsx
+++ b/VerveStacks_CHE_grids/ReportDefs_vervestacks.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Veda\Veda\Veda_models\vervestacks_models\VerveStacks_CHE_grids\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{35C31C95-2113-40D2-B737-3845768F8A44}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{816536C1-1A6A-49BC-8B75-2C9B57D41D37}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="17475" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1779,7 +1779,7 @@
         <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9A8DFCBC-4FCB-B9C0-0BA1-A42F5937C636}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4FA3E73A-C631-4361-F734-911A965D84F2}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1834,7 +1834,7 @@
         <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{973176DF-5AF3-6452-70C5-AFDF9B268BB3}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2766C111-C951-4D29-5B40-93EC75F24565}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2155,7 +2155,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F5DED83B-CA76-4E13-8A01-8EAF25611B5C}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B9653AD0-8FDC-4FB9-8F19-F7D7B61084CB}">
   <dimension ref="A1:H191"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
@@ -5248,7 +5248,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{70F2803A-4996-4D01-9E06-4F66553FE6CC}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{77FB699F-B42B-474B-9241-AE8FFD99F2EC}">
   <dimension ref="A1:H184"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>

<commit_message>
Updated CHE_grids model - 2025-08-21 15:51
</commit_message>
<xml_diff>
--- a/VerveStacks_CHE_grids/ReportDefs_vervestacks.xlsx
+++ b/VerveStacks_CHE_grids/ReportDefs_vervestacks.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Veda\Veda\Veda_models\vervestacks_models\VerveStacks_CHE_grids\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{816536C1-1A6A-49BC-8B75-2C9B57D41D37}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{706156B7-4716-4C00-873D-1AFCC8029758}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="17475" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1779,7 +1779,7 @@
         <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4FA3E73A-C631-4361-F734-911A965D84F2}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DEF087C9-2F56-6249-21AD-AB53C225D7D6}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1834,7 +1834,7 @@
         <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2766C111-C951-4D29-5B40-93EC75F24565}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{49665A5A-7B10-FC2F-E32B-E207C4C29A25}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2155,7 +2155,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B9653AD0-8FDC-4FB9-8F19-F7D7B61084CB}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{51E32516-432C-4A19-BF04-66C628E7255D}">
   <dimension ref="A1:H191"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
@@ -2199,10 +2199,10 @@
         <v>258</v>
       </c>
       <c r="C11" s="16">
+        <v>47.544890908098111</v>
+      </c>
+      <c r="D11" s="16">
         <v>7.9712762161849238</v>
-      </c>
-      <c r="D11" s="16">
-        <v>47.544890908098111</v>
       </c>
     </row>
     <row r="12" spans="1:8">
@@ -2210,10 +2210,10 @@
         <v>259</v>
       </c>
       <c r="C12" s="18">
+        <v>47.304724827935445</v>
+      </c>
+      <c r="D12" s="18">
         <v>7.7779031530618461</v>
-      </c>
-      <c r="D12" s="18">
-        <v>47.304724827935445</v>
       </c>
     </row>
     <row r="13" spans="1:8">
@@ -2221,10 +2221,10 @@
         <v>260</v>
       </c>
       <c r="C13" s="16">
+        <v>47.190849773284448</v>
+      </c>
+      <c r="D13" s="16">
         <v>8.98591839231268</v>
-      </c>
-      <c r="D13" s="16">
-        <v>47.190849773284448</v>
       </c>
     </row>
     <row r="14" spans="1:8">
@@ -2232,10 +2232,10 @@
         <v>261</v>
       </c>
       <c r="C14" s="18">
+        <v>47.178826311182746</v>
+      </c>
+      <c r="D14" s="18">
         <v>8.9144143549561985</v>
-      </c>
-      <c r="D14" s="18">
-        <v>47.178826311182746</v>
       </c>
     </row>
     <row r="15" spans="1:8">
@@ -2243,10 +2243,10 @@
         <v>262</v>
       </c>
       <c r="C15" s="16">
+        <v>47.092480331016233</v>
+      </c>
+      <c r="D15" s="16">
         <v>7.6486786287370201</v>
-      </c>
-      <c r="D15" s="16">
-        <v>47.092480331016233</v>
       </c>
     </row>
     <row r="16" spans="1:8">
@@ -2254,10 +2254,10 @@
         <v>263</v>
       </c>
       <c r="C16" s="18">
+        <v>47.075251392097968</v>
+      </c>
+      <c r="D16" s="18">
         <v>8.2262357999999978</v>
-      </c>
-      <c r="D16" s="18">
-        <v>47.075251392097968</v>
       </c>
     </row>
     <row r="17" spans="2:4">
@@ -2265,10 +2265,10 @@
         <v>264</v>
       </c>
       <c r="C17" s="16">
+        <v>46.998666392047838</v>
+      </c>
+      <c r="D17" s="16">
         <v>9.1028854000000017</v>
-      </c>
-      <c r="D17" s="16">
-        <v>46.998666392047838</v>
       </c>
     </row>
     <row r="18" spans="2:4">
@@ -2276,10 +2276,10 @@
         <v>265</v>
       </c>
       <c r="C18" s="18">
+        <v>46.948264900775179</v>
+      </c>
+      <c r="D18" s="18">
         <v>9.4806532222174642</v>
-      </c>
-      <c r="D18" s="18">
-        <v>46.948264900775179</v>
       </c>
     </row>
     <row r="19" spans="2:4">
@@ -2287,10 +2287,10 @@
         <v>266</v>
       </c>
       <c r="C19" s="16">
+        <v>46.881453574552602</v>
+      </c>
+      <c r="D19" s="16">
         <v>8.9862021733683619</v>
-      </c>
-      <c r="D19" s="16">
-        <v>46.881453574552602</v>
       </c>
     </row>
     <row r="20" spans="2:4">
@@ -2298,10 +2298,10 @@
         <v>267</v>
       </c>
       <c r="C20" s="18">
+        <v>46.810115191923131</v>
+      </c>
+      <c r="D20" s="18">
         <v>8.0932617000000064</v>
-      </c>
-      <c r="D20" s="18">
-        <v>46.810115191923131</v>
       </c>
     </row>
     <row r="21" spans="2:4">
@@ -2309,10 +2309,10 @@
         <v>268</v>
       </c>
       <c r="C21" s="16">
+        <v>47.539986892396122</v>
+      </c>
+      <c r="D21" s="16">
         <v>7.9955895999999997</v>
-      </c>
-      <c r="D21" s="16">
-        <v>47.539986892396122</v>
       </c>
     </row>
     <row r="22" spans="2:4">
@@ -2320,10 +2320,10 @@
         <v>269</v>
       </c>
       <c r="C22" s="18">
+        <v>46.788975991909084</v>
+      </c>
+      <c r="D22" s="18">
         <v>8.1290422999999965</v>
-      </c>
-      <c r="D22" s="18">
-        <v>46.788975991909084</v>
       </c>
     </row>
     <row r="23" spans="2:4">
@@ -2331,10 +2331,10 @@
         <v>270</v>
       </c>
       <c r="C23" s="16">
+        <v>46.786285291907262</v>
+      </c>
+      <c r="D23" s="16">
         <v>9.4018789000000034</v>
-      </c>
-      <c r="D23" s="16">
-        <v>46.786285291907262</v>
       </c>
     </row>
     <row r="24" spans="2:4">
@@ -2342,10 +2342,10 @@
         <v>271</v>
       </c>
       <c r="C24" s="18">
+        <v>46.664480125407628</v>
+      </c>
+      <c r="D24" s="18">
         <v>9.5632429943814046</v>
-      </c>
-      <c r="D24" s="18">
-        <v>46.664480125407628</v>
       </c>
     </row>
     <row r="25" spans="2:4">
@@ -2353,10 +2353,10 @@
         <v>272</v>
       </c>
       <c r="C25" s="16">
+        <v>46.655434346966651</v>
+      </c>
+      <c r="D25" s="16">
         <v>8.5931628753479483</v>
-      </c>
-      <c r="D25" s="16">
-        <v>46.655434346966651</v>
       </c>
     </row>
     <row r="26" spans="2:4">
@@ -2364,10 +2364,10 @@
         <v>273</v>
       </c>
       <c r="C26" s="18">
+        <v>46.649952591815854</v>
+      </c>
+      <c r="D26" s="18">
         <v>8.5784506999999994</v>
-      </c>
-      <c r="D26" s="18">
-        <v>46.649952591815854</v>
       </c>
     </row>
     <row r="27" spans="2:4">
@@ -2375,10 +2375,10 @@
         <v>274</v>
       </c>
       <c r="C27" s="16">
+        <v>46.644906911551253</v>
+      </c>
+      <c r="D27" s="16">
         <v>8.3005733260132732</v>
-      </c>
-      <c r="D27" s="16">
-        <v>46.644906911551253</v>
       </c>
     </row>
     <row r="28" spans="2:4">
@@ -2386,10 +2386,10 @@
         <v>275</v>
       </c>
       <c r="C28" s="18">
+        <v>46.623454943499027</v>
+      </c>
+      <c r="D28" s="18">
         <v>8.5532759599539414</v>
-      </c>
-      <c r="D28" s="18">
-        <v>46.623454943499027</v>
       </c>
     </row>
     <row r="29" spans="2:4">
@@ -2397,10 +2397,10 @@
         <v>276</v>
       </c>
       <c r="C29" s="16">
+        <v>46.618279365377013</v>
+      </c>
+      <c r="D29" s="16">
         <v>8.3074651919389026</v>
-      </c>
-      <c r="D29" s="16">
-        <v>46.618279365377013</v>
       </c>
     </row>
     <row r="30" spans="2:4">
@@ -2408,10 +2408,10 @@
         <v>277</v>
       </c>
       <c r="C30" s="18">
+        <v>46.612461191790615</v>
+      </c>
+      <c r="D30" s="18">
         <v>8.5613045000000074</v>
-      </c>
-      <c r="D30" s="18">
-        <v>46.612461191790615</v>
       </c>
     </row>
     <row r="31" spans="2:4">
@@ -2419,10 +2419,10 @@
         <v>278</v>
       </c>
       <c r="C31" s="16">
+        <v>46.581937628506168</v>
+      </c>
+      <c r="D31" s="16">
         <v>9.6114226583534901</v>
-      </c>
-      <c r="D31" s="16">
-        <v>46.581937628506168</v>
       </c>
     </row>
     <row r="32" spans="2:4">
@@ -2430,10 +2430,10 @@
         <v>279</v>
       </c>
       <c r="C32" s="18">
+        <v>47.446856248318333</v>
+      </c>
+      <c r="D32" s="18">
         <v>8.7203907336648729</v>
-      </c>
-      <c r="D32" s="18">
-        <v>47.446856248318333</v>
       </c>
     </row>
     <row r="33" spans="2:4">
@@ -2441,10 +2441,10 @@
         <v>280</v>
       </c>
       <c r="C33" s="16">
+        <v>46.568629391760908</v>
+      </c>
+      <c r="D33" s="16">
         <v>9.9176659999999917</v>
-      </c>
-      <c r="D33" s="16">
-        <v>46.568629391760908</v>
       </c>
     </row>
     <row r="34" spans="2:4">
@@ -2452,10 +2452,10 @@
         <v>281</v>
       </c>
       <c r="C34" s="18">
+        <v>46.56229679175663</v>
+      </c>
+      <c r="D34" s="18">
         <v>6.5602429000000066</v>
-      </c>
-      <c r="D34" s="18">
-        <v>46.56229679175663</v>
       </c>
     </row>
     <row r="35" spans="2:4">
@@ -2463,10 +2463,10 @@
         <v>282</v>
       </c>
       <c r="C35" s="16">
+        <v>46.534677991737887</v>
+      </c>
+      <c r="D35" s="16">
         <v>8.9442773999999901</v>
-      </c>
-      <c r="D35" s="16">
-        <v>46.534677991737887</v>
       </c>
     </row>
     <row r="36" spans="2:4">
@@ -2474,10 +2474,10 @@
         <v>283</v>
       </c>
       <c r="C36" s="18">
+        <v>46.526125791732063</v>
+      </c>
+      <c r="D36" s="18">
         <v>9.8856431000000047</v>
-      </c>
-      <c r="D36" s="18">
-        <v>46.526125791732063</v>
       </c>
     </row>
     <row r="37" spans="2:4">
@@ -2485,10 +2485,10 @@
         <v>284</v>
       </c>
       <c r="C37" s="16">
+        <v>46.497898379860622</v>
+      </c>
+      <c r="D37" s="16">
         <v>8.3151001429309765</v>
-      </c>
-      <c r="D37" s="16">
-        <v>46.497898379860622</v>
       </c>
     </row>
     <row r="38" spans="2:4">
@@ -2496,10 +2496,10 @@
         <v>285</v>
       </c>
       <c r="C38" s="18">
+        <v>46.488751691706611</v>
+      </c>
+      <c r="D38" s="18">
         <v>8.4733173999999973</v>
-      </c>
-      <c r="D38" s="18">
-        <v>46.488751691706611</v>
       </c>
     </row>
     <row r="39" spans="2:4">
@@ -2507,10 +2507,10 @@
         <v>286</v>
       </c>
       <c r="C39" s="16">
+        <v>46.484022953389079</v>
+      </c>
+      <c r="D39" s="16">
         <v>8.345911817931027</v>
-      </c>
-      <c r="D39" s="16">
-        <v>46.484022953389079</v>
       </c>
     </row>
     <row r="40" spans="2:4">
@@ -2518,10 +2518,10 @@
         <v>287</v>
       </c>
       <c r="C40" s="18">
+        <v>46.48232639170228</v>
+      </c>
+      <c r="D40" s="18">
         <v>9.9156705000000098</v>
-      </c>
-      <c r="D40" s="18">
-        <v>46.48232639170228</v>
       </c>
     </row>
     <row r="41" spans="2:4">
@@ -2529,10 +2529,10 @@
         <v>288</v>
       </c>
       <c r="C41" s="16">
+        <v>46.477333091698902</v>
+      </c>
+      <c r="D41" s="16">
         <v>8.4126624000000021</v>
-      </c>
-      <c r="D41" s="16">
-        <v>46.477333091698902</v>
       </c>
     </row>
     <row r="42" spans="2:4">
@@ -2540,10 +2540,10 @@
         <v>289</v>
       </c>
       <c r="C42" s="18">
+        <v>46.473546691696313</v>
+      </c>
+      <c r="D42" s="18">
         <v>8.3779117000000021</v>
-      </c>
-      <c r="D42" s="18">
-        <v>46.473546691696313</v>
       </c>
     </row>
     <row r="43" spans="2:4">
@@ -2551,10 +2551,10 @@
         <v>290</v>
       </c>
       <c r="C43" s="16">
+        <v>47.434850092329576</v>
+      </c>
+      <c r="D43" s="16">
         <v>9.4308717000000009</v>
-      </c>
-      <c r="D43" s="16">
-        <v>47.434850092329576</v>
       </c>
     </row>
     <row r="44" spans="2:4">
@@ -2562,10 +2562,10 @@
         <v>291</v>
       </c>
       <c r="C44" s="18">
+        <v>46.461142191687813</v>
+      </c>
+      <c r="D44" s="18">
         <v>8.4521007999999931</v>
-      </c>
-      <c r="D44" s="18">
-        <v>46.461142191687813</v>
       </c>
     </row>
     <row r="45" spans="2:4">
@@ -2573,10 +2573,10 @@
         <v>292</v>
       </c>
       <c r="C45" s="16">
+        <v>46.42086779166025</v>
+      </c>
+      <c r="D45" s="16">
         <v>9.2172236999999928</v>
-      </c>
-      <c r="D45" s="16">
-        <v>46.42086779166025</v>
       </c>
     </row>
     <row r="46" spans="2:4">
@@ -2584,10 +2584,10 @@
         <v>293</v>
       </c>
       <c r="C46" s="18">
+        <v>46.410782691653388</v>
+      </c>
+      <c r="D46" s="18">
         <v>8.6464327000000054</v>
-      </c>
-      <c r="D46" s="18">
-        <v>46.410782691653388</v>
       </c>
     </row>
     <row r="47" spans="2:4">
@@ -2595,10 +2595,10 @@
         <v>294</v>
       </c>
       <c r="C47" s="16">
+        <v>46.379313191631766</v>
+      </c>
+      <c r="D47" s="16">
         <v>7.2856905999999926</v>
-      </c>
-      <c r="D47" s="16">
-        <v>46.379313191631766</v>
       </c>
     </row>
     <row r="48" spans="2:4">
@@ -2606,10 +2606,10 @@
         <v>295</v>
       </c>
       <c r="C48" s="18">
+        <v>46.352076391613046</v>
+      </c>
+      <c r="D48" s="18">
         <v>7.2952704999999991</v>
-      </c>
-      <c r="D48" s="18">
-        <v>46.352076391613046</v>
       </c>
     </row>
     <row r="49" spans="2:4">
@@ -2617,10 +2617,10 @@
         <v>296</v>
       </c>
       <c r="C49" s="16">
+        <v>46.335742191601824</v>
+      </c>
+      <c r="D49" s="16">
         <v>9.515274700000008</v>
-      </c>
-      <c r="D49" s="16">
-        <v>46.335742191601824</v>
       </c>
     </row>
     <row r="50" spans="2:4">
@@ -2628,10 +2628,10 @@
         <v>297</v>
       </c>
       <c r="C50" s="18">
+        <v>46.332593945141092</v>
+      </c>
+      <c r="D50" s="18">
         <v>8.0099601184858678</v>
-      </c>
-      <c r="D50" s="18">
-        <v>46.332593945141092</v>
       </c>
     </row>
     <row r="51" spans="2:4">
@@ -2639,10 +2639,10 @@
         <v>298</v>
       </c>
       <c r="C51" s="16">
+        <v>46.300225691577296</v>
+      </c>
+      <c r="D51" s="16">
         <v>7.9090832000000049</v>
-      </c>
-      <c r="D51" s="16">
-        <v>46.300225691577296</v>
       </c>
     </row>
     <row r="52" spans="2:4">
@@ -2650,10 +2650,10 @@
         <v>299</v>
       </c>
       <c r="C52" s="18">
+        <v>46.265255891553082</v>
+      </c>
+      <c r="D52" s="18">
         <v>6.8250681999999925</v>
-      </c>
-      <c r="D52" s="18">
-        <v>46.265255891553082</v>
       </c>
     </row>
     <row r="53" spans="2:4">
@@ -2661,10 +2661,10 @@
         <v>300</v>
       </c>
       <c r="C53" s="16">
+        <v>46.258617991548483</v>
+      </c>
+      <c r="D53" s="16">
         <v>6.8503240000000041</v>
-      </c>
-      <c r="D53" s="16">
-        <v>46.258617991548483</v>
       </c>
     </row>
     <row r="54" spans="2:4">
@@ -2672,10 +2672,10 @@
         <v>301</v>
       </c>
       <c r="C54" s="18">
+        <v>47.417551492318573</v>
+      </c>
+      <c r="D54" s="18">
         <v>8.3560802000000063</v>
-      </c>
-      <c r="D54" s="18">
-        <v>47.417551492318573</v>
       </c>
     </row>
     <row r="55" spans="2:4">
@@ -2683,10 +2683,10 @@
         <v>302</v>
       </c>
       <c r="C55" s="16">
+        <v>46.242902191537631</v>
+      </c>
+      <c r="D55" s="16">
         <v>9.0158809000000044</v>
-      </c>
-      <c r="D55" s="16">
-        <v>46.242902191537631</v>
       </c>
     </row>
     <row r="56" spans="2:4">
@@ -2694,10 +2694,10 @@
         <v>303</v>
       </c>
       <c r="C56" s="18">
+        <v>46.238390468466378</v>
+      </c>
+      <c r="D56" s="18">
         <v>6.0514922014978874</v>
-      </c>
-      <c r="D56" s="18">
-        <v>46.238390468466378</v>
       </c>
     </row>
     <row r="57" spans="2:4">
@@ -2705,10 +2705,10 @@
         <v>304</v>
       </c>
       <c r="C57" s="16">
+        <v>46.235914155009169</v>
+      </c>
+      <c r="D57" s="16">
         <v>6.1174054082285867</v>
-      </c>
-      <c r="D57" s="16">
-        <v>46.235914155009169</v>
       </c>
     </row>
     <row r="58" spans="2:4">
@@ -2716,10 +2716,10 @@
         <v>305</v>
       </c>
       <c r="C58" s="18">
+        <v>46.224393391524778</v>
+      </c>
+      <c r="D58" s="18">
         <v>6.9826246999999961</v>
-      </c>
-      <c r="D58" s="18">
-        <v>46.224393391524778</v>
       </c>
     </row>
     <row r="59" spans="2:4">
@@ -2727,10 +2727,10 @@
         <v>306</v>
       </c>
       <c r="C59" s="16">
+        <v>46.194148141506382</v>
+      </c>
+      <c r="D59" s="16">
         <v>8.8493960000010343</v>
-      </c>
-      <c r="D59" s="16">
-        <v>46.194148141506382</v>
       </c>
     </row>
     <row r="60" spans="2:4">
@@ -2738,10 +2738,10 @@
         <v>307</v>
       </c>
       <c r="C60" s="18">
+        <v>46.186124268919009</v>
+      </c>
+      <c r="D60" s="18">
         <v>5.994340131372339</v>
-      </c>
-      <c r="D60" s="18">
-        <v>46.186124268919009</v>
       </c>
     </row>
     <row r="61" spans="2:4">
@@ -2749,10 +2749,10 @@
         <v>308</v>
       </c>
       <c r="C61" s="16">
+        <v>46.173823141643673</v>
+      </c>
+      <c r="D61" s="16">
         <v>8.8978103000914679</v>
-      </c>
-      <c r="D61" s="16">
-        <v>46.173823141643673</v>
       </c>
     </row>
     <row r="62" spans="2:4">
@@ -2760,10 +2760,10 @@
         <v>309</v>
       </c>
       <c r="C62" s="18">
+        <v>46.132986991479271</v>
+      </c>
+      <c r="D62" s="18">
         <v>8.718542699932085</v>
-      </c>
-      <c r="D62" s="18">
-        <v>46.132986991479271</v>
       </c>
     </row>
     <row r="63" spans="2:4">
@@ -2771,10 +2771,10 @@
         <v>310</v>
       </c>
       <c r="C63" s="16">
+        <v>47.388461918063442</v>
+      </c>
+      <c r="D63" s="16">
         <v>8.7320753615603035</v>
-      </c>
-      <c r="D63" s="16">
-        <v>47.388461918063442</v>
       </c>
     </row>
     <row r="64" spans="2:4">
@@ -2782,10 +2782,10 @@
         <v>311</v>
       </c>
       <c r="C64" s="18">
+        <v>46.119367580527111</v>
+      </c>
+      <c r="D64" s="18">
         <v>7.0694412517776462</v>
-      </c>
-      <c r="D64" s="18">
-        <v>46.119367580527111</v>
       </c>
     </row>
     <row r="65" spans="2:4">
@@ -2793,10 +2793,10 @@
         <v>312</v>
       </c>
       <c r="C65" s="16">
+        <v>47.346106146249483</v>
+      </c>
+      <c r="D65" s="16">
         <v>8.0436238635106729</v>
-      </c>
-      <c r="D65" s="16">
-        <v>47.346106146249483</v>
       </c>
     </row>
     <row r="66" spans="2:4">
@@ -2804,10 +2804,10 @@
         <v>313</v>
       </c>
       <c r="C66" s="18">
+        <v>47.328602392261772</v>
+      </c>
+      <c r="D66" s="18">
         <v>9.5426184000000038</v>
-      </c>
-      <c r="D66" s="18">
-        <v>47.328602392261772</v>
       </c>
     </row>
     <row r="67" spans="2:4">
@@ -2815,10 +2815,10 @@
         <v>314</v>
       </c>
       <c r="C67" s="16">
+        <v>46.974388444635309</v>
+      </c>
+      <c r="D67" s="16">
         <v>7.1904948515457114</v>
-      </c>
-      <c r="D67" s="16">
-        <v>46.974388444635309</v>
       </c>
     </row>
     <row r="68" spans="2:4">
@@ -2826,10 +2826,10 @@
         <v>315</v>
       </c>
       <c r="C68" s="18">
+        <v>46.804956344676071</v>
+      </c>
+      <c r="D68" s="18">
         <v>10.332156238823757</v>
-      </c>
-      <c r="D68" s="18">
-        <v>46.804956344676071</v>
       </c>
     </row>
     <row r="69" spans="2:4">
@@ -2837,10 +2837,10 @@
         <v>316</v>
       </c>
       <c r="C69" s="16">
+        <v>47.412318641275661</v>
+      </c>
+      <c r="D69" s="16">
         <v>8.5715564719984449</v>
-      </c>
-      <c r="D69" s="16">
-        <v>47.412318641275661</v>
       </c>
     </row>
     <row r="70" spans="2:4">
@@ -2848,10 +2848,10 @@
         <v>317</v>
       </c>
       <c r="C70" s="18">
+        <v>46.675294830039618</v>
+      </c>
+      <c r="D70" s="18">
         <v>8.7674518660095799</v>
-      </c>
-      <c r="D70" s="18">
-        <v>46.675294830039618</v>
       </c>
     </row>
     <row r="71" spans="2:4">
@@ -2859,10 +2859,10 @@
         <v>318</v>
       </c>
       <c r="C71" s="16">
+        <v>47.271158280917277</v>
+      </c>
+      <c r="D71" s="16">
         <v>8.4332838059847646</v>
-      </c>
-      <c r="D71" s="16">
-        <v>47.271158280917277</v>
       </c>
     </row>
     <row r="72" spans="2:4">
@@ -2870,10 +2870,10 @@
         <v>319</v>
       </c>
       <c r="C72" s="18">
+        <v>46.592025463687065</v>
+      </c>
+      <c r="D72" s="18">
         <v>8.3231337258397549</v>
-      </c>
-      <c r="D72" s="18">
-        <v>46.592025463687065</v>
       </c>
     </row>
     <row r="73" spans="2:4">
@@ -2881,10 +2881,10 @@
         <v>320</v>
       </c>
       <c r="C73" s="16">
+        <v>47.520027177779937</v>
+      </c>
+      <c r="D73" s="16">
         <v>7.6725301685729344</v>
-      </c>
-      <c r="D73" s="16">
-        <v>47.520027177779937</v>
       </c>
     </row>
     <row r="74" spans="2:4">
@@ -2892,10 +2892,10 @@
         <v>321</v>
       </c>
       <c r="C74" s="18">
+        <v>46.410514012428273</v>
+      </c>
+      <c r="D74" s="18">
         <v>8.5287472013709298</v>
-      </c>
-      <c r="D74" s="18">
-        <v>46.410514012428273</v>
       </c>
     </row>
     <row r="75" spans="2:4">
@@ -2903,10 +2903,10 @@
         <v>322</v>
       </c>
       <c r="C75" s="16">
+        <v>46.972086567773282</v>
+      </c>
+      <c r="D75" s="16">
         <v>7.282299486401616</v>
-      </c>
-      <c r="D75" s="16">
-        <v>46.972086567773282</v>
       </c>
     </row>
     <row r="76" spans="2:4">
@@ -2914,10 +2914,10 @@
         <v>323</v>
       </c>
       <c r="C76" s="18">
+        <v>46.557357312705733</v>
+      </c>
+      <c r="D76" s="18">
         <v>6.6139061630111931</v>
-      </c>
-      <c r="D76" s="18">
-        <v>46.557357312705733</v>
       </c>
     </row>
     <row r="77" spans="2:4">
@@ -2925,10 +2925,10 @@
         <v>324</v>
       </c>
       <c r="C77" s="16">
+        <v>47.378758073068163</v>
+      </c>
+      <c r="D77" s="16">
         <v>8.6247814788577859</v>
-      </c>
-      <c r="D77" s="16">
-        <v>47.378758073068163</v>
       </c>
     </row>
     <row r="78" spans="2:4">
@@ -2936,10 +2936,10 @@
         <v>325</v>
       </c>
       <c r="C78" s="18">
+        <v>46.590136747583571</v>
+      </c>
+      <c r="D78" s="18">
         <v>9.4208498140633523</v>
-      </c>
-      <c r="D78" s="18">
-        <v>46.590136747583571</v>
       </c>
     </row>
     <row r="79" spans="2:4">
@@ -2947,10 +2947,10 @@
         <v>326</v>
       </c>
       <c r="C79" s="16">
+        <v>46.766603972636261</v>
+      </c>
+      <c r="D79" s="16">
         <v>7.1256953875579114</v>
-      </c>
-      <c r="D79" s="16">
-        <v>46.766603972636261</v>
       </c>
     </row>
     <row r="80" spans="2:4">
@@ -2958,10 +2958,10 @@
         <v>327</v>
       </c>
       <c r="C80" s="18">
+        <v>47.337522798960869</v>
+      </c>
+      <c r="D80" s="18">
         <v>7.2588732640160751</v>
-      </c>
-      <c r="D80" s="18">
-        <v>47.337522798960869</v>
       </c>
     </row>
     <row r="81" spans="2:4">
@@ -2969,10 +2969,10 @@
         <v>328</v>
       </c>
       <c r="C81" s="16">
+        <v>47.436744661689957</v>
+      </c>
+      <c r="D81" s="16">
         <v>8.2162002170923429</v>
-      </c>
-      <c r="D81" s="16">
-        <v>47.436744661689957</v>
       </c>
     </row>
     <row r="82" spans="2:4">
@@ -2980,10 +2980,10 @@
         <v>329</v>
       </c>
       <c r="C82" s="18">
+        <v>46.667290772141591</v>
+      </c>
+      <c r="D82" s="18">
         <v>8.58387184139076</v>
-      </c>
-      <c r="D82" s="18">
-        <v>46.667290772141591</v>
       </c>
     </row>
     <row r="83" spans="2:4">
@@ -2991,10 +2991,10 @@
         <v>330</v>
       </c>
       <c r="C83" s="16">
+        <v>46.366800843099547</v>
+      </c>
+      <c r="D83" s="16">
         <v>6.1959931237841124</v>
-      </c>
-      <c r="D83" s="16">
-        <v>46.366800843099547</v>
       </c>
     </row>
     <row r="84" spans="2:4">
@@ -3002,10 +3002,10 @@
         <v>331</v>
       </c>
       <c r="C84" s="18">
+        <v>46.35035364659204</v>
+      </c>
+      <c r="D84" s="18">
         <v>8.5954343817427024</v>
-      </c>
-      <c r="D84" s="18">
-        <v>46.35035364659204</v>
       </c>
     </row>
     <row r="85" spans="2:4">
@@ -3013,10 +3013,10 @@
         <v>332</v>
       </c>
       <c r="C85" s="16">
+        <v>46.770135591197366</v>
+      </c>
+      <c r="D85" s="16">
         <v>8.6679070270868852</v>
-      </c>
-      <c r="D85" s="16">
-        <v>46.770135591197366</v>
       </c>
     </row>
     <row r="86" spans="2:4">
@@ -3024,10 +3024,10 @@
         <v>333</v>
       </c>
       <c r="C86" s="18">
+        <v>47.185453772379887</v>
+      </c>
+      <c r="D86" s="18">
         <v>8.1207667742378131</v>
-      </c>
-      <c r="D86" s="18">
-        <v>47.185453772379887</v>
       </c>
     </row>
     <row r="87" spans="2:4">
@@ -3035,10 +3035,10 @@
         <v>334</v>
       </c>
       <c r="C87" s="16">
+        <v>47.23246302223221</v>
+      </c>
+      <c r="D87" s="16">
         <v>7.6158921048685695</v>
-      </c>
-      <c r="D87" s="16">
-        <v>47.23246302223221</v>
       </c>
     </row>
     <row r="88" spans="2:4">
@@ -3046,10 +3046,10 @@
         <v>335</v>
       </c>
       <c r="C88" s="18">
+        <v>47.466610199741339</v>
+      </c>
+      <c r="D88" s="18">
         <v>8.6524389852250962</v>
-      </c>
-      <c r="D88" s="18">
-        <v>47.466610199741339</v>
       </c>
     </row>
     <row r="89" spans="2:4">
@@ -3057,10 +3057,10 @@
         <v>336</v>
       </c>
       <c r="C89" s="16">
+        <v>47.422793373651899</v>
+      </c>
+      <c r="D89" s="16">
         <v>8.5552286743996788</v>
-      </c>
-      <c r="D89" s="16">
-        <v>47.422793373651899</v>
       </c>
     </row>
     <row r="90" spans="2:4">
@@ -3068,10 +3068,10 @@
         <v>337</v>
       </c>
       <c r="C90" s="18">
+        <v>46.822356911553562</v>
+      </c>
+      <c r="D90" s="18">
         <v>8.1738143462569646</v>
-      </c>
-      <c r="D90" s="18">
-        <v>46.822356911553562</v>
       </c>
     </row>
     <row r="91" spans="2:4">
@@ -3079,10 +3079,10 @@
         <v>338</v>
       </c>
       <c r="C91" s="16">
+        <v>46.949503324895758</v>
+      </c>
+      <c r="D91" s="16">
         <v>7.1526297591744381</v>
-      </c>
-      <c r="D91" s="16">
-        <v>46.949503324895758</v>
       </c>
     </row>
     <row r="92" spans="2:4">
@@ -3090,10 +3090,10 @@
         <v>339</v>
       </c>
       <c r="C92" s="18">
+        <v>47.174970614196077</v>
+      </c>
+      <c r="D92" s="18">
         <v>7.5753719705379048</v>
-      </c>
-      <c r="D92" s="18">
-        <v>47.174970614196077</v>
       </c>
     </row>
     <row r="93" spans="2:4">
@@ -3101,10 +3101,10 @@
         <v>340</v>
       </c>
       <c r="C93" s="16">
+        <v>47.426405935677117</v>
+      </c>
+      <c r="D93" s="16">
         <v>8.2183855607953387</v>
-      </c>
-      <c r="D93" s="16">
-        <v>47.426405935677117</v>
       </c>
     </row>
     <row r="94" spans="2:4">
@@ -3112,10 +3112,10 @@
         <v>341</v>
       </c>
       <c r="C94" s="18">
+        <v>46.191060824589286</v>
+      </c>
+      <c r="D94" s="18">
         <v>6.0263528951053331</v>
-      </c>
-      <c r="D94" s="18">
-        <v>46.191060824589286</v>
       </c>
     </row>
     <row r="95" spans="2:4">
@@ -3123,10 +3123,10 @@
         <v>342</v>
       </c>
       <c r="C95" s="16">
+        <v>47.317528275969032</v>
+      </c>
+      <c r="D95" s="16">
         <v>7.9466109226610806</v>
-      </c>
-      <c r="D95" s="16">
-        <v>47.317528275969032</v>
       </c>
     </row>
     <row r="96" spans="2:4">
@@ -3134,10 +3134,10 @@
         <v>343</v>
       </c>
       <c r="C96" s="18">
+        <v>47.220028502558506</v>
+      </c>
+      <c r="D96" s="18">
         <v>8.9741608765490568</v>
-      </c>
-      <c r="D96" s="18">
-        <v>47.220028502558506</v>
       </c>
     </row>
     <row r="97" spans="2:4">
@@ -3145,10 +3145,10 @@
         <v>344</v>
       </c>
       <c r="C97" s="16">
+        <v>46.611103814178406</v>
+      </c>
+      <c r="D97" s="16">
         <v>7.1119095241485661</v>
-      </c>
-      <c r="D97" s="16">
-        <v>46.611103814178406</v>
       </c>
     </row>
     <row r="98" spans="2:4">
@@ -3156,10 +3156,10 @@
         <v>345</v>
       </c>
       <c r="C98" s="18">
+        <v>46.34885054673623</v>
+      </c>
+      <c r="D98" s="18">
         <v>10.062555293517526</v>
-      </c>
-      <c r="D98" s="18">
-        <v>46.34885054673623</v>
       </c>
     </row>
     <row r="99" spans="2:4">
@@ -3167,10 +3167,10 @@
         <v>346</v>
       </c>
       <c r="C99" s="16">
+        <v>46.704671298611736</v>
+      </c>
+      <c r="D99" s="16">
         <v>9.4671012537392354</v>
-      </c>
-      <c r="D99" s="16">
-        <v>46.704671298611736</v>
       </c>
     </row>
     <row r="100" spans="2:4">
@@ -3178,10 +3178,10 @@
         <v>347</v>
       </c>
       <c r="C100" s="18">
+        <v>46.669437648312751</v>
+      </c>
+      <c r="D100" s="18">
         <v>9.6896555979430463</v>
-      </c>
-      <c r="D100" s="18">
-        <v>46.669437648312751</v>
       </c>
     </row>
     <row r="101" spans="2:4">
@@ -3189,10 +3189,10 @@
         <v>348</v>
       </c>
       <c r="C101" s="16">
+        <v>46.670304209093366</v>
+      </c>
+      <c r="D101" s="16">
         <v>7.8586620471824489</v>
-      </c>
-      <c r="D101" s="16">
-        <v>46.670304209093366</v>
       </c>
     </row>
     <row r="102" spans="2:4">
@@ -3200,10 +3200,10 @@
         <v>349</v>
       </c>
       <c r="C102" s="18">
+        <v>46.751315983062611</v>
+      </c>
+      <c r="D102" s="18">
         <v>9.0427987835648143</v>
-      </c>
-      <c r="D102" s="18">
-        <v>46.751315983062611</v>
       </c>
     </row>
     <row r="103" spans="2:4">
@@ -3211,10 +3211,10 @@
         <v>350</v>
       </c>
       <c r="C103" s="16">
+        <v>46.977408013673561</v>
+      </c>
+      <c r="D103" s="16">
         <v>9.5391741699870458</v>
-      </c>
-      <c r="D103" s="16">
-        <v>46.977408013673561</v>
       </c>
     </row>
     <row r="104" spans="2:4">
@@ -3222,10 +3222,10 @@
         <v>351</v>
       </c>
       <c r="C104" s="18">
+        <v>46.530313679899571</v>
+      </c>
+      <c r="D104" s="18">
         <v>9.4339157546528778</v>
-      </c>
-      <c r="D104" s="18">
-        <v>46.530313679899571</v>
       </c>
     </row>
     <row r="105" spans="2:4">
@@ -3233,10 +3233,10 @@
         <v>352</v>
       </c>
       <c r="C105" s="16">
+        <v>46.287036690944227</v>
+      </c>
+      <c r="D105" s="16">
         <v>7.5577983541354428</v>
-      </c>
-      <c r="D105" s="16">
-        <v>46.287036690944227</v>
       </c>
     </row>
     <row r="106" spans="2:4">
@@ -3244,10 +3244,10 @@
         <v>353</v>
       </c>
       <c r="C106" s="18">
+        <v>46.083826692351948</v>
+      </c>
+      <c r="D106" s="18">
         <v>7.956552648739204</v>
-      </c>
-      <c r="D106" s="18">
-        <v>46.083826692351948</v>
       </c>
     </row>
     <row r="107" spans="2:4">
@@ -3255,10 +3255,10 @@
         <v>354</v>
       </c>
       <c r="C107" s="16">
+        <v>47.480988674223049</v>
+      </c>
+      <c r="D107" s="16">
         <v>8.705750623710184</v>
-      </c>
-      <c r="D107" s="16">
-        <v>47.480988674223049</v>
       </c>
     </row>
     <row r="108" spans="2:4">
@@ -3266,10 +3266,10 @@
         <v>355</v>
       </c>
       <c r="C108" s="18">
+        <v>46.756029375970002</v>
+      </c>
+      <c r="D108" s="18">
         <v>6.5540699286344619</v>
-      </c>
-      <c r="D108" s="18">
-        <v>46.756029375970002</v>
       </c>
     </row>
     <row r="109" spans="2:4">
@@ -3277,10 +3277,10 @@
         <v>356</v>
       </c>
       <c r="C109" s="16">
+        <v>46.185370247486951</v>
+      </c>
+      <c r="D109" s="16">
         <v>7.2493006931109596</v>
-      </c>
-      <c r="D109" s="16">
-        <v>46.185370247486951</v>
       </c>
     </row>
     <row r="110" spans="2:4">
@@ -3288,10 +3288,10 @@
         <v>357</v>
       </c>
       <c r="C110" s="18">
+        <v>46.23792888408876</v>
+      </c>
+      <c r="D110" s="18">
         <v>7.8746708803832934</v>
-      </c>
-      <c r="D110" s="18">
-        <v>46.23792888408876</v>
       </c>
     </row>
     <row r="111" spans="2:4">
@@ -3299,10 +3299,10 @@
         <v>358</v>
       </c>
       <c r="C111" s="16">
+        <v>46.066166211545358</v>
+      </c>
+      <c r="D111" s="16">
         <v>6.9015998074716354</v>
-      </c>
-      <c r="D111" s="16">
-        <v>46.066166211545358</v>
       </c>
     </row>
     <row r="112" spans="2:4">
@@ -3310,10 +3310,10 @@
         <v>359</v>
       </c>
       <c r="C112" s="18">
+        <v>46.249132718394094</v>
+      </c>
+      <c r="D112" s="18">
         <v>6.1334444282890637</v>
-      </c>
-      <c r="D112" s="18">
-        <v>46.249132718394094</v>
       </c>
     </row>
     <row r="113" spans="2:4">
@@ -3321,10 +3321,10 @@
         <v>360</v>
       </c>
       <c r="C113" s="16">
+        <v>47.330633116676246</v>
+      </c>
+      <c r="D113" s="16">
         <v>8.7565727921394849</v>
-      </c>
-      <c r="D113" s="16">
-        <v>47.330633116676246</v>
       </c>
     </row>
     <row r="114" spans="2:4">
@@ -3332,10 +3332,10 @@
         <v>361</v>
       </c>
       <c r="C114" s="18">
+        <v>46.702305741170029</v>
+      </c>
+      <c r="D114" s="18">
         <v>8.2346739749028277</v>
-      </c>
-      <c r="D114" s="18">
-        <v>46.702305741170029</v>
       </c>
     </row>
     <row r="115" spans="2:4">
@@ -3343,10 +3343,10 @@
         <v>362</v>
       </c>
       <c r="C115" s="16">
+        <v>47.111263596162431</v>
+      </c>
+      <c r="D115" s="16">
         <v>7.9702987999010633</v>
-      </c>
-      <c r="D115" s="16">
-        <v>47.111263596162431</v>
       </c>
     </row>
     <row r="116" spans="2:4">
@@ -3354,10 +3354,10 @@
         <v>363</v>
       </c>
       <c r="C116" s="18">
+        <v>46.050896100089638</v>
+      </c>
+      <c r="D116" s="18">
         <v>6.949838605733583</v>
-      </c>
-      <c r="D116" s="18">
-        <v>46.050896100089638</v>
       </c>
     </row>
     <row r="117" spans="2:4">
@@ -3365,10 +3365,10 @@
         <v>364</v>
       </c>
       <c r="C117" s="16">
+        <v>46.778607821978291</v>
+      </c>
+      <c r="D117" s="16">
         <v>7.5141567559463658</v>
-      </c>
-      <c r="D117" s="16">
-        <v>46.778607821978291</v>
       </c>
     </row>
     <row r="118" spans="2:4">
@@ -3376,10 +3376,10 @@
         <v>365</v>
       </c>
       <c r="C118" s="18">
+        <v>47.559810348453667</v>
+      </c>
+      <c r="D118" s="18">
         <v>9.0926775269382958</v>
-      </c>
-      <c r="D118" s="18">
-        <v>47.559810348453667</v>
       </c>
     </row>
     <row r="119" spans="2:4">
@@ -3387,10 +3387,10 @@
         <v>366</v>
       </c>
       <c r="C119" s="16">
+        <v>47.573740583075264</v>
+      </c>
+      <c r="D119" s="16">
         <v>8.4736401094130844</v>
-      </c>
-      <c r="D119" s="16">
-        <v>47.573740583075264</v>
       </c>
     </row>
     <row r="120" spans="2:4">
@@ -3398,10 +3398,10 @@
         <v>367</v>
       </c>
       <c r="C120" s="18">
+        <v>47.503332863504447</v>
+      </c>
+      <c r="D120" s="18">
         <v>7.5770135285257956</v>
-      </c>
-      <c r="D120" s="18">
-        <v>47.503332863504447</v>
       </c>
     </row>
     <row r="121" spans="2:4">
@@ -3409,10 +3409,10 @@
         <v>368</v>
       </c>
       <c r="C121" s="16">
+        <v>47.192525806627415</v>
+      </c>
+      <c r="D121" s="16">
         <v>8.5025953004376724</v>
-      </c>
-      <c r="D121" s="16">
-        <v>47.192525806627415</v>
       </c>
     </row>
     <row r="122" spans="2:4">
@@ -3420,10 +3420,10 @@
         <v>369</v>
       </c>
       <c r="C122" s="18">
+        <v>46.197778440184173</v>
+      </c>
+      <c r="D122" s="18">
         <v>8.7492453882474219</v>
-      </c>
-      <c r="D122" s="18">
-        <v>46.197778440184173</v>
       </c>
     </row>
     <row r="123" spans="2:4">
@@ -3431,10 +3431,10 @@
         <v>370</v>
       </c>
       <c r="C123" s="16">
+        <v>46.333583205772456</v>
+      </c>
+      <c r="D123" s="16">
         <v>8.9793979537338995</v>
-      </c>
-      <c r="D123" s="16">
-        <v>46.333583205772456</v>
       </c>
     </row>
     <row r="124" spans="2:4">
@@ -3442,10 +3442,10 @@
         <v>371</v>
       </c>
       <c r="C124" s="18">
+        <v>46.340257020596965</v>
+      </c>
+      <c r="D124" s="18">
         <v>9.2127758729274198</v>
-      </c>
-      <c r="D124" s="18">
-        <v>46.340257020596965</v>
       </c>
     </row>
     <row r="125" spans="2:4">
@@ -3453,10 +3453,10 @@
         <v>372</v>
       </c>
       <c r="C125" s="16">
+        <v>47.497542653552287</v>
+      </c>
+      <c r="D125" s="16">
         <v>8.9315918186612357</v>
-      </c>
-      <c r="D125" s="16">
-        <v>47.497542653552287</v>
       </c>
     </row>
     <row r="126" spans="2:4">
@@ -3464,10 +3464,10 @@
         <v>373</v>
       </c>
       <c r="C126" s="18">
+        <v>46.162021135169752</v>
+      </c>
+      <c r="D126" s="18">
         <v>8.9122525816708951</v>
-      </c>
-      <c r="D126" s="18">
-        <v>46.162021135169752</v>
       </c>
     </row>
     <row r="127" spans="2:4">
@@ -3475,10 +3475,10 @@
         <v>374</v>
       </c>
       <c r="C127" s="16">
+        <v>46.411435336637261</v>
+      </c>
+      <c r="D127" s="16">
         <v>8.6126265598333376</v>
-      </c>
-      <c r="D127" s="16">
-        <v>46.411435336637261</v>
       </c>
     </row>
     <row r="128" spans="2:4">
@@ -3486,10 +3486,10 @@
         <v>375</v>
       </c>
       <c r="C128" s="18">
+        <v>47.472181885969455</v>
+      </c>
+      <c r="D128" s="18">
         <v>7.862020493690677</v>
-      </c>
-      <c r="D128" s="18">
-        <v>47.472181885969455</v>
       </c>
     </row>
     <row r="129" spans="2:4">
@@ -3497,10 +3497,10 @@
         <v>376</v>
       </c>
       <c r="C129" s="16">
+        <v>47.452839734944206</v>
+      </c>
+      <c r="D129" s="16">
         <v>8.4518037652382549</v>
-      </c>
-      <c r="D129" s="16">
-        <v>47.452839734944206</v>
       </c>
     </row>
     <row r="130" spans="2:4">
@@ -3508,10 +3508,10 @@
         <v>377</v>
       </c>
       <c r="C130" s="18">
+        <v>47.378105927066514</v>
+      </c>
+      <c r="D130" s="18">
         <v>8.2848809002281207</v>
-      </c>
-      <c r="D130" s="18">
-        <v>47.378105927066514</v>
       </c>
     </row>
     <row r="131" spans="2:4">
@@ -3519,10 +3519,10 @@
         <v>378</v>
       </c>
       <c r="C131" s="16">
+        <v>47.115092797975542</v>
+      </c>
+      <c r="D131" s="16">
         <v>8.3367437842075223</v>
-      </c>
-      <c r="D131" s="16">
-        <v>47.115092797975542</v>
       </c>
     </row>
     <row r="132" spans="2:4">
@@ -3530,10 +3530,10 @@
         <v>379</v>
       </c>
       <c r="C132" s="18">
+        <v>46.028484492512405</v>
+      </c>
+      <c r="D132" s="18">
         <v>8.9205901102955742</v>
-      </c>
-      <c r="D132" s="18">
-        <v>46.028484492512405</v>
       </c>
     </row>
     <row r="133" spans="2:4">
@@ -3541,10 +3541,10 @@
         <v>380</v>
       </c>
       <c r="C133" s="16">
+        <v>47.365499855192191</v>
+      </c>
+      <c r="D133" s="16">
         <v>7.9731469676031752</v>
-      </c>
-      <c r="D133" s="16">
-        <v>47.365499855192191</v>
       </c>
     </row>
     <row r="134" spans="2:4">
@@ -3552,10 +3552,10 @@
         <v>381</v>
       </c>
       <c r="C134" s="18">
+        <v>47.598960217274261</v>
+      </c>
+      <c r="D134" s="18">
         <v>8.1833885380782423</v>
-      </c>
-      <c r="D134" s="18">
-        <v>47.598960217274261</v>
       </c>
     </row>
     <row r="135" spans="2:4">
@@ -3563,10 +3563,10 @@
         <v>382</v>
       </c>
       <c r="C135" s="16">
+        <v>46.765219065594323</v>
+      </c>
+      <c r="D135" s="16">
         <v>9.4186944777386383</v>
-      </c>
-      <c r="D135" s="16">
-        <v>46.765219065594323</v>
       </c>
     </row>
     <row r="136" spans="2:4">
@@ -3574,10 +3574,10 @@
         <v>383</v>
       </c>
       <c r="C136" s="18">
+        <v>46.395764934452949</v>
+      </c>
+      <c r="D136" s="18">
         <v>8.1308582732979851</v>
-      </c>
-      <c r="D136" s="18">
-        <v>46.395764934452949</v>
       </c>
     </row>
     <row r="137" spans="2:4">
@@ -3585,10 +3585,10 @@
         <v>384</v>
       </c>
       <c r="C137" s="16">
+        <v>46.774712160461192</v>
+      </c>
+      <c r="D137" s="16">
         <v>9.1952002264269037</v>
-      </c>
-      <c r="D137" s="16">
-        <v>46.774712160461192</v>
       </c>
     </row>
     <row r="138" spans="2:4">
@@ -3596,10 +3596,10 @@
         <v>385</v>
       </c>
       <c r="C138" s="18">
+        <v>46.167302808465202</v>
+      </c>
+      <c r="D138" s="18">
         <v>8.1183564066559004</v>
-      </c>
-      <c r="D138" s="18">
-        <v>46.167302808465202</v>
       </c>
     </row>
     <row r="139" spans="2:4">
@@ -3607,10 +3607,10 @@
         <v>386</v>
       </c>
       <c r="C139" s="16">
+        <v>46.188234494031683</v>
+      </c>
+      <c r="D139" s="16">
         <v>8.0701490996033112</v>
-      </c>
-      <c r="D139" s="16">
-        <v>46.188234494031683</v>
       </c>
     </row>
     <row r="140" spans="2:4">
@@ -3618,10 +3618,10 @@
         <v>387</v>
       </c>
       <c r="C140" s="18">
+        <v>47.539015634556947</v>
+      </c>
+      <c r="D140" s="18">
         <v>7.7524068439336924</v>
-      </c>
-      <c r="D140" s="18">
-        <v>47.539015634556947</v>
       </c>
     </row>
     <row r="141" spans="2:4">
@@ -3629,10 +3629,10 @@
         <v>388</v>
       </c>
       <c r="C141" s="16">
+        <v>47.154942264585237</v>
+      </c>
+      <c r="D141" s="16">
         <v>7.7918813512983336</v>
-      </c>
-      <c r="D141" s="16">
-        <v>47.154942264585237</v>
       </c>
     </row>
     <row r="142" spans="2:4">
@@ -3640,10 +3640,10 @@
         <v>389</v>
       </c>
       <c r="C142" s="18">
+        <v>46.491577066054226</v>
+      </c>
+      <c r="D142" s="18">
         <v>7.2732837108404942</v>
-      </c>
-      <c r="D142" s="18">
-        <v>46.491577066054226</v>
       </c>
     </row>
     <row r="143" spans="2:4">
@@ -3651,10 +3651,10 @@
         <v>390</v>
       </c>
       <c r="C143" s="16">
+        <v>46.526902581268999</v>
+      </c>
+      <c r="D143" s="16">
         <v>8.5970130861268519</v>
-      </c>
-      <c r="D143" s="16">
-        <v>46.526902581268999</v>
       </c>
     </row>
     <row r="144" spans="2:4">
@@ -3662,10 +3662,10 @@
         <v>391</v>
       </c>
       <c r="C144" s="18">
+        <v>46.546200095956507</v>
+      </c>
+      <c r="D144" s="18">
         <v>6.5707150506742265</v>
-      </c>
-      <c r="D144" s="18">
-        <v>46.546200095956507</v>
       </c>
     </row>
     <row r="145" spans="2:4">
@@ -3673,10 +3673,10 @@
         <v>392</v>
       </c>
       <c r="C145" s="16">
+        <v>47.302672807623779</v>
+      </c>
+      <c r="D145" s="16">
         <v>9.5558757704346071</v>
-      </c>
-      <c r="D145" s="16">
-        <v>47.302672807623779</v>
       </c>
     </row>
     <row r="146" spans="2:4">
@@ -3684,10 +3684,10 @@
         <v>393</v>
       </c>
       <c r="C146" s="18">
+        <v>47.549929778349131</v>
+      </c>
+      <c r="D146" s="18">
         <v>8.0505862642923702</v>
-      </c>
-      <c r="D146" s="18">
-        <v>47.549929778349131</v>
       </c>
     </row>
     <row r="147" spans="2:4">
@@ -3695,10 +3695,10 @@
         <v>394</v>
       </c>
       <c r="C147" s="16">
+        <v>47.534182026511104</v>
+      </c>
+      <c r="D147" s="16">
         <v>8.6975363672935035</v>
-      </c>
-      <c r="D147" s="16">
-        <v>47.534182026511104</v>
       </c>
     </row>
     <row r="148" spans="2:4">
@@ -3706,10 +3706,10 @@
         <v>395</v>
       </c>
       <c r="C148" s="18">
+        <v>47.186874616216762</v>
+      </c>
+      <c r="D148" s="18">
         <v>8.6845093233496922</v>
-      </c>
-      <c r="D148" s="18">
-        <v>47.186874616216762</v>
       </c>
     </row>
     <row r="149" spans="2:4">
@@ -3717,10 +3717,10 @@
         <v>396</v>
       </c>
       <c r="C149" s="16">
+        <v>46.541607589484336</v>
+      </c>
+      <c r="D149" s="16">
         <v>6.4691836479843738</v>
-      </c>
-      <c r="D149" s="16">
-        <v>46.541607589484336</v>
       </c>
     </row>
     <row r="150" spans="2:4">
@@ -3728,10 +3728,10 @@
         <v>397</v>
       </c>
       <c r="C150" s="18">
+        <v>46.266170983209811</v>
+      </c>
+      <c r="D150" s="18">
         <v>6.9744475162681168</v>
-      </c>
-      <c r="D150" s="18">
-        <v>46.266170983209811</v>
       </c>
     </row>
     <row r="151" spans="2:4">
@@ -3739,10 +3739,10 @@
         <v>398</v>
       </c>
       <c r="C151" s="16">
+        <v>46.811139511097466</v>
+      </c>
+      <c r="D151" s="16">
         <v>9.378873087203484</v>
-      </c>
-      <c r="D151" s="16">
-        <v>46.811139511097466</v>
       </c>
     </row>
     <row r="152" spans="2:4">
@@ -3750,10 +3750,10 @@
         <v>399</v>
       </c>
       <c r="C152" s="18">
+        <v>46.680751374315896</v>
+      </c>
+      <c r="D152" s="18">
         <v>7.6548635065014201</v>
-      </c>
-      <c r="D152" s="18">
-        <v>46.680751374315896</v>
       </c>
     </row>
     <row r="153" spans="2:4">
@@ -3761,10 +3761,10 @@
         <v>400</v>
       </c>
       <c r="C153" s="16">
+        <v>46.0317529216154</v>
+      </c>
+      <c r="D153" s="16">
         <v>7.3084509725129267</v>
-      </c>
-      <c r="D153" s="16">
-        <v>46.0317529216154</v>
       </c>
     </row>
     <row r="154" spans="2:4">
@@ -3772,10 +3772,10 @@
         <v>401</v>
       </c>
       <c r="C154" s="18">
+        <v>46.15852172448291</v>
+      </c>
+      <c r="D154" s="18">
         <v>7.2094009496203837</v>
-      </c>
-      <c r="D154" s="18">
-        <v>46.15852172448291</v>
       </c>
     </row>
     <row r="155" spans="2:4">
@@ -3783,10 +3783,10 @@
         <v>402</v>
       </c>
       <c r="C155" s="16">
+        <v>47.339117940297619</v>
+      </c>
+      <c r="D155" s="16">
         <v>9.5780970318362559</v>
-      </c>
-      <c r="D155" s="16">
-        <v>47.339117940297619</v>
       </c>
     </row>
     <row r="156" spans="2:4">
@@ -3794,10 +3794,10 @@
         <v>403</v>
       </c>
       <c r="C156" s="18">
+        <v>47.657573790258297</v>
+      </c>
+      <c r="D156" s="18">
         <v>8.7754632624143429</v>
-      </c>
-      <c r="D156" s="18">
-        <v>47.657573790258297</v>
       </c>
     </row>
     <row r="157" spans="2:4">
@@ -3805,10 +3805,10 @@
         <v>404</v>
       </c>
       <c r="C157" s="16">
+        <v>47.585912287118212</v>
+      </c>
+      <c r="D157" s="16">
         <v>7.8435782904311289</v>
-      </c>
-      <c r="D157" s="16">
-        <v>47.585912287118212</v>
       </c>
     </row>
     <row r="158" spans="2:4">
@@ -3816,10 +3816,10 @@
         <v>405</v>
       </c>
       <c r="C158" s="18">
+        <v>47.406318762945403</v>
+      </c>
+      <c r="D158" s="18">
         <v>8.105761472055045</v>
-      </c>
-      <c r="D158" s="18">
-        <v>47.406318762945403</v>
       </c>
     </row>
     <row r="159" spans="2:4">
@@ -3827,10 +3827,10 @@
         <v>406</v>
       </c>
       <c r="C159" s="16">
+        <v>47.427363293638969</v>
+      </c>
+      <c r="D159" s="16">
         <v>8.3803937353034943</v>
-      </c>
-      <c r="D159" s="16">
-        <v>47.427363293638969</v>
       </c>
     </row>
     <row r="160" spans="2:4">
@@ -3838,10 +3838,10 @@
         <v>407</v>
       </c>
       <c r="C160" s="18">
+        <v>47.397732455842615</v>
+      </c>
+      <c r="D160" s="18">
         <v>9.3025128506927892</v>
-      </c>
-      <c r="D160" s="18">
-        <v>47.397732455842615</v>
       </c>
     </row>
     <row r="161" spans="2:4">
@@ -3849,10 +3849,10 @@
         <v>408</v>
       </c>
       <c r="C161" s="16">
+        <v>47.481915935925542</v>
+      </c>
+      <c r="D161" s="16">
         <v>9.4326555268370722</v>
-      </c>
-      <c r="D161" s="16">
-        <v>47.481915935925542</v>
       </c>
     </row>
     <row r="162" spans="2:4">
@@ -3860,10 +3860,10 @@
         <v>409</v>
       </c>
       <c r="C162" s="18">
+        <v>46.110634293306326</v>
+      </c>
+      <c r="D162" s="18">
         <v>7.0612643589312309</v>
-      </c>
-      <c r="D162" s="18">
-        <v>46.110634293306326</v>
       </c>
     </row>
     <row r="163" spans="2:4">
@@ -3871,10 +3871,10 @@
         <v>410</v>
       </c>
       <c r="C163" s="16">
+        <v>46.44140479554256</v>
+      </c>
+      <c r="D163" s="16">
         <v>8.8374874894540767</v>
-      </c>
-      <c r="D163" s="16">
-        <v>46.44140479554256</v>
       </c>
     </row>
     <row r="164" spans="2:4">
@@ -3882,10 +3882,10 @@
         <v>411</v>
       </c>
       <c r="C164" s="18">
+        <v>46.350910363932599</v>
+      </c>
+      <c r="D164" s="18">
         <v>8.0409180183520075</v>
-      </c>
-      <c r="D164" s="18">
-        <v>46.350910363932599</v>
       </c>
     </row>
     <row r="165" spans="2:4">
@@ -3893,10 +3893,10 @@
         <v>412</v>
       </c>
       <c r="C165" s="16">
+        <v>47.058633982952401</v>
+      </c>
+      <c r="D165" s="16">
         <v>8.2563745533433206</v>
-      </c>
-      <c r="D165" s="16">
-        <v>47.058633982952401</v>
       </c>
     </row>
     <row r="166" spans="2:4">
@@ -3904,10 +3904,10 @@
         <v>413</v>
       </c>
       <c r="C166" s="18">
+        <v>47.555988773696292</v>
+      </c>
+      <c r="D166" s="18">
         <v>8.2320077689227631</v>
-      </c>
-      <c r="D166" s="18">
-        <v>47.555988773696292</v>
       </c>
     </row>
     <row r="167" spans="2:4">
@@ -5248,7 +5248,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{77FB699F-B42B-474B-9241-AE8FFD99F2EC}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DC3D8562-F8B6-4D4E-9663-B7E3A512752B}">
   <dimension ref="A1:H184"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>

<commit_message>
Updated CHE_grids model - 2025-08-23 15:37
</commit_message>
<xml_diff>
--- a/VerveStacks_CHE_grids/ReportDefs_vervestacks.xlsx
+++ b/VerveStacks_CHE_grids/ReportDefs_vervestacks.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Veda\Veda\Veda_models\vervestacks_models\VerveStacks_CHE_grids\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E8BF23D0-0B4E-473D-B688-2156EC0B97EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{EB942E12-3A80-442A-82DB-3848364AA3BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="17475" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1788,7 +1788,7 @@
         <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3ECAC9B3-65D2-899E-4BC8-0FBD9617E8DD}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{04DC4102-4CFF-6812-C91A-47583AA3208F}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1843,7 +1843,7 @@
         <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0F5A1CD0-51EF-630F-16E1-612C31E2D11D}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{87A67D54-EE94-DAEF-1DFD-32584632C824}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2164,7 +2164,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A66355D7-390C-4351-BB18-74D42E3FF4D6}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C7F2E9CE-6F2D-422A-9431-496BBD717AB1}">
   <dimension ref="A1:H191"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
@@ -5257,7 +5257,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F35DE795-59AE-46C7-9CE5-016A07FE1CCA}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{860F61D8-B1C9-4072-9A91-001B623E628B}">
   <dimension ref="A1:H184"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>

<commit_message>
Updated CHE_grids model - 2025-08-26 18:20
</commit_message>
<xml_diff>
--- a/VerveStacks_CHE_grids/ReportDefs_vervestacks.xlsx
+++ b/VerveStacks_CHE_grids/ReportDefs_vervestacks.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Veda\Veda\Veda_models\vervestacks_models\VerveStacks_CHE_grids\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{EB942E12-3A80-442A-82DB-3848364AA3BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{26D4F176-EFAA-4FBA-BFC2-3E2E1BD92FDF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="17475" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1788,7 +1788,7 @@
         <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{04DC4102-4CFF-6812-C91A-47583AA3208F}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D90FF6EA-4B72-DEF4-57B0-9BC34FB83F7F}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1843,7 +1843,7 @@
         <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{87A67D54-EE94-DAEF-1DFD-32584632C824}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{16F38C65-13F9-75C9-6A32-52594B4BC1D0}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2164,7 +2164,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C7F2E9CE-6F2D-422A-9431-496BBD717AB1}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C2BB2589-3215-439B-BA72-AE88D7DAAF88}">
   <dimension ref="A1:H191"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
@@ -5257,7 +5257,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{860F61D8-B1C9-4072-9A91-001B623E628B}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3A87FFEF-4ADA-48EE-A335-6FF9C166D827}">
   <dimension ref="A1:H184"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>

<commit_message>
Updated CHE_grids model - 2025-08-31 21:28
</commit_message>
<xml_diff>
--- a/VerveStacks_CHE_grids/ReportDefs_vervestacks.xlsx
+++ b/VerveStacks_CHE_grids/ReportDefs_vervestacks.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Veda\Veda\Veda_models\vervestacks_models\VerveStacks_CHE_grids\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{28822AB1-59B5-46F0-835C-9CB04B968184}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{3BB7625B-4570-48FB-90D9-769BF20918A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="17475" firstSheet="8" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1803,7 +1803,7 @@
         <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C1E31180-0E25-731F-887E-AEFE503AEB5A}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{102079BB-31C2-B175-0965-32659499A8A8}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1858,7 +1858,7 @@
         <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B733A9C0-D3B9-5473-D2A3-19DFDEC6A469}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EB543239-F6CA-4F30-560F-BC6DB9C8B149}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4050,7 +4050,7 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{18A60606-ABFE-437E-95EF-5DE892138E6E}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6FCFEAED-540B-44BC-8649-D82010E45470}">
   <dimension ref="A1:H184"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -8508,7 +8508,7 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8DB6D12F-1F85-4D20-9813-C07493ADD338}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D46D61E7-8350-4C3D-8A35-3A418CC8624E}">
   <dimension ref="A1:H191"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>

</xml_diff>

<commit_message>
Updated CHE_grids model - 2025-08-31 21:50
</commit_message>
<xml_diff>
--- a/VerveStacks_CHE_grids/ReportDefs_vervestacks.xlsx
+++ b/VerveStacks_CHE_grids/ReportDefs_vervestacks.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Veda\Veda\Veda_models\vervestacks_models\VerveStacks_CHE_grids\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{3BB7625B-4570-48FB-90D9-769BF20918A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{903A2BFB-BBF4-42F9-8F1A-8CDBE3837A7C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="17475" firstSheet="8" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1803,7 +1803,7 @@
         <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{102079BB-31C2-B175-0965-32659499A8A8}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9C332799-DBF9-326D-BAD6-E179C91A8276}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1858,7 +1858,7 @@
         <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EB543239-F6CA-4F30-560F-BC6DB9C8B149}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1D2EEABA-2361-DC98-EC92-AFAD6CEA8CD4}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4050,7 +4050,7 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6FCFEAED-540B-44BC-8649-D82010E45470}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B936E459-1184-4897-B30D-CD6DFB5C2DDB}">
   <dimension ref="A1:H184"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -8508,7 +8508,7 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D46D61E7-8350-4C3D-8A35-3A418CC8624E}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0360F5D6-D63D-4587-92C8-8AE0043041B9}">
   <dimension ref="A1:H191"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>

</xml_diff>

<commit_message>
Updated CHE_grids model - 2025-08-31 22:00
</commit_message>
<xml_diff>
--- a/VerveStacks_CHE_grids/ReportDefs_vervestacks.xlsx
+++ b/VerveStacks_CHE_grids/ReportDefs_vervestacks.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Veda\Veda\Veda_models\vervestacks_models\VerveStacks_CHE_grids\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{903A2BFB-BBF4-42F9-8F1A-8CDBE3837A7C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{1B5A9B09-8F57-40D3-98B9-02F2119ECBF1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="17475" firstSheet="8" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1803,7 +1803,7 @@
         <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9C332799-DBF9-326D-BAD6-E179C91A8276}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A204CCA1-0F3A-76BA-9503-B3EFC5814590}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1858,7 +1858,7 @@
         <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1D2EEABA-2361-DC98-EC92-AFAD6CEA8CD4}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{686DBA03-9EEB-D550-E477-49855E95644B}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4050,7 +4050,7 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B936E459-1184-4897-B30D-CD6DFB5C2DDB}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC74BFCA-6C82-431F-9DA7-58CB228C765C}">
   <dimension ref="A1:H184"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -8508,7 +8508,7 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0360F5D6-D63D-4587-92C8-8AE0043041B9}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BBFC48A0-EB8C-451B-B054-D42008457A04}">
   <dimension ref="A1:H191"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>

</xml_diff>

<commit_message>
Updated CHE_grids model - 2025-09-06 19:58
</commit_message>
<xml_diff>
--- a/VerveStacks_CHE_grids/ReportDefs_vervestacks.xlsx
+++ b/VerveStacks_CHE_grids/ReportDefs_vervestacks.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Veda\Veda\Veda_models\vervestacks_models\VerveStacks_CHE_grids\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{0CD0AF1E-06A8-4CF2-8B9C-FD7689FCD760}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{01BCD3F0-5731-4884-A79A-48515D7A6258}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="17475" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -5303,7 +5303,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{42CDFA74-0928-41B2-B56F-671121132B3C}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{85C1E6B5-3466-44D3-9FA6-7F7E6EA0FDFD}">
   <dimension ref="B9:D191"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
@@ -7323,7 +7323,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4BB20DD6-A02F-498C-B913-68FA11A2DCD7}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3AF9C309-3FCB-49AD-9A49-2D3F9580A998}">
   <dimension ref="B2:D184"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>

</xml_diff>

<commit_message>
Updated CHE_grids model - 2025-09-06 20:56
</commit_message>
<xml_diff>
--- a/VerveStacks_CHE_grids/ReportDefs_vervestacks.xlsx
+++ b/VerveStacks_CHE_grids/ReportDefs_vervestacks.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Veda\Veda\Veda_models\vervestacks_models\VerveStacks_CHE_grids\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{01BCD3F0-5731-4884-A79A-48515D7A6258}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{D8BD231E-53F1-477B-9F30-D6547477FE44}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="17475" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -5303,7 +5303,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{85C1E6B5-3466-44D3-9FA6-7F7E6EA0FDFD}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5DA00301-2FF6-4533-878B-82DA0FECC4F5}">
   <dimension ref="B9:D191"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
@@ -7323,7 +7323,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3AF9C309-3FCB-49AD-9A49-2D3F9580A998}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{730EB7E4-D14B-43F6-A32B-293B2C5EC513}">
   <dimension ref="B2:D184"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>

</xml_diff>